<commit_message>
On copie maintenant le style dans le fichier sauvegardé.
</commit_message>
<xml_diff>
--- a/fichiers_xls/test.xlsx
+++ b/fichiers_xls/test.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Feuille2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" name="_xlfn_T_TEST" vbProcedure="false">NA()</definedName>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="256">
   <si>
     <t xml:space="preserve">Nom</t>
   </si>
@@ -787,6 +788,15 @@
   </si>
   <si>
     <t xml:space="preserve">8 intermédiaires</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test !!!!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Il doit y avoir des notes.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zdzd</t>
   </si>
 </sst>
 </file>
@@ -825,6 +835,7 @@
       <color rgb="FF969696"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -832,11 +843,13 @@
       <color rgb="FFFF00FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="14"/>
@@ -1068,7 +1081,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1103,8 +1116,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.303115961083355"/>
-          <c:y val="0.0220736629667003"/>
+          <c:x val="0.303258309343104"/>
+          <c:y val="0.0224605678233438"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1121,10 +1134,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0134104654220352"/>
-          <c:y val="0.124621594349142"/>
-          <c:w val="0.96765711280568"/>
-          <c:h val="0.865035317860747"/>
+          <c:x val="0.0133472912850039"/>
+          <c:y val="0.124668769716088"/>
+          <c:w val="0.967416906568961"/>
+          <c:h val="0.864605678233438"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -1166,6 +1179,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1391,17 +1405,17 @@
         </c:ser>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="95729218"/>
-        <c:axId val="35544237"/>
+        <c:axId val="80292468"/>
+        <c:axId val="61949105"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="95729218"/>
+        <c:axId val="80292468"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1426,7 +1440,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="35544237"/>
+        <c:crossAx val="61949105"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1434,7 +1448,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="35544237"/>
+        <c:axId val="61949105"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -1473,7 +1487,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="95729218"/>
+        <c:crossAx val="80292468"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1511,9 +1525,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>109</xdr:col>
-      <xdr:colOff>48960</xdr:colOff>
+      <xdr:colOff>47880</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>92520</xdr:rowOff>
+      <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1521,8 +1535,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="103101840" y="2742120"/>
-        <a:ext cx="5475960" cy="2853720"/>
+        <a:off x="103442760" y="2742120"/>
+        <a:ext cx="5501880" cy="2852640"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1542,11 +1556,11 @@
   </sheetPr>
   <dimension ref="A1:DJ64077"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AO4" activeCellId="0" sqref="AO4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AO4" activeCellId="1" sqref="B7 AO4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.01953125" defaultRowHeight="16.05" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="16.05" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="14.38"/>
@@ -5708,165 +5722,165 @@
     <row r="15" customFormat="false" ht="16.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="L15" s="16" t="e">
         <f aca="false">#REF!*100/1472</f>
-        <v>#VALUE!</v>
+        <v>#REF!</v>
       </c>
       <c r="M15" s="16"/>
       <c r="N15" s="16" t="e">
         <f aca="false">#REF!*100/1472</f>
-        <v>#VALUE!</v>
+        <v>#REF!</v>
       </c>
       <c r="O15" s="16"/>
       <c r="P15" s="16" t="e">
         <f aca="false">#REF!*100/1472</f>
-        <v>#VALUE!</v>
+        <v>#REF!</v>
       </c>
       <c r="Q15" s="16"/>
       <c r="R15" s="16" t="e">
         <f aca="false">#REF!*100/1472</f>
-        <v>#VALUE!</v>
+        <v>#REF!</v>
       </c>
       <c r="S15" s="16"/>
       <c r="T15" s="16" t="e">
         <f aca="false">#REF!*100/1472</f>
-        <v>#VALUE!</v>
+        <v>#REF!</v>
       </c>
       <c r="U15" s="16"/>
       <c r="V15" s="16" t="e">
         <f aca="false">#REF!*100/1472</f>
-        <v>#VALUE!</v>
+        <v>#REF!</v>
       </c>
       <c r="W15" s="16"/>
       <c r="X15" s="16" t="e">
         <f aca="false">#REF!*100/1472</f>
-        <v>#VALUE!</v>
+        <v>#REF!</v>
       </c>
       <c r="Y15" s="16"/>
       <c r="Z15" s="16" t="e">
         <f aca="false">#REF!*100/1472</f>
-        <v>#VALUE!</v>
+        <v>#REF!</v>
       </c>
       <c r="AA15" s="16"/>
       <c r="AB15" s="16" t="e">
         <f aca="false">#REF!*100/1472</f>
-        <v>#VALUE!</v>
+        <v>#REF!</v>
       </c>
       <c r="AC15" s="16"/>
       <c r="AD15" s="16" t="e">
         <f aca="false">#REF!*100/1472</f>
-        <v>#VALUE!</v>
+        <v>#REF!</v>
       </c>
       <c r="AE15" s="16"/>
       <c r="AF15" s="16" t="e">
         <f aca="false">#REF!*100/1472</f>
-        <v>#VALUE!</v>
+        <v>#REF!</v>
       </c>
       <c r="AG15" s="16"/>
       <c r="AH15" s="16" t="e">
         <f aca="false">#REF!*100/1472</f>
-        <v>#VALUE!</v>
+        <v>#REF!</v>
       </c>
       <c r="AI15" s="16"/>
       <c r="AJ15" s="16" t="e">
         <f aca="false">#REF!*100/1472</f>
-        <v>#VALUE!</v>
+        <v>#REF!</v>
       </c>
       <c r="AK15" s="16"/>
       <c r="AL15" s="16" t="e">
         <f aca="false">#REF!*100/1472</f>
-        <v>#VALUE!</v>
+        <v>#REF!</v>
       </c>
       <c r="AM15" s="17"/>
       <c r="AN15" s="16"/>
       <c r="AO15" s="16" t="e">
         <f aca="false">#REF!*100/1472</f>
-        <v>#VALUE!</v>
+        <v>#REF!</v>
       </c>
       <c r="AP15" s="16"/>
       <c r="AQ15" s="16"/>
       <c r="AR15" s="16"/>
       <c r="AS15" s="16" t="e">
         <f aca="false">#REF!*100/1472</f>
-        <v>#VALUE!</v>
+        <v>#REF!</v>
       </c>
       <c r="AT15" s="16"/>
       <c r="AU15" s="16" t="e">
         <f aca="false">#REF!*100/1472</f>
-        <v>#VALUE!</v>
+        <v>#REF!</v>
       </c>
       <c r="AV15" s="16"/>
       <c r="AW15" s="16" t="e">
         <f aca="false">#REF!*100/1472</f>
-        <v>#VALUE!</v>
+        <v>#REF!</v>
       </c>
       <c r="AX15" s="16"/>
       <c r="AY15" s="16" t="e">
         <f aca="false">#REF!*100/1472</f>
-        <v>#VALUE!</v>
+        <v>#REF!</v>
       </c>
       <c r="AZ15" s="16"/>
       <c r="BA15" s="16" t="e">
         <f aca="false">#REF!*100/1472</f>
-        <v>#VALUE!</v>
+        <v>#REF!</v>
       </c>
       <c r="BB15" s="16"/>
       <c r="BC15" s="16" t="e">
         <f aca="false">#REF!*100/1472</f>
-        <v>#VALUE!</v>
+        <v>#REF!</v>
       </c>
       <c r="BD15" s="16"/>
       <c r="BE15" s="16" t="e">
         <f aca="false">#REF!*100/1472</f>
-        <v>#VALUE!</v>
+        <v>#REF!</v>
       </c>
       <c r="BF15" s="16"/>
       <c r="BG15" s="16" t="e">
         <f aca="false">#REF!*100/1472</f>
-        <v>#VALUE!</v>
+        <v>#REF!</v>
       </c>
       <c r="BH15" s="16"/>
       <c r="BI15" s="16" t="e">
         <f aca="false">#REF!*100/1472</f>
-        <v>#VALUE!</v>
+        <v>#REF!</v>
       </c>
       <c r="BJ15" s="16"/>
       <c r="BK15" s="16" t="e">
         <f aca="false">#REF!*100/1472</f>
-        <v>#VALUE!</v>
+        <v>#REF!</v>
       </c>
       <c r="BL15" s="16"/>
       <c r="BM15" s="16" t="e">
         <f aca="false">#REF!*100/1472</f>
-        <v>#VALUE!</v>
+        <v>#REF!</v>
       </c>
       <c r="BN15" s="16"/>
       <c r="BO15" s="16" t="e">
         <f aca="false">#REF!*100/1472</f>
-        <v>#VALUE!</v>
+        <v>#REF!</v>
       </c>
       <c r="BP15" s="16"/>
       <c r="BQ15" s="16" t="e">
         <f aca="false">#REF!*100/1472</f>
-        <v>#VALUE!</v>
+        <v>#REF!</v>
       </c>
       <c r="BR15" s="16"/>
       <c r="BS15" s="16" t="e">
         <f aca="false">#REF!*100/1472</f>
-        <v>#VALUE!</v>
+        <v>#REF!</v>
       </c>
       <c r="BT15" s="16"/>
       <c r="BU15" s="16" t="e">
         <f aca="false">#REF!*100/1472</f>
-        <v>#VALUE!</v>
+        <v>#REF!</v>
       </c>
       <c r="BV15" s="16"/>
       <c r="BW15" s="16" t="e">
         <f aca="false">#REF!*100/1472</f>
-        <v>#VALUE!</v>
+        <v>#REF!</v>
       </c>
       <c r="BX15" s="16"/>
       <c r="BY15" s="16" t="e">
         <f aca="false">#REF!*100/1472</f>
-        <v>#VALUE!</v>
+        <v>#REF!</v>
       </c>
       <c r="BZ15" s="17"/>
     </row>
@@ -7340,4 +7354,48 @@
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C4" s="0" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="0" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="0" t="s">
+        <v>255</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Nom du fichier de sauvegarde nom_date_****-**-**.xlsx
</commit_message>
<xml_diff>
--- a/fichiers_xls/test.xlsx
+++ b/fichiers_xls/test.xlsx
@@ -403,7 +403,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:t/>
+                  <a:t>None</a:t>
                 </a:r>
               </a:p>
             </txPr>
@@ -662,7 +662,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
           </a:p>
         </txPr>
@@ -714,7 +714,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
           </a:p>
         </txPr>

</xml_diff>

<commit_message>
Ajout de la fonction delete_lines et du dataset de dulcinee + execution.py
</commit_message>
<xml_diff>
--- a/fichiers_xls/test.xlsx
+++ b/fichiers_xls/test.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="10" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -16,6 +16,8 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="color_line" sheetId="7" state="visible" r:id="rId7"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="cutinparts" sheetId="8" state="visible" r:id="rId8"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="cutinpartsbis" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="delete_lines" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="delete_lines_bis" sheetId="11" state="visible" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName name="_xlfn_T_TEST" hidden="0" function="0" vbProcedure="0">NA()</definedName>
@@ -440,8 +442,8 @@
           <yMode val="edge"/>
           <wMode val="factor"/>
           <hMode val="factor"/>
-          <x val="0.304242886178862"/>
-          <y val="0.0253068455017082"/>
+          <x val="0.304284354173278"/>
+          <y val="0.0254365983295368"/>
         </manualLayout>
       </layout>
       <overlay val="0"/>
@@ -460,10 +462,10 @@
           <yMode val="edge"/>
           <wMode val="factor"/>
           <hMode val="factor"/>
-          <x val="0.0129573170731707"/>
-          <y val="0.125015816778439"/>
-          <w val="0.965891768292683"/>
-          <h val="0.861445020878148"/>
+          <x val="0.0129482703903523"/>
+          <y val="0.125031637560111"/>
+          <w val="0.96585211044113"/>
+          <h val="0.861300936471779"/>
         </manualLayout>
       </layout>
       <barChart>
@@ -636,11 +638,11 @@
         </ser>
         <gapWidth val="219"/>
         <overlap val="-27"/>
-        <axId val="48646592"/>
-        <axId val="6995127"/>
+        <axId val="82962979"/>
+        <axId val="64313139"/>
       </barChart>
       <catAx>
-        <axId val="48646592"/>
+        <axId val="82962979"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
@@ -675,7 +677,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="6995127"/>
+        <crossAx val="64313139"/>
         <crossesAt val="0"/>
         <auto val="1"/>
         <lblAlgn val="ctr"/>
@@ -683,7 +685,7 @@
         <noMultiLvlLbl val="0"/>
       </catAx>
       <valAx>
-        <axId val="6995127"/>
+        <axId val="64313139"/>
         <scaling>
           <orientation val="minMax"/>
           <max val="100"/>
@@ -727,7 +729,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="48646592"/>
+        <crossAx val="82962979"/>
         <crossesAt val="1"/>
         <crossBetween val="midCat"/>
       </valAx>
@@ -784,8 +786,8 @@
           <yMode val="edge"/>
           <wMode val="factor"/>
           <hMode val="factor"/>
-          <x val="0.304270007670672"/>
-          <y val="0.0253068455017082"/>
+          <x val="0.304283981357339"/>
+          <y val="0.0254365983295368"/>
         </manualLayout>
       </layout>
       <overlay val="0"/>
@@ -804,10 +806,10 @@
           <yMode val="edge"/>
           <wMode val="factor"/>
           <hMode val="factor"/>
-          <x val="0.0129762209153669"/>
-          <y val="0.125015816778439"/>
-          <w val="0.96573766300179"/>
-          <h val="0.861445020878148"/>
+          <x val="0.0129604801123667"/>
+          <y val="0.125031637560111"/>
+          <w val="0.965651535465747"/>
+          <h val="0.861300936471779"/>
         </manualLayout>
       </layout>
       <barChart>
@@ -980,11 +982,11 @@
         </ser>
         <gapWidth val="219"/>
         <overlap val="-27"/>
-        <axId val="62705975"/>
-        <axId val="13261077"/>
+        <axId val="10632551"/>
+        <axId val="42813938"/>
       </barChart>
       <catAx>
-        <axId val="62705975"/>
+        <axId val="10632551"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
@@ -1019,7 +1021,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="13261077"/>
+        <crossAx val="42813938"/>
         <crossesAt val="0"/>
         <auto val="1"/>
         <lblAlgn val="ctr"/>
@@ -1027,7 +1029,7 @@
         <noMultiLvlLbl val="0"/>
       </catAx>
       <valAx>
-        <axId val="13261077"/>
+        <axId val="42813938"/>
         <scaling>
           <orientation val="minMax"/>
           <max val="100"/>
@@ -1071,7 +1073,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="62705975"/>
+        <crossAx val="10632551"/>
         <crossesAt val="1"/>
         <crossBetween val="midCat"/>
       </valAx>
@@ -1128,8 +1130,8 @@
           <yMode val="edge"/>
           <wMode val="factor"/>
           <hMode val="factor"/>
-          <x val="0.30431447746884"/>
-          <y val="0.0254333797292167"/>
+          <x val="0.304372805617619"/>
+          <y val="0.0255631485699823"/>
         </manualLayout>
       </layout>
       <overlay val="0"/>
@@ -1149,10 +1151,10 @@
           <yMode val="edge"/>
           <wMode val="factor"/>
           <hMode val="factor"/>
-          <x val="0.0524129114733142"/>
-          <y val="0.145261293179805"/>
-          <w val="0.926685842122084"/>
-          <h val="0.821080602302923"/>
+          <x val="0.0524098308330674"/>
+          <y val="0.145279676031384"/>
+          <w val="0.926651771465049"/>
+          <h val="0.820931409769679"/>
         </manualLayout>
       </layout>
       <barChart>
@@ -1325,11 +1327,11 @@
         </ser>
         <gapWidth val="219"/>
         <overlap val="-27"/>
-        <axId val="88107833"/>
-        <axId val="20764433"/>
+        <axId val="83284912"/>
+        <axId val="19779740"/>
       </barChart>
       <catAx>
-        <axId val="88107833"/>
+        <axId val="83284912"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
@@ -1364,7 +1366,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="20764433"/>
+        <crossAx val="19779740"/>
         <crosses val="autoZero"/>
         <auto val="1"/>
         <lblAlgn val="ctr"/>
@@ -1372,7 +1374,7 @@
         <noMultiLvlLbl val="0"/>
       </catAx>
       <valAx>
-        <axId val="20764433"/>
+        <axId val="19779740"/>
         <scaling>
           <orientation val="minMax"/>
           <max val="100"/>
@@ -1416,7 +1418,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="88107833"/>
+        <crossAx val="83284912"/>
         <crossesAt val="1"/>
         <crossBetween val="midCat"/>
       </valAx>
@@ -1473,8 +1475,8 @@
           <yMode val="edge"/>
           <wMode val="factor"/>
           <hMode val="factor"/>
-          <x val="0.304378395653563"/>
-          <y val="0.0255599139567253"/>
+          <x val="0.304436642195978"/>
+          <y val="0.0256896988104277"/>
         </manualLayout>
       </layout>
       <overlay val="0"/>
@@ -1494,10 +1496,10 @@
           <yMode val="edge"/>
           <wMode val="factor"/>
           <hMode val="factor"/>
-          <x val="0.0524129114733142"/>
-          <y val="0.145261293179805"/>
-          <w val="0.926685842122084"/>
-          <h val="0.821080602302923"/>
+          <x val="0.0524098308330674"/>
+          <y val="0.145279676031384"/>
+          <w val="0.926651771465049"/>
+          <h val="0.820931409769679"/>
         </manualLayout>
       </layout>
       <barChart>
@@ -1670,11 +1672,11 @@
         </ser>
         <gapWidth val="219"/>
         <overlap val="-27"/>
-        <axId val="65714624"/>
-        <axId val="28127721"/>
+        <axId val="53177077"/>
+        <axId val="26377073"/>
       </barChart>
       <catAx>
-        <axId val="65714624"/>
+        <axId val="53177077"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
@@ -1709,7 +1711,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="28127721"/>
+        <crossAx val="26377073"/>
         <crosses val="autoZero"/>
         <auto val="1"/>
         <lblAlgn val="ctr"/>
@@ -1717,7 +1719,7 @@
         <noMultiLvlLbl val="0"/>
       </catAx>
       <valAx>
-        <axId val="28127721"/>
+        <axId val="26377073"/>
         <scaling>
           <orientation val="minMax"/>
           <max val="100"/>
@@ -1761,7 +1763,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="65714624"/>
+        <crossAx val="53177077"/>
         <crossesAt val="1"/>
         <crossBetween val="midCat"/>
       </valAx>
@@ -1794,9 +1796,9 @@
     </from>
     <to>
       <col>109</col>
-      <colOff>39960</colOff>
+      <colOff>39600</colOff>
       <row>27</row>
-      <rowOff>83520</rowOff>
+      <rowOff>83160</rowOff>
     </to>
     <graphicFrame>
       <nvGraphicFramePr>
@@ -1826,9 +1828,9 @@
     </from>
     <to>
       <col>100</col>
-      <colOff>691920</colOff>
+      <colOff>691560</colOff>
       <row>30</row>
-      <rowOff>133560</rowOff>
+      <rowOff>133200</rowOff>
     </to>
     <graphicFrame>
       <nvGraphicFramePr>
@@ -1858,9 +1860,9 @@
     </from>
     <to>
       <col>107</col>
-      <colOff>691920</colOff>
+      <colOff>691560</colOff>
       <row>30</row>
-      <rowOff>132840</rowOff>
+      <rowOff>132480</rowOff>
     </to>
     <graphicFrame>
       <nvGraphicFramePr>
@@ -1890,9 +1892,9 @@
     </from>
     <to>
       <col>107</col>
-      <colOff>691920</colOff>
+      <colOff>691560</colOff>
       <row>30</row>
-      <rowOff>132840</rowOff>
+      <rowOff>132480</rowOff>
     </to>
     <graphicFrame>
       <nvGraphicFramePr>
@@ -2206,7 +2208,7 @@
       <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.42578125" defaultRowHeight="16.05" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.43359375" defaultRowHeight="16.05" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="16.2" customWidth="1" style="20" min="6" max="6"/>
     <col width="14.38" customWidth="1" style="21" min="7" max="7"/>
@@ -8805,6 +8807,708 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr filterMode="0">
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr fitToPage="0"/>
+  </sheetPr>
+  <dimension ref="A1:F14"/>
+  <sheetViews>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <cols>
+    <col width="11.54" customWidth="1" style="20" min="1" max="1024"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="12.8" customHeight="1" s="23">
+      <c r="A1" s="35" t="inlineStr">
+        <is>
+          <t>Les électrons sont plus petits que les atomes</t>
+        </is>
+      </c>
+      <c r="B1" s="36" t="inlineStr">
+        <is>
+          <t>accuracy_Q6</t>
+        </is>
+      </c>
+      <c r="C1" s="24" t="inlineStr">
+        <is>
+          <t>Toute radioactivité résulte de l’action de l’homme</t>
+        </is>
+      </c>
+      <c r="D1" s="24" t="inlineStr">
+        <is>
+          <t>accuracy_Q7</t>
+        </is>
+      </c>
+      <c r="E1" s="24" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  La Terre fait le tour du Soleil en un mois</t>
+        </is>
+      </c>
+      <c r="F1" s="24" t="inlineStr">
+        <is>
+          <t>accuracy_Q8</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="12.8" customHeight="1" s="23">
+      <c r="A2" s="20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> partie 6 : Vrai</t>
+        </is>
+      </c>
+      <c r="B2" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> partie 7 : Faux</t>
+        </is>
+      </c>
+      <c r="D2" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" s="20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> partie 8 : Faux</t>
+        </is>
+      </c>
+      <c r="F2" s="20" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" ht="12.8" customHeight="1" s="23">
+      <c r="A3" s="20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> partie 6 : Vrai</t>
+        </is>
+      </c>
+      <c r="B3" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> partie 7 : Faux</t>
+        </is>
+      </c>
+      <c r="D3" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" s="20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> partie 8 : Faux</t>
+        </is>
+      </c>
+      <c r="F3" s="20" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" ht="12.8" customHeight="1" s="23">
+      <c r="A4" s="20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> partie 6 : Vrai</t>
+        </is>
+      </c>
+      <c r="B4" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" s="20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> partie 7 : Faux</t>
+        </is>
+      </c>
+      <c r="D4" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" s="20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> partie 8 : Faux</t>
+        </is>
+      </c>
+      <c r="F4" s="20" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" ht="12.8" customHeight="1" s="23">
+      <c r="A5" s="37" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> partie 6 : Faux</t>
+        </is>
+      </c>
+      <c r="B5" s="38" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" s="20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> partie 7 : Faux</t>
+        </is>
+      </c>
+      <c r="D5" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" s="20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> partie 8 : Faux</t>
+        </is>
+      </c>
+      <c r="F5" s="20" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" ht="12.8" customHeight="1" s="23">
+      <c r="A6" s="20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> partie 6 : Vrai</t>
+        </is>
+      </c>
+      <c r="B6" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" s="20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> partie 7 : Faux</t>
+        </is>
+      </c>
+      <c r="D6" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" s="20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> partie 8 : Faux</t>
+        </is>
+      </c>
+      <c r="F6" s="20" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" ht="12.8" customHeight="1" s="23">
+      <c r="A7" s="20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> partie 6 : Vrai</t>
+        </is>
+      </c>
+      <c r="B7" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" s="20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> partie 7 : Faux</t>
+        </is>
+      </c>
+      <c r="D7" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" s="20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> partie 8 : Faux</t>
+        </is>
+      </c>
+      <c r="F7" s="20" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" ht="12.8" customHeight="1" s="23">
+      <c r="A8" s="20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> partie 6 : Vrai</t>
+        </is>
+      </c>
+      <c r="B8" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" s="20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> partie 7 : Faux</t>
+        </is>
+      </c>
+      <c r="D8" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" s="20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> partie 8 : Faux</t>
+        </is>
+      </c>
+      <c r="F8" s="20" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" ht="12.8" customHeight="1" s="23">
+      <c r="A9" s="20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> partie 6 : Vrai</t>
+        </is>
+      </c>
+      <c r="B9" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" s="20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> partie 7 : Faux</t>
+        </is>
+      </c>
+      <c r="D9" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" s="20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> partie 8 : Faux</t>
+        </is>
+      </c>
+      <c r="F9" s="20" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" ht="12.8" customHeight="1" s="23">
+      <c r="A10" s="20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> partie 6 : Vrai</t>
+        </is>
+      </c>
+      <c r="B10" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" s="20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> partie 7 : Faux</t>
+        </is>
+      </c>
+      <c r="D10" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="E10" s="20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> partie 8 : Faux</t>
+        </is>
+      </c>
+      <c r="F10" s="20" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" ht="12.8" customHeight="1" s="23">
+      <c r="A11" s="20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> partie 6 : Vrai</t>
+        </is>
+      </c>
+      <c r="B11" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" s="20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> partie 7 : Faux</t>
+        </is>
+      </c>
+      <c r="D11" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="E11" s="20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> partie 8 : Faux</t>
+        </is>
+      </c>
+      <c r="F11" s="20" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" ht="12.8" customHeight="1" s="23">
+      <c r="A12" s="20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> partie 6 : Vrai</t>
+        </is>
+      </c>
+      <c r="B12" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" s="20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> partie 7 : Faux</t>
+        </is>
+      </c>
+      <c r="D12" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="E12" s="20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> partie 8 : Faux</t>
+        </is>
+      </c>
+      <c r="F12" s="20" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" ht="12.8" customHeight="1" s="23"/>
+    <row r="14" ht="12.8" customHeight="1" s="23"/>
+  </sheetData>
+  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentOddEven="0" differentFirst="0">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12 &amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12 Page &amp;P</oddFooter>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr filterMode="0">
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr fitToPage="0"/>
+  </sheetPr>
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <cols>
+    <col width="11.54" customWidth="1" style="20" min="1" max="1024"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="12.8" customHeight="1" s="23">
+      <c r="A1" s="35" t="inlineStr">
+        <is>
+          <t>Les électrons sont plus petits que les atomes</t>
+        </is>
+      </c>
+      <c r="B1" s="36" t="inlineStr">
+        <is>
+          <t>accuracy_Q6</t>
+        </is>
+      </c>
+      <c r="C1" s="24" t="inlineStr">
+        <is>
+          <t>Toute radioactivité résulte de l’action de l’homme</t>
+        </is>
+      </c>
+      <c r="D1" s="24" t="inlineStr">
+        <is>
+          <t>accuracy_Q7</t>
+        </is>
+      </c>
+      <c r="E1" s="24" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  La Terre fait le tour du Soleil en un mois</t>
+        </is>
+      </c>
+      <c r="F1" s="24" t="inlineStr">
+        <is>
+          <t>accuracy_Q8</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="12.8" customHeight="1" s="23">
+      <c r="A2" s="20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> partie 6 : Vrai</t>
+        </is>
+      </c>
+      <c r="B2" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> partie 7 : Faux</t>
+        </is>
+      </c>
+      <c r="D2" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" s="20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> partie 8 : Faux</t>
+        </is>
+      </c>
+      <c r="F2" s="20" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" ht="12.8" customHeight="1" s="23">
+      <c r="A3" s="20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> partie 6 : Vrai</t>
+        </is>
+      </c>
+      <c r="B3" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> partie 7 : Faux</t>
+        </is>
+      </c>
+      <c r="D3" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" s="20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> partie 8 : Faux</t>
+        </is>
+      </c>
+      <c r="F3" s="20" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" ht="12.8" customHeight="1" s="23">
+      <c r="A4" s="20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> partie 6 : Vrai</t>
+        </is>
+      </c>
+      <c r="B4" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" s="20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> partie 7 : Faux</t>
+        </is>
+      </c>
+      <c r="D4" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" s="20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> partie 8 : Faux</t>
+        </is>
+      </c>
+      <c r="F4" s="20" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" ht="12.8" customHeight="1" s="23">
+      <c r="A5" s="37" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> partie 6 : Faux</t>
+        </is>
+      </c>
+      <c r="B5" s="38" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" s="20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> partie 7 : Faux</t>
+        </is>
+      </c>
+      <c r="D5" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" s="20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> partie 8 : Faux</t>
+        </is>
+      </c>
+      <c r="F5" s="20" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" ht="12.8" customHeight="1" s="23">
+      <c r="A6" s="20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> partie 6 : Vrai</t>
+        </is>
+      </c>
+      <c r="B6" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" s="20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> partie 7 : Faux</t>
+        </is>
+      </c>
+      <c r="D6" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" s="20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> partie 8 : Faux</t>
+        </is>
+      </c>
+      <c r="F6" s="20" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" ht="12.8" customHeight="1" s="23">
+      <c r="A7" s="20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> partie 6 : Vrai</t>
+        </is>
+      </c>
+      <c r="B7" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" s="20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> partie 7 : Faux</t>
+        </is>
+      </c>
+      <c r="D7" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" s="20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> partie 8 : Faux</t>
+        </is>
+      </c>
+      <c r="F7" s="20" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" ht="12.8" customHeight="1" s="23">
+      <c r="A8" s="20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> partie 6 : Vrai</t>
+        </is>
+      </c>
+      <c r="B8" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" s="20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> partie 7 : Faux</t>
+        </is>
+      </c>
+      <c r="D8" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" s="20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> partie 8 : Faux</t>
+        </is>
+      </c>
+      <c r="F8" s="20" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" ht="12.8" customHeight="1" s="23">
+      <c r="A9" s="20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> partie 6 : Vrai</t>
+        </is>
+      </c>
+      <c r="B9" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" s="20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> partie 7 : Faux</t>
+        </is>
+      </c>
+      <c r="D9" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" s="20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> partie 8 : Faux</t>
+        </is>
+      </c>
+      <c r="F9" s="20" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" ht="12.8" customHeight="1" s="23">
+      <c r="A10" s="20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> partie 6 : Vrai</t>
+        </is>
+      </c>
+      <c r="B10" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" s="20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> partie 7 : Faux</t>
+        </is>
+      </c>
+      <c r="D10" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="E10" s="20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> partie 8 : Faux</t>
+        </is>
+      </c>
+      <c r="F10" s="20" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" ht="12.8" customHeight="1" s="23">
+      <c r="A11" s="20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> partie 6 : Vrai</t>
+        </is>
+      </c>
+      <c r="B11" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" s="20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> partie 7 : Faux</t>
+        </is>
+      </c>
+      <c r="D11" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="E11" s="20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> partie 8 : Faux</t>
+        </is>
+      </c>
+      <c r="F11" s="20" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" ht="12.8" customHeight="1" s="23">
+      <c r="A12" s="20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> partie 6 : Vrai</t>
+        </is>
+      </c>
+      <c r="B12" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" s="20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> partie 7 : Faux</t>
+        </is>
+      </c>
+      <c r="D12" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="E12" s="20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> partie 8 : Faux</t>
+        </is>
+      </c>
+      <c r="F12" s="20" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentOddEven="0" differentFirst="0">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12 &amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12 Page &amp;P</oddFooter>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr filterMode="0">
@@ -8817,7 +9521,7 @@
       <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.95703125" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="11.08" customWidth="1" style="20" min="6" max="6"/>
     <col width="11.52" customWidth="1" style="20" min="947" max="1024"/>
@@ -9015,10 +9719,10 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="I22" activeCellId="0" sqref="I22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="11.54" customWidth="1" style="20" min="1" max="1024"/>
   </cols>
@@ -9420,7 +10124,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="11.54" customWidth="1" style="20" min="1" max="1024"/>
   </cols>
@@ -9822,7 +10526,7 @@
       <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData>
     <row r="1" ht="16.05" customHeight="1" s="23">
       <c r="A1" s="20" t="inlineStr">
@@ -10230,7 +10934,7 @@
       <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData>
     <row r="1" ht="16.05" customHeight="1" s="23">
       <c r="A1" s="20" t="inlineStr">
@@ -10778,7 +11482,7 @@
       <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData>
     <row r="1" ht="16.05" customHeight="1" s="23">
       <c r="A1" s="20" t="inlineStr">
@@ -11322,15 +12026,14 @@
   </sheetPr>
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H15" activeCellId="0" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="11.31" customWidth="1" style="20" min="1" max="2"/>
-    <col width="11.52" customWidth="1" style="20" min="1010" max="1021"/>
-    <col width="11.52" customWidth="1" style="20" min="1022" max="1024"/>
+    <col width="11.52" customWidth="1" style="20" min="1010" max="1024"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.8" customHeight="1" s="23">
@@ -11445,7 +12148,7 @@
       <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="11.31" customWidth="1" style="20" min="1" max="3"/>
     <col width="21.53" customWidth="1" style="20" min="4" max="4"/>

</xml_diff>

<commit_message>
Ajout d'une fonction column_set_answer
</commit_message>
<xml_diff>
--- a/fichiers_xls/test.xlsx
+++ b/fichiers_xls/test.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="10" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="sheet1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Feuille2" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Feuille3" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Feuille4" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Feuille5" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Feuille5bis" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="color_line" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="cutinparts" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="cutinpartsbis" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="delete_lines" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="delete_lines_bis" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Feuille2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Feuille3" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Feuille4" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Feuille5" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Feuille5bis" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="color_line" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="cutinparts" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="cutinpartsbis" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="delete_lines" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="delete_lines_bis" sheetId="11" state="visible" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName name="_xlfn_T_TEST" hidden="0" function="0" vbProcedure="0">NA()</definedName>
@@ -408,14 +408,14 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0"/>
-          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
             <a:pPr>
               <a:defRPr sz="1400" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
@@ -448,8 +448,8 @@
       </layout>
       <overlay val="0"/>
       <spPr>
-        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="0">
+        <a:noFill/>
+        <a:ln w="0">
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
@@ -487,10 +487,10 @@
             </strRef>
           </tx>
           <spPr>
-            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:solidFill>
               <a:srgbClr val="5b9bd5"/>
             </a:solidFill>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="0">
+            <a:ln w="0">
               <a:noFill/>
               <a:prstDash val="solid"/>
             </a:ln>
@@ -498,9 +498,9 @@
           <invertIfNegative val="0"/>
           <dLbls>
             <txPr>
-              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square"/>
-              <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:bodyPr wrap="square"/>
+              <a:lstStyle/>
+              <a:p>
                 <a:pPr>
                   <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
@@ -653,7 +653,7 @@
         <minorTickMark val="none"/>
         <tickLblPos val="nextTo"/>
         <spPr>
-          <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="0">
+          <a:ln w="0">
             <a:solidFill>
               <a:srgbClr val="c0c0c0"/>
             </a:solidFill>
@@ -661,9 +661,9 @@
           </a:ln>
         </spPr>
         <txPr>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="-5400000"/>
-          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr rot="-5400000"/>
+          <a:lstStyle/>
+          <a:p>
             <a:pPr>
               <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
@@ -694,7 +694,7 @@
         <axPos val="l"/>
         <majorGridlines>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="0">
+            <a:ln w="0">
               <a:solidFill>
                 <a:srgbClr val="c0c0c0"/>
               </a:solidFill>
@@ -707,15 +707,15 @@
         <minorTickMark val="none"/>
         <tickLblPos val="nextTo"/>
         <spPr>
-          <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="0">
+          <a:ln w="0">
             <a:noFill/>
             <a:prstDash val="solid"/>
           </a:ln>
         </spPr>
         <txPr>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
             <a:pPr>
               <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
@@ -738,10 +738,10 @@
     <dispBlanksAs val="gap"/>
   </chart>
   <spPr>
-    <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+    <a:solidFill>
       <a:srgbClr val="ffffff"/>
     </a:solidFill>
-    <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="0">
+    <a:ln w="0">
       <a:solidFill>
         <a:srgbClr val="c0c0c0"/>
       </a:solidFill>
@@ -752,14 +752,14 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0"/>
-          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
             <a:pPr>
               <a:defRPr sz="1400" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
@@ -792,8 +792,8 @@
       </layout>
       <overlay val="0"/>
       <spPr>
-        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="0">
+        <a:noFill/>
+        <a:ln w="0">
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
@@ -831,10 +831,10 @@
             </strRef>
           </tx>
           <spPr>
-            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:solidFill>
               <a:srgbClr val="5b9bd5"/>
             </a:solidFill>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="0">
+            <a:ln w="0">
               <a:noFill/>
               <a:prstDash val="solid"/>
             </a:ln>
@@ -842,9 +842,9 @@
           <invertIfNegative val="0"/>
           <dLbls>
             <txPr>
-              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square"/>
-              <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:bodyPr wrap="square"/>
+              <a:lstStyle/>
+              <a:p>
                 <a:pPr>
                   <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
@@ -997,7 +997,7 @@
         <minorTickMark val="none"/>
         <tickLblPos val="nextTo"/>
         <spPr>
-          <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="0">
+          <a:ln w="0">
             <a:solidFill>
               <a:srgbClr val="c0c0c0"/>
             </a:solidFill>
@@ -1005,9 +1005,9 @@
           </a:ln>
         </spPr>
         <txPr>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="-5400000"/>
-          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr rot="-5400000"/>
+          <a:lstStyle/>
+          <a:p>
             <a:pPr>
               <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
@@ -1038,7 +1038,7 @@
         <axPos val="l"/>
         <majorGridlines>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="0">
+            <a:ln w="0">
               <a:solidFill>
                 <a:srgbClr val="c0c0c0"/>
               </a:solidFill>
@@ -1051,15 +1051,15 @@
         <minorTickMark val="none"/>
         <tickLblPos val="nextTo"/>
         <spPr>
-          <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="0">
+          <a:ln w="0">
             <a:noFill/>
             <a:prstDash val="solid"/>
           </a:ln>
         </spPr>
         <txPr>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
             <a:pPr>
               <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
@@ -1082,10 +1082,10 @@
     <dispBlanksAs val="gap"/>
   </chart>
   <spPr>
-    <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+    <a:solidFill>
       <a:srgbClr val="ffffff"/>
     </a:solidFill>
-    <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="0">
+    <a:ln w="0">
       <a:solidFill>
         <a:srgbClr val="c0c0c0"/>
       </a:solidFill>
@@ -1096,14 +1096,14 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0"/>
-          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
             <a:pPr>
               <a:defRPr sz="1400" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
@@ -1136,8 +1136,8 @@
       </layout>
       <overlay val="0"/>
       <spPr>
-        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="0">
+        <a:noFill/>
+        <a:ln w="0">
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
@@ -1176,10 +1176,10 @@
             </strRef>
           </tx>
           <spPr>
-            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:solidFill>
               <a:srgbClr val="5b9bd5"/>
             </a:solidFill>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="0">
+            <a:ln w="0">
               <a:noFill/>
               <a:prstDash val="solid"/>
             </a:ln>
@@ -1187,9 +1187,9 @@
           <invertIfNegative val="0"/>
           <dLbls>
             <txPr>
-              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square"/>
-              <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:bodyPr wrap="square"/>
+              <a:lstStyle/>
+              <a:p>
                 <a:pPr>
                   <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
@@ -1342,7 +1342,7 @@
         <minorTickMark val="none"/>
         <tickLblPos val="nextTo"/>
         <spPr>
-          <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="0">
+          <a:ln w="0">
             <a:solidFill>
               <a:srgbClr val="c0c0c0"/>
             </a:solidFill>
@@ -1350,9 +1350,9 @@
           </a:ln>
         </spPr>
         <txPr>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="-5400000"/>
-          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr rot="-5400000"/>
+          <a:lstStyle/>
+          <a:p>
             <a:pPr>
               <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
@@ -1383,7 +1383,7 @@
         <axPos val="l"/>
         <majorGridlines>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="0">
+            <a:ln w="0">
               <a:solidFill>
                 <a:srgbClr val="c0c0c0"/>
               </a:solidFill>
@@ -1396,15 +1396,15 @@
         <minorTickMark val="none"/>
         <tickLblPos val="nextTo"/>
         <spPr>
-          <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="0">
+          <a:ln w="0">
             <a:noFill/>
             <a:prstDash val="solid"/>
           </a:ln>
         </spPr>
         <txPr>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
             <a:pPr>
               <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
@@ -1427,10 +1427,10 @@
     <dispBlanksAs val="gap"/>
   </chart>
   <spPr>
-    <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+    <a:solidFill>
       <a:srgbClr val="ffffff"/>
     </a:solidFill>
-    <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="0">
+    <a:ln w="0">
       <a:solidFill>
         <a:srgbClr val="c0c0c0"/>
       </a:solidFill>
@@ -1441,14 +1441,14 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0"/>
-          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
             <a:pPr>
               <a:defRPr sz="1400" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
@@ -1481,8 +1481,8 @@
       </layout>
       <overlay val="0"/>
       <spPr>
-        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="0">
+        <a:noFill/>
+        <a:ln w="0">
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
@@ -1521,10 +1521,10 @@
             </strRef>
           </tx>
           <spPr>
-            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:solidFill>
               <a:srgbClr val="5b9bd5"/>
             </a:solidFill>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="0">
+            <a:ln w="0">
               <a:noFill/>
               <a:prstDash val="solid"/>
             </a:ln>
@@ -1532,9 +1532,9 @@
           <invertIfNegative val="0"/>
           <dLbls>
             <txPr>
-              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square"/>
-              <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:bodyPr wrap="square"/>
+              <a:lstStyle/>
+              <a:p>
                 <a:pPr>
                   <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
@@ -1687,7 +1687,7 @@
         <minorTickMark val="none"/>
         <tickLblPos val="nextTo"/>
         <spPr>
-          <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="0">
+          <a:ln w="0">
             <a:solidFill>
               <a:srgbClr val="c0c0c0"/>
             </a:solidFill>
@@ -1695,9 +1695,9 @@
           </a:ln>
         </spPr>
         <txPr>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="-5400000"/>
-          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr rot="-5400000"/>
+          <a:lstStyle/>
+          <a:p>
             <a:pPr>
               <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
@@ -1728,7 +1728,7 @@
         <axPos val="l"/>
         <majorGridlines>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="0">
+            <a:ln w="0">
               <a:solidFill>
                 <a:srgbClr val="c0c0c0"/>
               </a:solidFill>
@@ -1741,15 +1741,15 @@
         <minorTickMark val="none"/>
         <tickLblPos val="nextTo"/>
         <spPr>
-          <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="0">
+          <a:ln w="0">
             <a:noFill/>
             <a:prstDash val="solid"/>
           </a:ln>
         </spPr>
         <txPr>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
             <a:pPr>
               <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
@@ -1772,10 +1772,10 @@
     <dispBlanksAs val="gap"/>
   </chart>
   <spPr>
-    <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+    <a:solidFill>
       <a:srgbClr val="ffffff"/>
     </a:solidFill>
-    <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="0">
+    <a:ln w="0">
       <a:solidFill>
         <a:srgbClr val="c0c0c0"/>
       </a:solidFill>
@@ -1786,7 +1786,7 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <twoCellAnchor editAs="oneCell">
     <from>
       <col>102</col>
@@ -1806,9 +1806,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+      <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <c:chart r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -1818,7 +1818,7 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <twoCellAnchor editAs="oneCell">
     <from>
       <col>94</col>
@@ -1838,9 +1838,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+      <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <c:chart r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -1850,7 +1850,7 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <twoCellAnchor editAs="oneCell">
     <from>
       <col>101</col>
@@ -1870,9 +1870,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+      <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <c:chart r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -1882,7 +1882,7 @@
 </file>
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <twoCellAnchor editAs="oneCell">
     <from>
       <col>101</col>
@@ -1902,9 +1902,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+      <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <c:chart r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -2197,7 +2197,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr filterMode="0">
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
@@ -8803,7 +8803,7 @@
     <firstHeader/>
     <firstFooter/>
   </headerFooter>
-  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -8813,7 +8813,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -10515,7 +10515,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr filterMode="0">
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
@@ -10918,12 +10918,12 @@
     <firstHeader/>
     <firstFooter/>
   </headerFooter>
-  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr filterMode="0">
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
@@ -11466,12 +11466,12 @@
     <firstHeader/>
     <firstFooter/>
   </headerFooter>
-  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr filterMode="0">
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
@@ -12014,7 +12014,7 @@
     <firstHeader/>
     <firstFooter/>
   </headerFooter>
-  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Addition of the possibility to choose colum by label instead of number except for add_column_in_sheet_differently_sorted
</commit_message>
<xml_diff>
--- a/fichiers_xls/test.xlsx
+++ b/fichiers_xls/test.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="10" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -91,7 +91,7 @@
       <sz val="11"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="12">
     <fill>
       <patternFill/>
     </fill>
@@ -157,26 +157,6 @@
         <fgColor rgb="0000a933"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="002a6099"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00bf0041"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00ffff00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00ff0000"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -197,7 +177,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
@@ -320,21 +300,6 @@
     <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -442,8 +407,8 @@
           <yMode val="edge"/>
           <wMode val="factor"/>
           <hMode val="factor"/>
-          <x val="0.304284354173278"/>
-          <y val="0.0254365983295368"/>
+          <x val="0.30432576430293"/>
+          <y val="0.0255663840020251"/>
         </manualLayout>
       </layout>
       <overlay val="0"/>
@@ -462,10 +427,10 @@
           <yMode val="edge"/>
           <wMode val="factor"/>
           <hMode val="factor"/>
-          <x val="0.0129482703903523"/>
-          <y val="0.125031637560111"/>
-          <w val="0.96585211044113"/>
-          <h val="0.861300936471779"/>
+          <x val="0.0129392363313459"/>
+          <y val="0.125047462346538"/>
+          <w val="0.965812507928454"/>
+          <h val="0.861156815592963"/>
         </manualLayout>
       </layout>
       <barChart>
@@ -638,11 +603,11 @@
         </ser>
         <gapWidth val="219"/>
         <overlap val="-27"/>
-        <axId val="82962979"/>
-        <axId val="64313139"/>
+        <axId val="45756070"/>
+        <axId val="48929188"/>
       </barChart>
       <catAx>
-        <axId val="82962979"/>
+        <axId val="45756070"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
@@ -677,7 +642,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="64313139"/>
+        <crossAx val="48929188"/>
         <crossesAt val="0"/>
         <auto val="1"/>
         <lblAlgn val="ctr"/>
@@ -685,7 +650,7 @@
         <noMultiLvlLbl val="0"/>
       </catAx>
       <valAx>
-        <axId val="64313139"/>
+        <axId val="48929188"/>
         <scaling>
           <orientation val="minMax"/>
           <max val="100"/>
@@ -729,7 +694,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="82962979"/>
+        <crossAx val="45756070"/>
         <crossesAt val="1"/>
         <crossBetween val="midCat"/>
       </valAx>
@@ -786,8 +751,8 @@
           <yMode val="edge"/>
           <wMode val="factor"/>
           <hMode val="factor"/>
-          <x val="0.304283981357339"/>
-          <y val="0.0254365983295368"/>
+          <x val="0.304322876817138"/>
+          <y val="0.0255663840020251"/>
         </manualLayout>
       </layout>
       <overlay val="0"/>
@@ -806,10 +771,10 @@
           <yMode val="edge"/>
           <wMode val="factor"/>
           <hMode val="factor"/>
-          <x val="0.0129604801123667"/>
-          <y val="0.125031637560111"/>
-          <w val="0.965651535465747"/>
-          <h val="0.861300936471779"/>
+          <x val="0.0129431267533792"/>
+          <y val="0.125047462346538"/>
+          <w val="0.965570007651109"/>
+          <h val="0.861156815592963"/>
         </manualLayout>
       </layout>
       <barChart>
@@ -982,11 +947,11 @@
         </ser>
         <gapWidth val="219"/>
         <overlap val="-27"/>
-        <axId val="10632551"/>
-        <axId val="42813938"/>
+        <axId val="43487628"/>
+        <axId val="30788276"/>
       </barChart>
       <catAx>
-        <axId val="10632551"/>
+        <axId val="43487628"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
@@ -1021,7 +986,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="42813938"/>
+        <crossAx val="30788276"/>
         <crossesAt val="0"/>
         <auto val="1"/>
         <lblAlgn val="ctr"/>
@@ -1029,7 +994,7 @@
         <noMultiLvlLbl val="0"/>
       </catAx>
       <valAx>
-        <axId val="42813938"/>
+        <axId val="30788276"/>
         <scaling>
           <orientation val="minMax"/>
           <max val="100"/>
@@ -1073,7 +1038,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="10632551"/>
+        <crossAx val="43487628"/>
         <crossesAt val="1"/>
         <crossBetween val="midCat"/>
       </valAx>
@@ -1130,8 +1095,8 @@
           <yMode val="edge"/>
           <wMode val="factor"/>
           <hMode val="factor"/>
-          <x val="0.304372805617619"/>
-          <y val="0.0255631485699823"/>
+          <x val="0.304430985017533"/>
+          <y val="0.0256929502594608"/>
         </manualLayout>
       </layout>
       <overlay val="0"/>
@@ -1151,10 +1116,10 @@
           <yMode val="edge"/>
           <wMode val="factor"/>
           <hMode val="factor"/>
-          <x val="0.0524098308330674"/>
-          <y val="0.145279676031384"/>
-          <w val="0.926651771465049"/>
-          <h val="0.820931409769679"/>
+          <x val="0.0524067580490915"/>
+          <y val="0.145298063536261"/>
+          <w val="0.9266177876952501"/>
+          <h val="0.820782179470953"/>
         </manualLayout>
       </layout>
       <barChart>
@@ -1327,11 +1292,11 @@
         </ser>
         <gapWidth val="219"/>
         <overlap val="-27"/>
-        <axId val="83284912"/>
-        <axId val="19779740"/>
+        <axId val="6685342"/>
+        <axId val="30578753"/>
       </barChart>
       <catAx>
-        <axId val="83284912"/>
+        <axId val="6685342"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
@@ -1366,7 +1331,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="19779740"/>
+        <crossAx val="30578753"/>
         <crosses val="autoZero"/>
         <auto val="1"/>
         <lblAlgn val="ctr"/>
@@ -1374,7 +1339,7 @@
         <noMultiLvlLbl val="0"/>
       </catAx>
       <valAx>
-        <axId val="19779740"/>
+        <axId val="30578753"/>
         <scaling>
           <orientation val="minMax"/>
           <max val="100"/>
@@ -1418,7 +1383,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="83284912"/>
+        <crossAx val="6685342"/>
         <crossesAt val="1"/>
         <crossBetween val="midCat"/>
       </valAx>
@@ -1475,8 +1440,8 @@
           <yMode val="edge"/>
           <wMode val="factor"/>
           <hMode val="factor"/>
-          <x val="0.304436642195978"/>
-          <y val="0.0256896988104277"/>
+          <x val="0.304494740197641"/>
+          <y val="0.0258195165168966"/>
         </manualLayout>
       </layout>
       <overlay val="0"/>
@@ -1496,10 +1461,10 @@
           <yMode val="edge"/>
           <wMode val="factor"/>
           <hMode val="factor"/>
-          <x val="0.0524098308330674"/>
-          <y val="0.145279676031384"/>
-          <w val="0.926651771465049"/>
-          <h val="0.820931409769679"/>
+          <x val="0.0524067580490915"/>
+          <y val="0.145298063536261"/>
+          <w val="0.9266177876952501"/>
+          <h val="0.820782179470953"/>
         </manualLayout>
       </layout>
       <barChart>
@@ -1672,11 +1637,11 @@
         </ser>
         <gapWidth val="219"/>
         <overlap val="-27"/>
-        <axId val="53177077"/>
-        <axId val="26377073"/>
+        <axId val="46266503"/>
+        <axId val="60432670"/>
       </barChart>
       <catAx>
-        <axId val="53177077"/>
+        <axId val="46266503"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
@@ -1711,7 +1676,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="26377073"/>
+        <crossAx val="60432670"/>
         <crosses val="autoZero"/>
         <auto val="1"/>
         <lblAlgn val="ctr"/>
@@ -1719,7 +1684,7 @@
         <noMultiLvlLbl val="0"/>
       </catAx>
       <valAx>
-        <axId val="26377073"/>
+        <axId val="60432670"/>
         <scaling>
           <orientation val="minMax"/>
           <max val="100"/>
@@ -1763,7 +1728,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="53177077"/>
+        <crossAx val="46266503"/>
         <crossesAt val="1"/>
         <crossBetween val="midCat"/>
       </valAx>
@@ -1796,9 +1761,9 @@
     </from>
     <to>
       <col>109</col>
-      <colOff>39600</colOff>
+      <colOff>39240</colOff>
       <row>27</row>
-      <rowOff>83160</rowOff>
+      <rowOff>82800</rowOff>
     </to>
     <graphicFrame>
       <nvGraphicFramePr>
@@ -1828,9 +1793,9 @@
     </from>
     <to>
       <col>100</col>
-      <colOff>691560</colOff>
+      <colOff>691200</colOff>
       <row>30</row>
-      <rowOff>133200</rowOff>
+      <rowOff>132840</rowOff>
     </to>
     <graphicFrame>
       <nvGraphicFramePr>
@@ -1860,9 +1825,9 @@
     </from>
     <to>
       <col>107</col>
-      <colOff>691560</colOff>
+      <colOff>691200</colOff>
       <row>30</row>
-      <rowOff>132480</rowOff>
+      <rowOff>132120</rowOff>
     </to>
     <graphicFrame>
       <nvGraphicFramePr>
@@ -1892,9 +1857,9 @@
     </from>
     <to>
       <col>107</col>
-      <colOff>691560</colOff>
+      <colOff>691200</colOff>
       <row>30</row>
-      <rowOff>132480</rowOff>
+      <rowOff>132120</rowOff>
     </to>
     <graphicFrame>
       <nvGraphicFramePr>
@@ -2208,7 +2173,7 @@
       <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.43359375" defaultRowHeight="16.05" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.4453125" defaultRowHeight="16.05" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="16.2" customWidth="1" style="20" min="6" max="6"/>
     <col width="14.38" customWidth="1" style="21" min="7" max="7"/>
@@ -9167,7 +9132,7 @@
   </sheetPr>
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -9521,7 +9486,7 @@
       <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.95703125" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.9765625" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="11.08" customWidth="1" style="20" min="6" max="6"/>
     <col width="11.52" customWidth="1" style="20" min="947" max="1024"/>
@@ -9728,12 +9693,12 @@
   </cols>
   <sheetData>
     <row r="1" ht="12.8" customHeight="1" s="23">
-      <c r="A1" s="42" t="inlineStr">
+      <c r="A1" s="35" t="inlineStr">
         <is>
           <t>Les électrons sont plus petits que les atomes</t>
         </is>
       </c>
-      <c r="B1" s="44" t="inlineStr">
+      <c r="B1" s="36" t="inlineStr">
         <is>
           <t>accuracy_Q6</t>
         </is>
@@ -9838,12 +9803,12 @@
       </c>
     </row>
     <row r="5" ht="12.8" customHeight="1" s="23">
-      <c r="A5" s="43" t="inlineStr">
+      <c r="A5" s="37" t="inlineStr">
         <is>
           <t xml:space="preserve"> partie 6 : Faux</t>
         </is>
       </c>
-      <c r="B5" s="45" t="n">
+      <c r="B5" s="38" t="n">
         <v>0</v>
       </c>
       <c r="C5" s="20" t="inlineStr">
@@ -9872,12 +9837,12 @@
       <c r="B6" s="20" t="n">
         <v>1</v>
       </c>
-      <c r="C6" s="46" t="inlineStr">
+      <c r="C6" s="32" t="inlineStr">
         <is>
           <t xml:space="preserve"> partie 7 : Vrai</t>
         </is>
       </c>
-      <c r="D6" s="45" t="n">
+      <c r="D6" s="38" t="n">
         <v>0</v>
       </c>
       <c r="E6" s="20" t="inlineStr">
@@ -10080,12 +10045,12 @@
       <c r="B14" s="20" t="n">
         <v>1</v>
       </c>
-      <c r="C14" s="46" t="inlineStr">
+      <c r="C14" s="32" t="inlineStr">
         <is>
           <t xml:space="preserve"> partie 7 : Vrai</t>
         </is>
       </c>
-      <c r="D14" s="45" t="n">
+      <c r="D14" s="38" t="n">
         <v>0</v>
       </c>
       <c r="E14" s="20" t="inlineStr">
@@ -10526,7 +10491,7 @@
       <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData>
     <row r="1" ht="16.05" customHeight="1" s="23">
       <c r="A1" s="20" t="inlineStr">
@@ -10934,7 +10899,7 @@
       <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData>
     <row r="1" ht="16.05" customHeight="1" s="23">
       <c r="A1" s="20" t="inlineStr">
@@ -11482,7 +11447,7 @@
       <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData>
     <row r="1" ht="16.05" customHeight="1" s="23">
       <c r="A1" s="20" t="inlineStr">
@@ -12026,14 +11991,15 @@
   </sheetPr>
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H15" activeCellId="0" sqref="H15"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="11.31" customWidth="1" style="20" min="1" max="2"/>
-    <col width="11.52" customWidth="1" style="20" min="1010" max="1024"/>
+    <col width="11.52" customWidth="1" style="20" min="998" max="1012"/>
+    <col width="11.52" customWidth="1" style="20" min="1013" max="1024"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.8" customHeight="1" s="23">
@@ -12148,7 +12114,7 @@
       <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="11.31" customWidth="1" style="20" min="1" max="3"/>
     <col width="21.53" customWidth="1" style="20" min="4" max="4"/>

</xml_diff>

<commit_message>
Ajout du choix des colonnes par l'étiquette dans add_column_in_sheet_differently_sorted
</commit_message>
<xml_diff>
--- a/fichiers_xls/test.xlsx
+++ b/fichiers_xls/test.xlsx
@@ -10485,7 +10485,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
@@ -10516,6 +10516,16 @@
       </c>
       <c r="E1" s="20" t="inlineStr">
         <is>
+          <t>Prénom</t>
+        </is>
+      </c>
+      <c r="F1" s="20" t="inlineStr">
+        <is>
+          <t>Note/10,00</t>
+        </is>
+      </c>
+      <c r="G1" s="20" t="inlineStr">
+        <is>
           <t>Temps utilisé</t>
         </is>
       </c>
@@ -10541,7 +10551,17 @@
           <t>Terminé</t>
         </is>
       </c>
-      <c r="E2" s="25" t="inlineStr">
+      <c r="E2" s="20" t="inlineStr">
+        <is>
+          <t>Houzefa</t>
+        </is>
+      </c>
+      <c r="F2" s="20" t="inlineStr">
+        <is>
+          <t>7,83</t>
+        </is>
+      </c>
+      <c r="G2" s="25" t="inlineStr">
         <is>
           <t>5 min 49 s</t>
         </is>
@@ -10568,7 +10588,17 @@
           <t>Terminé</t>
         </is>
       </c>
-      <c r="E3" s="25" t="inlineStr">
+      <c r="E3" s="20" t="inlineStr">
+        <is>
+          <t>Yasmine</t>
+        </is>
+      </c>
+      <c r="F3" s="20" t="inlineStr">
+        <is>
+          <t>7,83</t>
+        </is>
+      </c>
+      <c r="G3" s="25" t="inlineStr">
         <is>
           <t>7 min 22 s</t>
         </is>
@@ -10595,7 +10625,17 @@
           <t>Terminé</t>
         </is>
       </c>
-      <c r="E4" s="25" t="inlineStr">
+      <c r="E4" s="20" t="inlineStr">
+        <is>
+          <t>Zina</t>
+        </is>
+      </c>
+      <c r="F4" s="20" t="inlineStr">
+        <is>
+          <t>7,28</t>
+        </is>
+      </c>
+      <c r="G4" s="25" t="inlineStr">
         <is>
           <t>5 min 15 s</t>
         </is>
@@ -10622,7 +10662,17 @@
           <t>Terminé</t>
         </is>
       </c>
-      <c r="E5" s="25" t="inlineStr">
+      <c r="E5" s="20" t="inlineStr">
+        <is>
+          <t>Aboubaker</t>
+        </is>
+      </c>
+      <c r="F5" s="20" t="inlineStr">
+        <is>
+          <t>7,98</t>
+        </is>
+      </c>
+      <c r="G5" s="25" t="inlineStr">
         <is>
           <t>7 min 57 s</t>
         </is>
@@ -10649,7 +10699,17 @@
           <t>Terminé</t>
         </is>
       </c>
-      <c r="E6" s="25" t="inlineStr">
+      <c r="E6" s="20" t="inlineStr">
+        <is>
+          <t>Yasmine</t>
+        </is>
+      </c>
+      <c r="F6" s="20" t="inlineStr">
+        <is>
+          <t>7,83</t>
+        </is>
+      </c>
+      <c r="G6" s="25" t="inlineStr">
         <is>
           <t>7 min 44 s</t>
         </is>
@@ -10676,7 +10736,17 @@
           <t>Terminé</t>
         </is>
       </c>
-      <c r="E7" s="28" t="inlineStr">
+      <c r="E7" s="20" t="inlineStr">
+        <is>
+          <t>Hassan Mahamat</t>
+        </is>
+      </c>
+      <c r="F7" s="20" t="inlineStr">
+        <is>
+          <t>7,52</t>
+        </is>
+      </c>
+      <c r="G7" s="28" t="inlineStr">
         <is>
           <t>23 min 37 s</t>
         </is>
@@ -10703,7 +10773,17 @@
           <t>Terminé</t>
         </is>
       </c>
-      <c r="E8" s="25" t="inlineStr">
+      <c r="E8" s="20" t="inlineStr">
+        <is>
+          <t>Yacine</t>
+        </is>
+      </c>
+      <c r="F8" s="20" t="inlineStr">
+        <is>
+          <t>8,07</t>
+        </is>
+      </c>
+      <c r="G8" s="25" t="inlineStr">
         <is>
           <t>4 min 17 s</t>
         </is>
@@ -10730,7 +10810,17 @@
           <t>Terminé</t>
         </is>
       </c>
-      <c r="E9" s="25" t="inlineStr">
+      <c r="E9" s="20" t="inlineStr">
+        <is>
+          <t>Paola</t>
+        </is>
+      </c>
+      <c r="F9" s="20" t="inlineStr">
+        <is>
+          <t>7,16</t>
+        </is>
+      </c>
+      <c r="G9" s="25" t="inlineStr">
         <is>
           <t>8 min 33 s</t>
         </is>
@@ -10757,7 +10847,17 @@
           <t>Terminé</t>
         </is>
       </c>
-      <c r="E10" s="25" t="inlineStr">
+      <c r="E10" s="39" t="inlineStr">
+        <is>
+          <t>Rodolphe</t>
+        </is>
+      </c>
+      <c r="F10" s="20" t="inlineStr">
+        <is>
+          <t>8,88</t>
+        </is>
+      </c>
+      <c r="G10" s="25" t="inlineStr">
         <is>
           <t>15 min 32 s</t>
         </is>
@@ -10784,7 +10884,17 @@
           <t>Terminé</t>
         </is>
       </c>
-      <c r="E11" s="25" t="inlineStr">
+      <c r="E11" s="20" t="inlineStr">
+        <is>
+          <t>Nouh</t>
+        </is>
+      </c>
+      <c r="F11" s="20" t="inlineStr">
+        <is>
+          <t>7,35</t>
+        </is>
+      </c>
+      <c r="G11" s="25" t="inlineStr">
         <is>
           <t>9 min 27 s</t>
         </is>
@@ -10811,7 +10921,17 @@
           <t>Terminé</t>
         </is>
       </c>
-      <c r="E12" s="25" t="inlineStr">
+      <c r="E12" s="20" t="inlineStr">
+        <is>
+          <t>Iness</t>
+        </is>
+      </c>
+      <c r="F12" s="20" t="inlineStr">
+        <is>
+          <t>6,51</t>
+        </is>
+      </c>
+      <c r="G12" s="25" t="inlineStr">
         <is>
           <t>10 min 33 s</t>
         </is>
@@ -10838,7 +10958,17 @@
           <t>Terminé</t>
         </is>
       </c>
-      <c r="E13" s="25" t="inlineStr">
+      <c r="E13" s="20" t="inlineStr">
+        <is>
+          <t>Zakaria</t>
+        </is>
+      </c>
+      <c r="F13" s="20" t="inlineStr">
+        <is>
+          <t>7,70</t>
+        </is>
+      </c>
+      <c r="G13" s="25" t="inlineStr">
         <is>
           <t>9 min 14 s</t>
         </is>
@@ -10865,7 +10995,17 @@
           <t>Terminé</t>
         </is>
       </c>
-      <c r="E14" s="28" t="inlineStr">
+      <c r="E14" s="39" t="inlineStr">
+        <is>
+          <t>Christian</t>
+        </is>
+      </c>
+      <c r="F14" s="20" t="inlineStr">
+        <is>
+          <t>6,72</t>
+        </is>
+      </c>
+      <c r="G14" s="28" t="inlineStr">
         <is>
           <t>21 min 49 s</t>
         </is>

</xml_diff>

<commit_message>
feat(commands) : add in utils.py a class UtilsForCommands. It allows to ask the user to enter an arbitrary number of optional arguments in the shell.
</commit_message>
<xml_diff>
--- a/fichiers_xls/test.xlsx
+++ b/fichiers_xls/test.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -395,8 +395,8 @@
           <yMode val="edge"/>
           <wMode val="factor"/>
           <hMode val="factor"/>
-          <x val="0.304454976303318"/>
-          <y val="0.0259559382122056"/>
+          <x val="0.30458577090017"/>
+          <y val="0.0263457884737175"/>
         </manualLayout>
       </layout>
       <overlay val="0"/>
@@ -415,10 +415,10 @@
           <yMode val="edge"/>
           <wMode val="factor"/>
           <hMode val="factor"/>
-          <x val="0.0128909952606635"/>
-          <y val="0.125094960749557"/>
-          <w val="0.9656240126382311"/>
-          <h val="0.860724233983287"/>
+          <x val="0.0128326099264012"/>
+          <y val="0.125142495250158"/>
+          <w val="0.965402277159213"/>
+          <h val="0.860291323622546"/>
         </manualLayout>
       </layout>
       <barChart>
@@ -591,11 +591,11 @@
         </ser>
         <gapWidth val="219"/>
         <overlap val="-27"/>
-        <axId val="54704306"/>
-        <axId val="58898256"/>
+        <axId val="60210764"/>
+        <axId val="39655215"/>
       </barChart>
       <catAx>
-        <axId val="54704306"/>
+        <axId val="60210764"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
@@ -630,7 +630,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="58898256"/>
+        <crossAx val="39655215"/>
         <crossesAt val="0"/>
         <auto val="1"/>
         <lblAlgn val="ctr"/>
@@ -638,7 +638,7 @@
         <noMultiLvlLbl val="0"/>
       </catAx>
       <valAx>
-        <axId val="58898256"/>
+        <axId val="39655215"/>
         <scaling>
           <orientation val="minMax"/>
           <max val="100"/>
@@ -682,7 +682,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="54704306"/>
+        <crossAx val="60210764"/>
         <crossesAt val="1"/>
         <crossBetween val="midCat"/>
       </valAx>
@@ -739,8 +739,8 @@
           <yMode val="edge"/>
           <wMode val="factor"/>
           <hMode val="factor"/>
-          <x val="0.304436252701157"/>
-          <y val="0.0259559382122056"/>
+          <x val="0.304590060145616"/>
+          <y val="0.0263457884737175"/>
         </manualLayout>
       </layout>
       <overlay val="0"/>
@@ -759,10 +759,10 @@
           <yMode val="edge"/>
           <wMode val="factor"/>
           <hMode val="factor"/>
-          <x val="0.0129019956781492"/>
-          <y val="0.125094960749557"/>
-          <w val="0.965361637218762"/>
-          <h val="0.860724233983287"/>
+          <x val="0.012852168407724"/>
+          <y val="0.125142495250158"/>
+          <w val="0.965115542893321"/>
+          <h val="0.860291323622546"/>
         </manualLayout>
       </layout>
       <barChart>
@@ -935,11 +935,11 @@
         </ser>
         <gapWidth val="219"/>
         <overlap val="-27"/>
-        <axId val="16642026"/>
-        <axId val="26930782"/>
+        <axId val="16185274"/>
+        <axId val="62137394"/>
       </barChart>
       <catAx>
-        <axId val="16642026"/>
+        <axId val="16185274"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
@@ -974,7 +974,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="26930782"/>
+        <crossAx val="62137394"/>
         <crossesAt val="0"/>
         <auto val="1"/>
         <lblAlgn val="ctr"/>
@@ -982,7 +982,7 @@
         <noMultiLvlLbl val="0"/>
       </catAx>
       <valAx>
-        <axId val="26930782"/>
+        <axId val="62137394"/>
         <scaling>
           <orientation val="minMax"/>
           <max val="100"/>
@@ -1026,7 +1026,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="16642026"/>
+        <crossAx val="16185274"/>
         <crossesAt val="1"/>
         <crossBetween val="midCat"/>
       </valAx>
@@ -1083,8 +1083,8 @@
           <yMode val="edge"/>
           <wMode val="factor"/>
           <hMode val="factor"/>
-          <x val="0.304544010168414"/>
-          <y val="0.0260825525449481"/>
+          <x val="0.304697391744746"/>
+          <y val="0.0264724509183027"/>
         </manualLayout>
       </layout>
       <overlay val="0"/>
@@ -1104,10 +1104,10 @@
           <yMode val="edge"/>
           <wMode val="factor"/>
           <hMode val="factor"/>
-          <x val="0.0523673339688592"/>
-          <y val="0.145353253988351"/>
-          <w val="0.926469653638386"/>
-          <h val="0.82033426183844"/>
+          <x val="0.0523550265890099"/>
+          <y val="0.145408486383787"/>
+          <w val="0.926373765510256"/>
+          <h val="0.819886003799873"/>
         </manualLayout>
       </layout>
       <barChart>
@@ -1280,11 +1280,11 @@
         </ser>
         <gapWidth val="219"/>
         <overlap val="-27"/>
-        <axId val="68931994"/>
-        <axId val="89550226"/>
+        <axId val="42916953"/>
+        <axId val="10666216"/>
       </barChart>
       <catAx>
-        <axId val="68931994"/>
+        <axId val="42916953"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
@@ -1319,7 +1319,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="89550226"/>
+        <crossAx val="10666216"/>
         <crosses val="autoZero"/>
         <auto val="1"/>
         <lblAlgn val="ctr"/>
@@ -1327,7 +1327,7 @@
         <noMultiLvlLbl val="0"/>
       </catAx>
       <valAx>
-        <axId val="89550226"/>
+        <axId val="10666216"/>
         <scaling>
           <orientation val="minMax"/>
           <max val="100"/>
@@ -1371,7 +1371,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="68931994"/>
+        <crossAx val="42916953"/>
         <crossesAt val="1"/>
         <crossBetween val="midCat"/>
       </valAx>
@@ -1428,8 +1428,8 @@
           <yMode val="edge"/>
           <wMode val="factor"/>
           <hMode val="factor"/>
-          <x val="0.304607562758182"/>
-          <y val="0.0262091668776906"/>
+          <x val="0.304760698911117"/>
+          <y val="0.0265991133628879"/>
         </manualLayout>
       </layout>
       <overlay val="0"/>
@@ -1449,10 +1449,10 @@
           <yMode val="edge"/>
           <wMode val="factor"/>
           <hMode val="factor"/>
-          <x val="0.0523673339688592"/>
-          <y val="0.145353253988351"/>
-          <w val="0.926469653638386"/>
-          <h val="0.82033426183844"/>
+          <x val="0.0523550265890099"/>
+          <y val="0.145408486383787"/>
+          <w val="0.926373765510256"/>
+          <h val="0.819886003799873"/>
         </manualLayout>
       </layout>
       <barChart>
@@ -1625,11 +1625,11 @@
         </ser>
         <gapWidth val="219"/>
         <overlap val="-27"/>
-        <axId val="58469090"/>
-        <axId val="4680451"/>
+        <axId val="67993797"/>
+        <axId val="68842535"/>
       </barChart>
       <catAx>
-        <axId val="58469090"/>
+        <axId val="67993797"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
@@ -1664,7 +1664,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="4680451"/>
+        <crossAx val="68842535"/>
         <crosses val="autoZero"/>
         <auto val="1"/>
         <lblAlgn val="ctr"/>
@@ -1672,7 +1672,7 @@
         <noMultiLvlLbl val="0"/>
       </catAx>
       <valAx>
-        <axId val="4680451"/>
+        <axId val="68842535"/>
         <scaling>
           <orientation val="minMax"/>
           <max val="100"/>
@@ -1716,7 +1716,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="58469090"/>
+        <crossAx val="67993797"/>
         <crossesAt val="1"/>
         <crossBetween val="midCat"/>
       </valAx>
@@ -1742,16 +1742,16 @@
 <wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <twoCellAnchor editAs="oneCell">
     <from>
-      <col>102</col>
-      <colOff>9360</colOff>
+      <col>99</col>
+      <colOff>10080</colOff>
       <row>13</row>
-      <rowOff>92880</rowOff>
+      <rowOff>93960</rowOff>
     </from>
     <to>
-      <col>109</col>
+      <col>106</col>
       <colOff>38520</colOff>
-      <row>27</row>
-      <rowOff>82080</rowOff>
+      <row>30</row>
+      <rowOff>131040</rowOff>
     </to>
     <graphicFrame>
       <nvGraphicFramePr>
@@ -1781,9 +1781,9 @@
     </from>
     <to>
       <col>100</col>
-      <colOff>690120</colOff>
+      <colOff>689040</colOff>
       <row>30</row>
-      <rowOff>131760</rowOff>
+      <rowOff>130680</rowOff>
     </to>
     <graphicFrame>
       <nvGraphicFramePr>
@@ -1813,9 +1813,9 @@
     </from>
     <to>
       <col>107</col>
-      <colOff>690120</colOff>
+      <colOff>689040</colOff>
       <row>30</row>
-      <rowOff>131040</rowOff>
+      <rowOff>129960</rowOff>
     </to>
     <graphicFrame>
       <nvGraphicFramePr>
@@ -1845,9 +1845,9 @@
     </from>
     <to>
       <col>107</col>
-      <colOff>690120</colOff>
+      <colOff>689040</colOff>
       <row>30</row>
-      <rowOff>131040</rowOff>
+      <rowOff>129960</rowOff>
     </to>
     <graphicFrame>
       <nvGraphicFramePr>
@@ -2157,25 +2157,24 @@
   </sheetPr>
   <dimension ref="A1:DJ14"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K15" activeCellId="0" sqref="K15"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="J1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.48828125" defaultRowHeight="16.05" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.54296875" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="16.2" customWidth="1" style="18" min="6" max="6"/>
     <col width="14.38" customWidth="1" style="19" min="7" max="7"/>
     <col width="140.36" customWidth="1" style="18" min="10" max="10"/>
     <col width="13.5" customWidth="1" style="18" min="12" max="12"/>
-    <col width="13.5" customWidth="1" style="18" min="14" max="14"/>
-    <col width="139.25" customWidth="1" style="18" min="37" max="37"/>
-    <col width="15.61" customWidth="1" style="18" min="38" max="38"/>
-    <col width="15.61" customWidth="1" style="20" min="39" max="39"/>
-    <col width="37.25" customWidth="1" style="18" min="40" max="40"/>
-    <col width="37.25" customWidth="1" style="20" min="42" max="42"/>
-    <col width="11.5" customWidth="1" style="19" min="43" max="43"/>
-    <col width="15.61" customWidth="1" style="20" min="78" max="78"/>
-    <col width="11.5" customWidth="1" style="20" min="79" max="79"/>
+    <col width="139.25" customWidth="1" style="18" min="34" max="34"/>
+    <col width="15.61" customWidth="1" style="18" min="35" max="35"/>
+    <col width="15.61" customWidth="1" style="20" min="36" max="36"/>
+    <col width="37.25" customWidth="1" style="18" min="37" max="37"/>
+    <col width="37.25" customWidth="1" style="20" min="39" max="39"/>
+    <col width="11.5" customWidth="1" style="19" min="40" max="40"/>
+    <col width="15.61" customWidth="1" style="20" min="75" max="75"/>
+    <col width="11.5" customWidth="1" style="20" min="76" max="76"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.05" customHeight="1" s="21">
@@ -7151,1466 +7150,6 @@
         </is>
       </c>
     </row>
-    <row r="64076" ht="12.8" customHeight="1" s="21"/>
-    <row r="64077" ht="12.8" customHeight="1" s="21"/>
-    <row r="64078" ht="12.8" customHeight="1" s="21"/>
-    <row r="64079" ht="12.8" customHeight="1" s="21"/>
-    <row r="64080" ht="12.8" customHeight="1" s="21"/>
-    <row r="64081" ht="12.8" customHeight="1" s="21"/>
-    <row r="64082" ht="12.8" customHeight="1" s="21"/>
-    <row r="64083" ht="12.8" customHeight="1" s="21"/>
-    <row r="64084" ht="12.8" customHeight="1" s="21"/>
-    <row r="64085" ht="12.8" customHeight="1" s="21"/>
-    <row r="64086" ht="12.8" customHeight="1" s="21"/>
-    <row r="64087" ht="12.8" customHeight="1" s="21"/>
-    <row r="64088" ht="12.8" customHeight="1" s="21"/>
-    <row r="64089" ht="12.8" customHeight="1" s="21"/>
-    <row r="64090" ht="12.8" customHeight="1" s="21"/>
-    <row r="64091" ht="12.8" customHeight="1" s="21"/>
-    <row r="64092" ht="12.8" customHeight="1" s="21"/>
-    <row r="64093" ht="12.8" customHeight="1" s="21"/>
-    <row r="64094" ht="12.8" customHeight="1" s="21"/>
-    <row r="64095" ht="12.8" customHeight="1" s="21"/>
-    <row r="64096" ht="12.8" customHeight="1" s="21"/>
-    <row r="64097" ht="12.8" customHeight="1" s="21"/>
-    <row r="64098" ht="12.8" customHeight="1" s="21"/>
-    <row r="64099" ht="12.8" customHeight="1" s="21"/>
-    <row r="64100" ht="12.8" customHeight="1" s="21"/>
-    <row r="64101" ht="12.8" customHeight="1" s="21"/>
-    <row r="64102" ht="12.8" customHeight="1" s="21"/>
-    <row r="64103" ht="12.8" customHeight="1" s="21"/>
-    <row r="64104" ht="12.8" customHeight="1" s="21"/>
-    <row r="64105" ht="12.8" customHeight="1" s="21"/>
-    <row r="64106" ht="12.8" customHeight="1" s="21"/>
-    <row r="64107" ht="12.8" customHeight="1" s="21"/>
-    <row r="64108" ht="12.8" customHeight="1" s="21"/>
-    <row r="64109" ht="12.8" customHeight="1" s="21"/>
-    <row r="64110" ht="12.8" customHeight="1" s="21"/>
-    <row r="64111" ht="12.8" customHeight="1" s="21"/>
-    <row r="64112" ht="12.8" customHeight="1" s="21"/>
-    <row r="64113" ht="12.8" customHeight="1" s="21"/>
-    <row r="64114" ht="12.8" customHeight="1" s="21"/>
-    <row r="64115" ht="12.8" customHeight="1" s="21"/>
-    <row r="64116" ht="12.8" customHeight="1" s="21"/>
-    <row r="64117" ht="12.8" customHeight="1" s="21"/>
-    <row r="64118" ht="12.8" customHeight="1" s="21"/>
-    <row r="64119" ht="12.8" customHeight="1" s="21"/>
-    <row r="64120" ht="12.8" customHeight="1" s="21"/>
-    <row r="64121" ht="12.8" customHeight="1" s="21"/>
-    <row r="64122" ht="12.8" customHeight="1" s="21"/>
-    <row r="64123" ht="12.8" customHeight="1" s="21"/>
-    <row r="64124" ht="12.8" customHeight="1" s="21"/>
-    <row r="64125" ht="12.8" customHeight="1" s="21"/>
-    <row r="64126" ht="12.8" customHeight="1" s="21"/>
-    <row r="64127" ht="12.8" customHeight="1" s="21"/>
-    <row r="64128" ht="12.8" customHeight="1" s="21"/>
-    <row r="64129" ht="12.8" customHeight="1" s="21"/>
-    <row r="64130" ht="12.8" customHeight="1" s="21"/>
-    <row r="64131" ht="12.8" customHeight="1" s="21"/>
-    <row r="64132" ht="12.8" customHeight="1" s="21"/>
-    <row r="64133" ht="12.8" customHeight="1" s="21"/>
-    <row r="64134" ht="12.8" customHeight="1" s="21"/>
-    <row r="64135" ht="12.8" customHeight="1" s="21"/>
-    <row r="64136" ht="12.8" customHeight="1" s="21"/>
-    <row r="64137" ht="12.8" customHeight="1" s="21"/>
-    <row r="64138" ht="12.8" customHeight="1" s="21"/>
-    <row r="64139" ht="12.8" customHeight="1" s="21"/>
-    <row r="64140" ht="12.8" customHeight="1" s="21"/>
-    <row r="64141" ht="12.8" customHeight="1" s="21"/>
-    <row r="64142" ht="12.8" customHeight="1" s="21"/>
-    <row r="64143" ht="12.8" customHeight="1" s="21"/>
-    <row r="64144" ht="12.8" customHeight="1" s="21"/>
-    <row r="64145" ht="12.8" customHeight="1" s="21"/>
-    <row r="64146" ht="12.8" customHeight="1" s="21"/>
-    <row r="64147" ht="12.8" customHeight="1" s="21"/>
-    <row r="64148" ht="12.8" customHeight="1" s="21"/>
-    <row r="64149" ht="12.8" customHeight="1" s="21"/>
-    <row r="64150" ht="12.8" customHeight="1" s="21"/>
-    <row r="64151" ht="12.8" customHeight="1" s="21"/>
-    <row r="64152" ht="12.8" customHeight="1" s="21"/>
-    <row r="64153" ht="12.8" customHeight="1" s="21"/>
-    <row r="64154" ht="12.8" customHeight="1" s="21"/>
-    <row r="64155" ht="12.8" customHeight="1" s="21"/>
-    <row r="64156" ht="12.8" customHeight="1" s="21"/>
-    <row r="64157" ht="12.8" customHeight="1" s="21"/>
-    <row r="64158" ht="12.8" customHeight="1" s="21"/>
-    <row r="64159" ht="12.8" customHeight="1" s="21"/>
-    <row r="64160" ht="12.8" customHeight="1" s="21"/>
-    <row r="64161" ht="12.8" customHeight="1" s="21"/>
-    <row r="64162" ht="12.8" customHeight="1" s="21"/>
-    <row r="64163" ht="12.8" customHeight="1" s="21"/>
-    <row r="64164" ht="12.8" customHeight="1" s="21"/>
-    <row r="64165" ht="12.8" customHeight="1" s="21"/>
-    <row r="64166" ht="12.8" customHeight="1" s="21"/>
-    <row r="64167" ht="12.8" customHeight="1" s="21"/>
-    <row r="64168" ht="12.8" customHeight="1" s="21"/>
-    <row r="64169" ht="12.8" customHeight="1" s="21"/>
-    <row r="64170" ht="12.8" customHeight="1" s="21"/>
-    <row r="64171" ht="12.8" customHeight="1" s="21"/>
-    <row r="64172" ht="12.8" customHeight="1" s="21"/>
-    <row r="64173" ht="12.8" customHeight="1" s="21"/>
-    <row r="64174" ht="12.8" customHeight="1" s="21"/>
-    <row r="64175" ht="12.8" customHeight="1" s="21"/>
-    <row r="64176" ht="12.8" customHeight="1" s="21"/>
-    <row r="64177" ht="12.8" customHeight="1" s="21"/>
-    <row r="64178" ht="12.8" customHeight="1" s="21"/>
-    <row r="64179" ht="12.8" customHeight="1" s="21"/>
-    <row r="64180" ht="12.8" customHeight="1" s="21"/>
-    <row r="64181" ht="12.8" customHeight="1" s="21"/>
-    <row r="64182" ht="12.8" customHeight="1" s="21"/>
-    <row r="64183" ht="12.8" customHeight="1" s="21"/>
-    <row r="64184" ht="12.8" customHeight="1" s="21"/>
-    <row r="64185" ht="12.8" customHeight="1" s="21"/>
-    <row r="64186" ht="12.8" customHeight="1" s="21"/>
-    <row r="64187" ht="12.8" customHeight="1" s="21"/>
-    <row r="64188" ht="12.8" customHeight="1" s="21"/>
-    <row r="64189" ht="12.8" customHeight="1" s="21"/>
-    <row r="64190" ht="12.8" customHeight="1" s="21"/>
-    <row r="64191" ht="12.8" customHeight="1" s="21"/>
-    <row r="64192" ht="12.8" customHeight="1" s="21"/>
-    <row r="64193" ht="12.8" customHeight="1" s="21"/>
-    <row r="64194" ht="12.8" customHeight="1" s="21"/>
-    <row r="64195" ht="12.8" customHeight="1" s="21"/>
-    <row r="64196" ht="12.8" customHeight="1" s="21"/>
-    <row r="64197" ht="12.8" customHeight="1" s="21"/>
-    <row r="64198" ht="12.8" customHeight="1" s="21"/>
-    <row r="64199" ht="12.8" customHeight="1" s="21"/>
-    <row r="64200" ht="12.8" customHeight="1" s="21"/>
-    <row r="64201" ht="12.8" customHeight="1" s="21"/>
-    <row r="64202" ht="12.8" customHeight="1" s="21"/>
-    <row r="64203" ht="12.8" customHeight="1" s="21"/>
-    <row r="64204" ht="12.8" customHeight="1" s="21"/>
-    <row r="64205" ht="12.8" customHeight="1" s="21"/>
-    <row r="64206" ht="12.8" customHeight="1" s="21"/>
-    <row r="64207" ht="12.8" customHeight="1" s="21"/>
-    <row r="64208" ht="12.8" customHeight="1" s="21"/>
-    <row r="64209" ht="12.8" customHeight="1" s="21"/>
-    <row r="64210" ht="12.8" customHeight="1" s="21"/>
-    <row r="64211" ht="12.8" customHeight="1" s="21"/>
-    <row r="64212" ht="12.8" customHeight="1" s="21"/>
-    <row r="64213" ht="12.8" customHeight="1" s="21"/>
-    <row r="64214" ht="12.8" customHeight="1" s="21"/>
-    <row r="64215" ht="12.8" customHeight="1" s="21"/>
-    <row r="64216" ht="12.8" customHeight="1" s="21"/>
-    <row r="64217" ht="12.8" customHeight="1" s="21"/>
-    <row r="64218" ht="12.8" customHeight="1" s="21"/>
-    <row r="64219" ht="12.8" customHeight="1" s="21"/>
-    <row r="64220" ht="12.8" customHeight="1" s="21"/>
-    <row r="64221" ht="12.8" customHeight="1" s="21"/>
-    <row r="64222" ht="12.8" customHeight="1" s="21"/>
-    <row r="64223" ht="12.8" customHeight="1" s="21"/>
-    <row r="64224" ht="12.8" customHeight="1" s="21"/>
-    <row r="64225" ht="12.8" customHeight="1" s="21"/>
-    <row r="64226" ht="12.8" customHeight="1" s="21"/>
-    <row r="64227" ht="12.8" customHeight="1" s="21"/>
-    <row r="64228" ht="12.8" customHeight="1" s="21"/>
-    <row r="64229" ht="12.8" customHeight="1" s="21"/>
-    <row r="64230" ht="12.8" customHeight="1" s="21"/>
-    <row r="64231" ht="12.8" customHeight="1" s="21"/>
-    <row r="64232" ht="12.8" customHeight="1" s="21"/>
-    <row r="64233" ht="12.8" customHeight="1" s="21"/>
-    <row r="64234" ht="12.8" customHeight="1" s="21"/>
-    <row r="64235" ht="12.8" customHeight="1" s="21"/>
-    <row r="64236" ht="12.8" customHeight="1" s="21"/>
-    <row r="64237" ht="12.8" customHeight="1" s="21"/>
-    <row r="64238" ht="12.8" customHeight="1" s="21"/>
-    <row r="64239" ht="12.8" customHeight="1" s="21"/>
-    <row r="64240" ht="12.8" customHeight="1" s="21"/>
-    <row r="64241" ht="12.8" customHeight="1" s="21"/>
-    <row r="64242" ht="12.8" customHeight="1" s="21"/>
-    <row r="64243" ht="12.8" customHeight="1" s="21"/>
-    <row r="64244" ht="12.8" customHeight="1" s="21"/>
-    <row r="64245" ht="12.8" customHeight="1" s="21"/>
-    <row r="64246" ht="12.8" customHeight="1" s="21"/>
-    <row r="64247" ht="12.8" customHeight="1" s="21"/>
-    <row r="64248" ht="12.8" customHeight="1" s="21"/>
-    <row r="64249" ht="12.8" customHeight="1" s="21"/>
-    <row r="64250" ht="12.8" customHeight="1" s="21"/>
-    <row r="64251" ht="12.8" customHeight="1" s="21"/>
-    <row r="64252" ht="12.8" customHeight="1" s="21"/>
-    <row r="64253" ht="12.8" customHeight="1" s="21"/>
-    <row r="64254" ht="12.8" customHeight="1" s="21"/>
-    <row r="64255" ht="12.8" customHeight="1" s="21"/>
-    <row r="64256" ht="12.8" customHeight="1" s="21"/>
-    <row r="64257" ht="12.8" customHeight="1" s="21"/>
-    <row r="64258" ht="12.8" customHeight="1" s="21"/>
-    <row r="64259" ht="12.8" customHeight="1" s="21"/>
-    <row r="64260" ht="12.8" customHeight="1" s="21"/>
-    <row r="64261" ht="12.8" customHeight="1" s="21"/>
-    <row r="64262" ht="12.8" customHeight="1" s="21"/>
-    <row r="64263" ht="12.8" customHeight="1" s="21"/>
-    <row r="64264" ht="12.8" customHeight="1" s="21"/>
-    <row r="64265" ht="12.8" customHeight="1" s="21"/>
-    <row r="64266" ht="12.8" customHeight="1" s="21"/>
-    <row r="64267" ht="12.8" customHeight="1" s="21"/>
-    <row r="64268" ht="12.8" customHeight="1" s="21"/>
-    <row r="64269" ht="12.8" customHeight="1" s="21"/>
-    <row r="64270" ht="12.8" customHeight="1" s="21"/>
-    <row r="64271" ht="12.8" customHeight="1" s="21"/>
-    <row r="64272" ht="12.8" customHeight="1" s="21"/>
-    <row r="64273" ht="12.8" customHeight="1" s="21"/>
-    <row r="64274" ht="12.8" customHeight="1" s="21"/>
-    <row r="64275" ht="12.8" customHeight="1" s="21"/>
-    <row r="64276" ht="12.8" customHeight="1" s="21"/>
-    <row r="64277" ht="12.8" customHeight="1" s="21"/>
-    <row r="64278" ht="12.8" customHeight="1" s="21"/>
-    <row r="64279" ht="12.8" customHeight="1" s="21"/>
-    <row r="64280" ht="12.8" customHeight="1" s="21"/>
-    <row r="64281" ht="12.8" customHeight="1" s="21"/>
-    <row r="64282" ht="12.8" customHeight="1" s="21"/>
-    <row r="64283" ht="12.8" customHeight="1" s="21"/>
-    <row r="64284" ht="12.8" customHeight="1" s="21"/>
-    <row r="64285" ht="12.8" customHeight="1" s="21"/>
-    <row r="64286" ht="12.8" customHeight="1" s="21"/>
-    <row r="64287" ht="12.8" customHeight="1" s="21"/>
-    <row r="64288" ht="12.8" customHeight="1" s="21"/>
-    <row r="64289" ht="12.8" customHeight="1" s="21"/>
-    <row r="64290" ht="12.8" customHeight="1" s="21"/>
-    <row r="64291" ht="12.8" customHeight="1" s="21"/>
-    <row r="64292" ht="12.8" customHeight="1" s="21"/>
-    <row r="64293" ht="12.8" customHeight="1" s="21"/>
-    <row r="64294" ht="12.8" customHeight="1" s="21"/>
-    <row r="64295" ht="12.8" customHeight="1" s="21"/>
-    <row r="64296" ht="12.8" customHeight="1" s="21"/>
-    <row r="64297" ht="12.8" customHeight="1" s="21"/>
-    <row r="64298" ht="12.8" customHeight="1" s="21"/>
-    <row r="64299" ht="12.8" customHeight="1" s="21"/>
-    <row r="64300" ht="12.8" customHeight="1" s="21"/>
-    <row r="64301" ht="12.8" customHeight="1" s="21"/>
-    <row r="64302" ht="12.8" customHeight="1" s="21"/>
-    <row r="64303" ht="12.8" customHeight="1" s="21"/>
-    <row r="64304" ht="12.8" customHeight="1" s="21"/>
-    <row r="64305" ht="12.8" customHeight="1" s="21"/>
-    <row r="64306" ht="12.8" customHeight="1" s="21"/>
-    <row r="64307" ht="12.8" customHeight="1" s="21"/>
-    <row r="64308" ht="12.8" customHeight="1" s="21"/>
-    <row r="64309" ht="12.8" customHeight="1" s="21"/>
-    <row r="64310" ht="12.8" customHeight="1" s="21"/>
-    <row r="64311" ht="12.8" customHeight="1" s="21"/>
-    <row r="64312" ht="12.8" customHeight="1" s="21"/>
-    <row r="64313" ht="12.8" customHeight="1" s="21"/>
-    <row r="64314" ht="12.8" customHeight="1" s="21"/>
-    <row r="64315" ht="12.8" customHeight="1" s="21"/>
-    <row r="64316" ht="12.8" customHeight="1" s="21"/>
-    <row r="64317" ht="12.8" customHeight="1" s="21"/>
-    <row r="64318" ht="12.8" customHeight="1" s="21"/>
-    <row r="64319" ht="12.8" customHeight="1" s="21"/>
-    <row r="64320" ht="12.8" customHeight="1" s="21"/>
-    <row r="64321" ht="12.8" customHeight="1" s="21"/>
-    <row r="64322" ht="12.8" customHeight="1" s="21"/>
-    <row r="64323" ht="12.8" customHeight="1" s="21"/>
-    <row r="64324" ht="12.8" customHeight="1" s="21"/>
-    <row r="64325" ht="12.8" customHeight="1" s="21"/>
-    <row r="64326" ht="12.8" customHeight="1" s="21"/>
-    <row r="64327" ht="12.8" customHeight="1" s="21"/>
-    <row r="64328" ht="12.8" customHeight="1" s="21"/>
-    <row r="64329" ht="12.8" customHeight="1" s="21"/>
-    <row r="64330" ht="12.8" customHeight="1" s="21"/>
-    <row r="64331" ht="12.8" customHeight="1" s="21"/>
-    <row r="64332" ht="12.8" customHeight="1" s="21"/>
-    <row r="64333" ht="12.8" customHeight="1" s="21"/>
-    <row r="64334" ht="12.8" customHeight="1" s="21"/>
-    <row r="64335" ht="12.8" customHeight="1" s="21"/>
-    <row r="64336" ht="12.8" customHeight="1" s="21"/>
-    <row r="64337" ht="12.8" customHeight="1" s="21"/>
-    <row r="64338" ht="12.8" customHeight="1" s="21"/>
-    <row r="64339" ht="12.8" customHeight="1" s="21"/>
-    <row r="64340" ht="12.8" customHeight="1" s="21"/>
-    <row r="64341" ht="12.8" customHeight="1" s="21"/>
-    <row r="64342" ht="12.8" customHeight="1" s="21"/>
-    <row r="64343" ht="12.8" customHeight="1" s="21"/>
-    <row r="64344" ht="12.8" customHeight="1" s="21"/>
-    <row r="64345" ht="12.8" customHeight="1" s="21"/>
-    <row r="64346" ht="12.8" customHeight="1" s="21"/>
-    <row r="64347" ht="12.8" customHeight="1" s="21"/>
-    <row r="64348" ht="12.8" customHeight="1" s="21"/>
-    <row r="64349" ht="12.8" customHeight="1" s="21"/>
-    <row r="64350" ht="12.8" customHeight="1" s="21"/>
-    <row r="64351" ht="12.8" customHeight="1" s="21"/>
-    <row r="64352" ht="12.8" customHeight="1" s="21"/>
-    <row r="64353" ht="12.8" customHeight="1" s="21"/>
-    <row r="64354" ht="12.8" customHeight="1" s="21"/>
-    <row r="64355" ht="12.8" customHeight="1" s="21"/>
-    <row r="64356" ht="12.8" customHeight="1" s="21"/>
-    <row r="64357" ht="12.8" customHeight="1" s="21"/>
-    <row r="64358" ht="12.8" customHeight="1" s="21"/>
-    <row r="64359" ht="12.8" customHeight="1" s="21"/>
-    <row r="64360" ht="12.8" customHeight="1" s="21"/>
-    <row r="64361" ht="12.8" customHeight="1" s="21"/>
-    <row r="64362" ht="12.8" customHeight="1" s="21"/>
-    <row r="64363" ht="12.8" customHeight="1" s="21"/>
-    <row r="64364" ht="12.8" customHeight="1" s="21"/>
-    <row r="64365" ht="12.8" customHeight="1" s="21"/>
-    <row r="64366" ht="12.8" customHeight="1" s="21"/>
-    <row r="64367" ht="12.8" customHeight="1" s="21"/>
-    <row r="64368" ht="12.8" customHeight="1" s="21"/>
-    <row r="64369" ht="12.8" customHeight="1" s="21"/>
-    <row r="64370" ht="12.8" customHeight="1" s="21"/>
-    <row r="64371" ht="12.8" customHeight="1" s="21"/>
-    <row r="64372" ht="12.8" customHeight="1" s="21"/>
-    <row r="64373" ht="12.8" customHeight="1" s="21"/>
-    <row r="64374" ht="12.8" customHeight="1" s="21"/>
-    <row r="64375" ht="12.8" customHeight="1" s="21"/>
-    <row r="64376" ht="12.8" customHeight="1" s="21"/>
-    <row r="64377" ht="12.8" customHeight="1" s="21"/>
-    <row r="64378" ht="12.8" customHeight="1" s="21"/>
-    <row r="64379" ht="12.8" customHeight="1" s="21"/>
-    <row r="64380" ht="12.8" customHeight="1" s="21"/>
-    <row r="64381" ht="12.8" customHeight="1" s="21"/>
-    <row r="64382" ht="12.8" customHeight="1" s="21"/>
-    <row r="64383" ht="12.8" customHeight="1" s="21"/>
-    <row r="64384" ht="12.8" customHeight="1" s="21"/>
-    <row r="64385" ht="12.8" customHeight="1" s="21"/>
-    <row r="64386" ht="12.8" customHeight="1" s="21"/>
-    <row r="64387" ht="12.8" customHeight="1" s="21"/>
-    <row r="64388" ht="12.8" customHeight="1" s="21"/>
-    <row r="64389" ht="12.8" customHeight="1" s="21"/>
-    <row r="64390" ht="12.8" customHeight="1" s="21"/>
-    <row r="64391" ht="12.8" customHeight="1" s="21"/>
-    <row r="64392" ht="12.8" customHeight="1" s="21"/>
-    <row r="64393" ht="12.8" customHeight="1" s="21"/>
-    <row r="64394" ht="12.8" customHeight="1" s="21"/>
-    <row r="64395" ht="12.8" customHeight="1" s="21"/>
-    <row r="64396" ht="12.8" customHeight="1" s="21"/>
-    <row r="64397" ht="12.8" customHeight="1" s="21"/>
-    <row r="64398" ht="12.8" customHeight="1" s="21"/>
-    <row r="64399" ht="12.8" customHeight="1" s="21"/>
-    <row r="64400" ht="12.8" customHeight="1" s="21"/>
-    <row r="64401" ht="12.8" customHeight="1" s="21"/>
-    <row r="64402" ht="12.8" customHeight="1" s="21"/>
-    <row r="64403" ht="12.8" customHeight="1" s="21"/>
-    <row r="64404" ht="12.8" customHeight="1" s="21"/>
-    <row r="64405" ht="12.8" customHeight="1" s="21"/>
-    <row r="64406" ht="12.8" customHeight="1" s="21"/>
-    <row r="64407" ht="12.8" customHeight="1" s="21"/>
-    <row r="64408" ht="12.8" customHeight="1" s="21"/>
-    <row r="64409" ht="12.8" customHeight="1" s="21"/>
-    <row r="64410" ht="12.8" customHeight="1" s="21"/>
-    <row r="64411" ht="12.8" customHeight="1" s="21"/>
-    <row r="64412" ht="12.8" customHeight="1" s="21"/>
-    <row r="64413" ht="12.8" customHeight="1" s="21"/>
-    <row r="64414" ht="12.8" customHeight="1" s="21"/>
-    <row r="64415" ht="12.8" customHeight="1" s="21"/>
-    <row r="64416" ht="12.8" customHeight="1" s="21"/>
-    <row r="64417" ht="12.8" customHeight="1" s="21"/>
-    <row r="64418" ht="12.8" customHeight="1" s="21"/>
-    <row r="64419" ht="12.8" customHeight="1" s="21"/>
-    <row r="64420" ht="12.8" customHeight="1" s="21"/>
-    <row r="64421" ht="12.8" customHeight="1" s="21"/>
-    <row r="64422" ht="12.8" customHeight="1" s="21"/>
-    <row r="64423" ht="12.8" customHeight="1" s="21"/>
-    <row r="64424" ht="12.8" customHeight="1" s="21"/>
-    <row r="64425" ht="12.8" customHeight="1" s="21"/>
-    <row r="64426" ht="12.8" customHeight="1" s="21"/>
-    <row r="64427" ht="12.8" customHeight="1" s="21"/>
-    <row r="64428" ht="12.8" customHeight="1" s="21"/>
-    <row r="64429" ht="12.8" customHeight="1" s="21"/>
-    <row r="64430" ht="12.8" customHeight="1" s="21"/>
-    <row r="64431" ht="12.8" customHeight="1" s="21"/>
-    <row r="64432" ht="12.8" customHeight="1" s="21"/>
-    <row r="64433" ht="12.8" customHeight="1" s="21"/>
-    <row r="64434" ht="12.8" customHeight="1" s="21"/>
-    <row r="64435" ht="12.8" customHeight="1" s="21"/>
-    <row r="64436" ht="12.8" customHeight="1" s="21"/>
-    <row r="64437" ht="12.8" customHeight="1" s="21"/>
-    <row r="64438" ht="12.8" customHeight="1" s="21"/>
-    <row r="64439" ht="12.8" customHeight="1" s="21"/>
-    <row r="64440" ht="12.8" customHeight="1" s="21"/>
-    <row r="64441" ht="12.8" customHeight="1" s="21"/>
-    <row r="64442" ht="12.8" customHeight="1" s="21"/>
-    <row r="64443" ht="12.8" customHeight="1" s="21"/>
-    <row r="64444" ht="12.8" customHeight="1" s="21"/>
-    <row r="64445" ht="12.8" customHeight="1" s="21"/>
-    <row r="64446" ht="12.8" customHeight="1" s="21"/>
-    <row r="64447" ht="12.8" customHeight="1" s="21"/>
-    <row r="64448" ht="12.8" customHeight="1" s="21"/>
-    <row r="64449" ht="12.8" customHeight="1" s="21"/>
-    <row r="64450" ht="12.8" customHeight="1" s="21"/>
-    <row r="64451" ht="12.8" customHeight="1" s="21"/>
-    <row r="64452" ht="12.8" customHeight="1" s="21"/>
-    <row r="64453" ht="12.8" customHeight="1" s="21"/>
-    <row r="64454" ht="12.8" customHeight="1" s="21"/>
-    <row r="64455" ht="12.8" customHeight="1" s="21"/>
-    <row r="64456" ht="12.8" customHeight="1" s="21"/>
-    <row r="64457" ht="12.8" customHeight="1" s="21"/>
-    <row r="64458" ht="12.8" customHeight="1" s="21"/>
-    <row r="64459" ht="12.8" customHeight="1" s="21"/>
-    <row r="64460" ht="12.8" customHeight="1" s="21"/>
-    <row r="64461" ht="12.8" customHeight="1" s="21"/>
-    <row r="64462" ht="12.8" customHeight="1" s="21"/>
-    <row r="64463" ht="12.8" customHeight="1" s="21"/>
-    <row r="64464" ht="12.8" customHeight="1" s="21"/>
-    <row r="64465" ht="12.8" customHeight="1" s="21"/>
-    <row r="64466" ht="12.8" customHeight="1" s="21"/>
-    <row r="64467" ht="12.8" customHeight="1" s="21"/>
-    <row r="64468" ht="12.8" customHeight="1" s="21"/>
-    <row r="64469" ht="12.8" customHeight="1" s="21"/>
-    <row r="64470" ht="12.8" customHeight="1" s="21"/>
-    <row r="64471" ht="12.8" customHeight="1" s="21"/>
-    <row r="64472" ht="12.8" customHeight="1" s="21"/>
-    <row r="64473" ht="12.8" customHeight="1" s="21"/>
-    <row r="64474" ht="12.8" customHeight="1" s="21"/>
-    <row r="64475" ht="12.8" customHeight="1" s="21"/>
-    <row r="64476" ht="12.8" customHeight="1" s="21"/>
-    <row r="64477" ht="12.8" customHeight="1" s="21"/>
-    <row r="64478" ht="12.8" customHeight="1" s="21"/>
-    <row r="64479" ht="12.8" customHeight="1" s="21"/>
-    <row r="64480" ht="12.8" customHeight="1" s="21"/>
-    <row r="64481" ht="12.8" customHeight="1" s="21"/>
-    <row r="64482" ht="12.8" customHeight="1" s="21"/>
-    <row r="64483" ht="12.8" customHeight="1" s="21"/>
-    <row r="64484" ht="12.8" customHeight="1" s="21"/>
-    <row r="64485" ht="12.8" customHeight="1" s="21"/>
-    <row r="64486" ht="12.8" customHeight="1" s="21"/>
-    <row r="64487" ht="12.8" customHeight="1" s="21"/>
-    <row r="64488" ht="12.8" customHeight="1" s="21"/>
-    <row r="64489" ht="12.8" customHeight="1" s="21"/>
-    <row r="64490" ht="12.8" customHeight="1" s="21"/>
-    <row r="64491" ht="12.8" customHeight="1" s="21"/>
-    <row r="64492" ht="12.8" customHeight="1" s="21"/>
-    <row r="64493" ht="12.8" customHeight="1" s="21"/>
-    <row r="64494" ht="12.8" customHeight="1" s="21"/>
-    <row r="64495" ht="12.8" customHeight="1" s="21"/>
-    <row r="64496" ht="12.8" customHeight="1" s="21"/>
-    <row r="64497" ht="12.8" customHeight="1" s="21"/>
-    <row r="64498" ht="12.8" customHeight="1" s="21"/>
-    <row r="64499" ht="12.8" customHeight="1" s="21"/>
-    <row r="64500" ht="12.8" customHeight="1" s="21"/>
-    <row r="64501" ht="12.8" customHeight="1" s="21"/>
-    <row r="64502" ht="12.8" customHeight="1" s="21"/>
-    <row r="64503" ht="12.8" customHeight="1" s="21"/>
-    <row r="64504" ht="12.8" customHeight="1" s="21"/>
-    <row r="64505" ht="12.8" customHeight="1" s="21"/>
-    <row r="64506" ht="12.8" customHeight="1" s="21"/>
-    <row r="64507" ht="12.8" customHeight="1" s="21"/>
-    <row r="64508" ht="12.8" customHeight="1" s="21"/>
-    <row r="64509" ht="12.8" customHeight="1" s="21"/>
-    <row r="64510" ht="12.8" customHeight="1" s="21"/>
-    <row r="64511" ht="12.8" customHeight="1" s="21"/>
-    <row r="64512" ht="12.8" customHeight="1" s="21"/>
-    <row r="64513" ht="12.8" customHeight="1" s="21"/>
-    <row r="64514" ht="12.8" customHeight="1" s="21"/>
-    <row r="64515" ht="12.8" customHeight="1" s="21"/>
-    <row r="64516" ht="12.8" customHeight="1" s="21"/>
-    <row r="64517" ht="12.8" customHeight="1" s="21"/>
-    <row r="64518" ht="12.8" customHeight="1" s="21"/>
-    <row r="64519" ht="12.8" customHeight="1" s="21"/>
-    <row r="64520" ht="12.8" customHeight="1" s="21"/>
-    <row r="64521" ht="12.8" customHeight="1" s="21"/>
-    <row r="64522" ht="12.8" customHeight="1" s="21"/>
-    <row r="64523" ht="12.8" customHeight="1" s="21"/>
-    <row r="64524" ht="12.8" customHeight="1" s="21"/>
-    <row r="64525" ht="12.8" customHeight="1" s="21"/>
-    <row r="64526" ht="12.8" customHeight="1" s="21"/>
-    <row r="64527" ht="12.8" customHeight="1" s="21"/>
-    <row r="64528" ht="12.8" customHeight="1" s="21"/>
-    <row r="64529" ht="12.8" customHeight="1" s="21"/>
-    <row r="64530" ht="12.8" customHeight="1" s="21"/>
-    <row r="64531" ht="12.8" customHeight="1" s="21"/>
-    <row r="64532" ht="12.8" customHeight="1" s="21"/>
-    <row r="64533" ht="12.8" customHeight="1" s="21"/>
-    <row r="64534" ht="12.8" customHeight="1" s="21"/>
-    <row r="64535" ht="12.8" customHeight="1" s="21"/>
-    <row r="64536" ht="12.8" customHeight="1" s="21"/>
-    <row r="64537" ht="12.8" customHeight="1" s="21"/>
-    <row r="64538" ht="12.8" customHeight="1" s="21"/>
-    <row r="64539" ht="12.8" customHeight="1" s="21"/>
-    <row r="64540" ht="12.8" customHeight="1" s="21"/>
-    <row r="64541" ht="12.8" customHeight="1" s="21"/>
-    <row r="64542" ht="12.8" customHeight="1" s="21"/>
-    <row r="64543" ht="12.8" customHeight="1" s="21"/>
-    <row r="64544" ht="12.8" customHeight="1" s="21"/>
-    <row r="64545" ht="12.8" customHeight="1" s="21"/>
-    <row r="64546" ht="12.8" customHeight="1" s="21"/>
-    <row r="64547" ht="12.8" customHeight="1" s="21"/>
-    <row r="64548" ht="12.8" customHeight="1" s="21"/>
-    <row r="64549" ht="12.8" customHeight="1" s="21"/>
-    <row r="64550" ht="12.8" customHeight="1" s="21"/>
-    <row r="64551" ht="12.8" customHeight="1" s="21"/>
-    <row r="64552" ht="12.8" customHeight="1" s="21"/>
-    <row r="64553" ht="12.8" customHeight="1" s="21"/>
-    <row r="64554" ht="12.8" customHeight="1" s="21"/>
-    <row r="64555" ht="12.8" customHeight="1" s="21"/>
-    <row r="64556" ht="12.8" customHeight="1" s="21"/>
-    <row r="64557" ht="12.8" customHeight="1" s="21"/>
-    <row r="64558" ht="12.8" customHeight="1" s="21"/>
-    <row r="64559" ht="12.8" customHeight="1" s="21"/>
-    <row r="64560" ht="12.8" customHeight="1" s="21"/>
-    <row r="64561" ht="12.8" customHeight="1" s="21"/>
-    <row r="64562" ht="12.8" customHeight="1" s="21"/>
-    <row r="64563" ht="12.8" customHeight="1" s="21"/>
-    <row r="64564" ht="12.8" customHeight="1" s="21"/>
-    <row r="64565" ht="12.8" customHeight="1" s="21"/>
-    <row r="64566" ht="12.8" customHeight="1" s="21"/>
-    <row r="64567" ht="12.8" customHeight="1" s="21"/>
-    <row r="64568" ht="12.8" customHeight="1" s="21"/>
-    <row r="64569" ht="12.8" customHeight="1" s="21"/>
-    <row r="64570" ht="12.8" customHeight="1" s="21"/>
-    <row r="64571" ht="12.8" customHeight="1" s="21"/>
-    <row r="64572" ht="12.8" customHeight="1" s="21"/>
-    <row r="64573" ht="12.8" customHeight="1" s="21"/>
-    <row r="64574" ht="12.8" customHeight="1" s="21"/>
-    <row r="64575" ht="12.8" customHeight="1" s="21"/>
-    <row r="64576" ht="12.8" customHeight="1" s="21"/>
-    <row r="64577" ht="12.8" customHeight="1" s="21"/>
-    <row r="64578" ht="12.8" customHeight="1" s="21"/>
-    <row r="64579" ht="12.8" customHeight="1" s="21"/>
-    <row r="64580" ht="12.8" customHeight="1" s="21"/>
-    <row r="64581" ht="12.8" customHeight="1" s="21"/>
-    <row r="64582" ht="12.8" customHeight="1" s="21"/>
-    <row r="64583" ht="12.8" customHeight="1" s="21"/>
-    <row r="64584" ht="12.8" customHeight="1" s="21"/>
-    <row r="64585" ht="12.8" customHeight="1" s="21"/>
-    <row r="64586" ht="12.8" customHeight="1" s="21"/>
-    <row r="64587" ht="12.8" customHeight="1" s="21"/>
-    <row r="64588" ht="12.8" customHeight="1" s="21"/>
-    <row r="64589" ht="12.8" customHeight="1" s="21"/>
-    <row r="64590" ht="12.8" customHeight="1" s="21"/>
-    <row r="64591" ht="12.8" customHeight="1" s="21"/>
-    <row r="64592" ht="12.8" customHeight="1" s="21"/>
-    <row r="64593" ht="12.8" customHeight="1" s="21"/>
-    <row r="64594" ht="12.8" customHeight="1" s="21"/>
-    <row r="64595" ht="12.8" customHeight="1" s="21"/>
-    <row r="64596" ht="12.8" customHeight="1" s="21"/>
-    <row r="64597" ht="12.8" customHeight="1" s="21"/>
-    <row r="64598" ht="12.8" customHeight="1" s="21"/>
-    <row r="64599" ht="12.8" customHeight="1" s="21"/>
-    <row r="64600" ht="12.8" customHeight="1" s="21"/>
-    <row r="64601" ht="12.8" customHeight="1" s="21"/>
-    <row r="64602" ht="12.8" customHeight="1" s="21"/>
-    <row r="64603" ht="12.8" customHeight="1" s="21"/>
-    <row r="64604" ht="12.8" customHeight="1" s="21"/>
-    <row r="64605" ht="12.8" customHeight="1" s="21"/>
-    <row r="64606" ht="12.8" customHeight="1" s="21"/>
-    <row r="64607" ht="12.8" customHeight="1" s="21"/>
-    <row r="64608" ht="12.8" customHeight="1" s="21"/>
-    <row r="64609" ht="12.8" customHeight="1" s="21"/>
-    <row r="64610" ht="12.8" customHeight="1" s="21"/>
-    <row r="64611" ht="12.8" customHeight="1" s="21"/>
-    <row r="64612" ht="12.8" customHeight="1" s="21"/>
-    <row r="64613" ht="12.8" customHeight="1" s="21"/>
-    <row r="64614" ht="12.8" customHeight="1" s="21"/>
-    <row r="64615" ht="12.8" customHeight="1" s="21"/>
-    <row r="64616" ht="12.8" customHeight="1" s="21"/>
-    <row r="64617" ht="12.8" customHeight="1" s="21"/>
-    <row r="64618" ht="12.8" customHeight="1" s="21"/>
-    <row r="64619" ht="12.8" customHeight="1" s="21"/>
-    <row r="64620" ht="12.8" customHeight="1" s="21"/>
-    <row r="64621" ht="12.8" customHeight="1" s="21"/>
-    <row r="64622" ht="12.8" customHeight="1" s="21"/>
-    <row r="64623" ht="12.8" customHeight="1" s="21"/>
-    <row r="64624" ht="12.8" customHeight="1" s="21"/>
-    <row r="64625" ht="12.8" customHeight="1" s="21"/>
-    <row r="64626" ht="12.8" customHeight="1" s="21"/>
-    <row r="64627" ht="12.8" customHeight="1" s="21"/>
-    <row r="64628" ht="12.8" customHeight="1" s="21"/>
-    <row r="64629" ht="12.8" customHeight="1" s="21"/>
-    <row r="64630" ht="12.8" customHeight="1" s="21"/>
-    <row r="64631" ht="12.8" customHeight="1" s="21"/>
-    <row r="64632" ht="12.8" customHeight="1" s="21"/>
-    <row r="64633" ht="12.8" customHeight="1" s="21"/>
-    <row r="64634" ht="12.8" customHeight="1" s="21"/>
-    <row r="64635" ht="12.8" customHeight="1" s="21"/>
-    <row r="64636" ht="12.8" customHeight="1" s="21"/>
-    <row r="64637" ht="12.8" customHeight="1" s="21"/>
-    <row r="64638" ht="12.8" customHeight="1" s="21"/>
-    <row r="64639" ht="12.8" customHeight="1" s="21"/>
-    <row r="64640" ht="12.8" customHeight="1" s="21"/>
-    <row r="64641" ht="12.8" customHeight="1" s="21"/>
-    <row r="64642" ht="12.8" customHeight="1" s="21"/>
-    <row r="64643" ht="12.8" customHeight="1" s="21"/>
-    <row r="64644" ht="12.8" customHeight="1" s="21"/>
-    <row r="64645" ht="12.8" customHeight="1" s="21"/>
-    <row r="64646" ht="12.8" customHeight="1" s="21"/>
-    <row r="64647" ht="12.8" customHeight="1" s="21"/>
-    <row r="64648" ht="12.8" customHeight="1" s="21"/>
-    <row r="64649" ht="12.8" customHeight="1" s="21"/>
-    <row r="64650" ht="12.8" customHeight="1" s="21"/>
-    <row r="64651" ht="12.8" customHeight="1" s="21"/>
-    <row r="64652" ht="12.8" customHeight="1" s="21"/>
-    <row r="64653" ht="12.8" customHeight="1" s="21"/>
-    <row r="64654" ht="12.8" customHeight="1" s="21"/>
-    <row r="64655" ht="12.8" customHeight="1" s="21"/>
-    <row r="64656" ht="12.8" customHeight="1" s="21"/>
-    <row r="64657" ht="12.8" customHeight="1" s="21"/>
-    <row r="64658" ht="12.8" customHeight="1" s="21"/>
-    <row r="64659" ht="12.8" customHeight="1" s="21"/>
-    <row r="64660" ht="12.8" customHeight="1" s="21"/>
-    <row r="64661" ht="12.8" customHeight="1" s="21"/>
-    <row r="64662" ht="12.8" customHeight="1" s="21"/>
-    <row r="64663" ht="12.8" customHeight="1" s="21"/>
-    <row r="64664" ht="12.8" customHeight="1" s="21"/>
-    <row r="64665" ht="12.8" customHeight="1" s="21"/>
-    <row r="64666" ht="12.8" customHeight="1" s="21"/>
-    <row r="64667" ht="12.8" customHeight="1" s="21"/>
-    <row r="64668" ht="12.8" customHeight="1" s="21"/>
-    <row r="64669" ht="12.8" customHeight="1" s="21"/>
-    <row r="64670" ht="12.8" customHeight="1" s="21"/>
-    <row r="64671" ht="12.8" customHeight="1" s="21"/>
-    <row r="64672" ht="12.8" customHeight="1" s="21"/>
-    <row r="64673" ht="12.8" customHeight="1" s="21"/>
-    <row r="64674" ht="12.8" customHeight="1" s="21"/>
-    <row r="64675" ht="12.8" customHeight="1" s="21"/>
-    <row r="64676" ht="12.8" customHeight="1" s="21"/>
-    <row r="64677" ht="12.8" customHeight="1" s="21"/>
-    <row r="64678" ht="12.8" customHeight="1" s="21"/>
-    <row r="64679" ht="12.8" customHeight="1" s="21"/>
-    <row r="64680" ht="12.8" customHeight="1" s="21"/>
-    <row r="64681" ht="12.8" customHeight="1" s="21"/>
-    <row r="64682" ht="12.8" customHeight="1" s="21"/>
-    <row r="64683" ht="12.8" customHeight="1" s="21"/>
-    <row r="64684" ht="12.8" customHeight="1" s="21"/>
-    <row r="64685" ht="12.8" customHeight="1" s="21"/>
-    <row r="64686" ht="12.8" customHeight="1" s="21"/>
-    <row r="64687" ht="12.8" customHeight="1" s="21"/>
-    <row r="64688" ht="12.8" customHeight="1" s="21"/>
-    <row r="64689" ht="12.8" customHeight="1" s="21"/>
-    <row r="64690" ht="12.8" customHeight="1" s="21"/>
-    <row r="64691" ht="12.8" customHeight="1" s="21"/>
-    <row r="64692" ht="12.8" customHeight="1" s="21"/>
-    <row r="64693" ht="12.8" customHeight="1" s="21"/>
-    <row r="64694" ht="12.8" customHeight="1" s="21"/>
-    <row r="64695" ht="12.8" customHeight="1" s="21"/>
-    <row r="64696" ht="12.8" customHeight="1" s="21"/>
-    <row r="64697" ht="12.8" customHeight="1" s="21"/>
-    <row r="64698" ht="12.8" customHeight="1" s="21"/>
-    <row r="64699" ht="12.8" customHeight="1" s="21"/>
-    <row r="64700" ht="12.8" customHeight="1" s="21"/>
-    <row r="64701" ht="12.8" customHeight="1" s="21"/>
-    <row r="64702" ht="12.8" customHeight="1" s="21"/>
-    <row r="64703" ht="12.8" customHeight="1" s="21"/>
-    <row r="64704" ht="12.8" customHeight="1" s="21"/>
-    <row r="64705" ht="12.8" customHeight="1" s="21"/>
-    <row r="64706" ht="12.8" customHeight="1" s="21"/>
-    <row r="64707" ht="12.8" customHeight="1" s="21"/>
-    <row r="64708" ht="12.8" customHeight="1" s="21"/>
-    <row r="64709" ht="12.8" customHeight="1" s="21"/>
-    <row r="64710" ht="12.8" customHeight="1" s="21"/>
-    <row r="64711" ht="12.8" customHeight="1" s="21"/>
-    <row r="64712" ht="12.8" customHeight="1" s="21"/>
-    <row r="64713" ht="12.8" customHeight="1" s="21"/>
-    <row r="64714" ht="12.8" customHeight="1" s="21"/>
-    <row r="64715" ht="12.8" customHeight="1" s="21"/>
-    <row r="64716" ht="12.8" customHeight="1" s="21"/>
-    <row r="64717" ht="12.8" customHeight="1" s="21"/>
-    <row r="64718" ht="12.8" customHeight="1" s="21"/>
-    <row r="64719" ht="12.8" customHeight="1" s="21"/>
-    <row r="64720" ht="12.8" customHeight="1" s="21"/>
-    <row r="64721" ht="12.8" customHeight="1" s="21"/>
-    <row r="64722" ht="12.8" customHeight="1" s="21"/>
-    <row r="64723" ht="12.8" customHeight="1" s="21"/>
-    <row r="64724" ht="12.8" customHeight="1" s="21"/>
-    <row r="64725" ht="12.8" customHeight="1" s="21"/>
-    <row r="64726" ht="12.8" customHeight="1" s="21"/>
-    <row r="64727" ht="12.8" customHeight="1" s="21"/>
-    <row r="64728" ht="12.8" customHeight="1" s="21"/>
-    <row r="64729" ht="12.8" customHeight="1" s="21"/>
-    <row r="64730" ht="12.8" customHeight="1" s="21"/>
-    <row r="64731" ht="12.8" customHeight="1" s="21"/>
-    <row r="64732" ht="12.8" customHeight="1" s="21"/>
-    <row r="64733" ht="12.8" customHeight="1" s="21"/>
-    <row r="64734" ht="12.8" customHeight="1" s="21"/>
-    <row r="64735" ht="12.8" customHeight="1" s="21"/>
-    <row r="64736" ht="12.8" customHeight="1" s="21"/>
-    <row r="64737" ht="12.8" customHeight="1" s="21"/>
-    <row r="64738" ht="12.8" customHeight="1" s="21"/>
-    <row r="64739" ht="12.8" customHeight="1" s="21"/>
-    <row r="64740" ht="12.8" customHeight="1" s="21"/>
-    <row r="64741" ht="12.8" customHeight="1" s="21"/>
-    <row r="64742" ht="12.8" customHeight="1" s="21"/>
-    <row r="64743" ht="12.8" customHeight="1" s="21"/>
-    <row r="64744" ht="12.8" customHeight="1" s="21"/>
-    <row r="64745" ht="12.8" customHeight="1" s="21"/>
-    <row r="64746" ht="12.8" customHeight="1" s="21"/>
-    <row r="64747" ht="12.8" customHeight="1" s="21"/>
-    <row r="64748" ht="12.8" customHeight="1" s="21"/>
-    <row r="64749" ht="12.8" customHeight="1" s="21"/>
-    <row r="64750" ht="12.8" customHeight="1" s="21"/>
-    <row r="64751" ht="12.8" customHeight="1" s="21"/>
-    <row r="64752" ht="12.8" customHeight="1" s="21"/>
-    <row r="64753" ht="12.8" customHeight="1" s="21"/>
-    <row r="64754" ht="12.8" customHeight="1" s="21"/>
-    <row r="64755" ht="12.8" customHeight="1" s="21"/>
-    <row r="64756" ht="12.8" customHeight="1" s="21"/>
-    <row r="64757" ht="12.8" customHeight="1" s="21"/>
-    <row r="64758" ht="12.8" customHeight="1" s="21"/>
-    <row r="64759" ht="12.8" customHeight="1" s="21"/>
-    <row r="64760" ht="12.8" customHeight="1" s="21"/>
-    <row r="64761" ht="12.8" customHeight="1" s="21"/>
-    <row r="64762" ht="12.8" customHeight="1" s="21"/>
-    <row r="64763" ht="12.8" customHeight="1" s="21"/>
-    <row r="64764" ht="12.8" customHeight="1" s="21"/>
-    <row r="64765" ht="12.8" customHeight="1" s="21"/>
-    <row r="64766" ht="12.8" customHeight="1" s="21"/>
-    <row r="64767" ht="12.8" customHeight="1" s="21"/>
-    <row r="64768" ht="12.8" customHeight="1" s="21"/>
-    <row r="64769" ht="12.8" customHeight="1" s="21"/>
-    <row r="64770" ht="12.8" customHeight="1" s="21"/>
-    <row r="64771" ht="12.8" customHeight="1" s="21"/>
-    <row r="64772" ht="12.8" customHeight="1" s="21"/>
-    <row r="64773" ht="12.8" customHeight="1" s="21"/>
-    <row r="64774" ht="12.8" customHeight="1" s="21"/>
-    <row r="64775" ht="12.8" customHeight="1" s="21"/>
-    <row r="64776" ht="12.8" customHeight="1" s="21"/>
-    <row r="64777" ht="12.8" customHeight="1" s="21"/>
-    <row r="64778" ht="12.8" customHeight="1" s="21"/>
-    <row r="64779" ht="12.8" customHeight="1" s="21"/>
-    <row r="64780" ht="12.8" customHeight="1" s="21"/>
-    <row r="64781" ht="12.8" customHeight="1" s="21"/>
-    <row r="64782" ht="12.8" customHeight="1" s="21"/>
-    <row r="64783" ht="12.8" customHeight="1" s="21"/>
-    <row r="64784" ht="12.8" customHeight="1" s="21"/>
-    <row r="64785" ht="12.8" customHeight="1" s="21"/>
-    <row r="64786" ht="12.8" customHeight="1" s="21"/>
-    <row r="64787" ht="12.8" customHeight="1" s="21"/>
-    <row r="64788" ht="12.8" customHeight="1" s="21"/>
-    <row r="64789" ht="12.8" customHeight="1" s="21"/>
-    <row r="64790" ht="12.8" customHeight="1" s="21"/>
-    <row r="64791" ht="12.8" customHeight="1" s="21"/>
-    <row r="64792" ht="12.8" customHeight="1" s="21"/>
-    <row r="64793" ht="12.8" customHeight="1" s="21"/>
-    <row r="64794" ht="12.8" customHeight="1" s="21"/>
-    <row r="64795" ht="12.8" customHeight="1" s="21"/>
-    <row r="64796" ht="12.8" customHeight="1" s="21"/>
-    <row r="64797" ht="12.8" customHeight="1" s="21"/>
-    <row r="64798" ht="12.8" customHeight="1" s="21"/>
-    <row r="64799" ht="12.8" customHeight="1" s="21"/>
-    <row r="64800" ht="12.8" customHeight="1" s="21"/>
-    <row r="64801" ht="12.8" customHeight="1" s="21"/>
-    <row r="64802" ht="12.8" customHeight="1" s="21"/>
-    <row r="64803" ht="12.8" customHeight="1" s="21"/>
-    <row r="64804" ht="12.8" customHeight="1" s="21"/>
-    <row r="64805" ht="12.8" customHeight="1" s="21"/>
-    <row r="64806" ht="12.8" customHeight="1" s="21"/>
-    <row r="64807" ht="12.8" customHeight="1" s="21"/>
-    <row r="64808" ht="12.8" customHeight="1" s="21"/>
-    <row r="64809" ht="12.8" customHeight="1" s="21"/>
-    <row r="64810" ht="12.8" customHeight="1" s="21"/>
-    <row r="64811" ht="12.8" customHeight="1" s="21"/>
-    <row r="64812" ht="12.8" customHeight="1" s="21"/>
-    <row r="64813" ht="12.8" customHeight="1" s="21"/>
-    <row r="64814" ht="12.8" customHeight="1" s="21"/>
-    <row r="64815" ht="12.8" customHeight="1" s="21"/>
-    <row r="64816" ht="12.8" customHeight="1" s="21"/>
-    <row r="64817" ht="12.8" customHeight="1" s="21"/>
-    <row r="64818" ht="12.8" customHeight="1" s="21"/>
-    <row r="64819" ht="12.8" customHeight="1" s="21"/>
-    <row r="64820" ht="12.8" customHeight="1" s="21"/>
-    <row r="64821" ht="12.8" customHeight="1" s="21"/>
-    <row r="64822" ht="12.8" customHeight="1" s="21"/>
-    <row r="64823" ht="12.8" customHeight="1" s="21"/>
-    <row r="64824" ht="12.8" customHeight="1" s="21"/>
-    <row r="64825" ht="12.8" customHeight="1" s="21"/>
-    <row r="64826" ht="12.8" customHeight="1" s="21"/>
-    <row r="64827" ht="12.8" customHeight="1" s="21"/>
-    <row r="64828" ht="12.8" customHeight="1" s="21"/>
-    <row r="64829" ht="12.8" customHeight="1" s="21"/>
-    <row r="64830" ht="12.8" customHeight="1" s="21"/>
-    <row r="64831" ht="12.8" customHeight="1" s="21"/>
-    <row r="64832" ht="12.8" customHeight="1" s="21"/>
-    <row r="64833" ht="12.8" customHeight="1" s="21"/>
-    <row r="64834" ht="12.8" customHeight="1" s="21"/>
-    <row r="64835" ht="12.8" customHeight="1" s="21"/>
-    <row r="64836" ht="12.8" customHeight="1" s="21"/>
-    <row r="64837" ht="12.8" customHeight="1" s="21"/>
-    <row r="64838" ht="12.8" customHeight="1" s="21"/>
-    <row r="64839" ht="12.8" customHeight="1" s="21"/>
-    <row r="64840" ht="12.8" customHeight="1" s="21"/>
-    <row r="64841" ht="12.8" customHeight="1" s="21"/>
-    <row r="64842" ht="12.8" customHeight="1" s="21"/>
-    <row r="64843" ht="12.8" customHeight="1" s="21"/>
-    <row r="64844" ht="12.8" customHeight="1" s="21"/>
-    <row r="64845" ht="12.8" customHeight="1" s="21"/>
-    <row r="64846" ht="12.8" customHeight="1" s="21"/>
-    <row r="64847" ht="12.8" customHeight="1" s="21"/>
-    <row r="64848" ht="12.8" customHeight="1" s="21"/>
-    <row r="64849" ht="12.8" customHeight="1" s="21"/>
-    <row r="64850" ht="12.8" customHeight="1" s="21"/>
-    <row r="64851" ht="12.8" customHeight="1" s="21"/>
-    <row r="64852" ht="12.8" customHeight="1" s="21"/>
-    <row r="64853" ht="12.8" customHeight="1" s="21"/>
-    <row r="64854" ht="12.8" customHeight="1" s="21"/>
-    <row r="64855" ht="12.8" customHeight="1" s="21"/>
-    <row r="64856" ht="12.8" customHeight="1" s="21"/>
-    <row r="64857" ht="12.8" customHeight="1" s="21"/>
-    <row r="64858" ht="12.8" customHeight="1" s="21"/>
-    <row r="64859" ht="12.8" customHeight="1" s="21"/>
-    <row r="64860" ht="12.8" customHeight="1" s="21"/>
-    <row r="64861" ht="12.8" customHeight="1" s="21"/>
-    <row r="64862" ht="12.8" customHeight="1" s="21"/>
-    <row r="64863" ht="12.8" customHeight="1" s="21"/>
-    <row r="64864" ht="12.8" customHeight="1" s="21"/>
-    <row r="64865" ht="12.8" customHeight="1" s="21"/>
-    <row r="64866" ht="12.8" customHeight="1" s="21"/>
-    <row r="64867" ht="12.8" customHeight="1" s="21"/>
-    <row r="64868" ht="12.8" customHeight="1" s="21"/>
-    <row r="64869" ht="12.8" customHeight="1" s="21"/>
-    <row r="64870" ht="12.8" customHeight="1" s="21"/>
-    <row r="64871" ht="12.8" customHeight="1" s="21"/>
-    <row r="64872" ht="12.8" customHeight="1" s="21"/>
-    <row r="64873" ht="12.8" customHeight="1" s="21"/>
-    <row r="64874" ht="12.8" customHeight="1" s="21"/>
-    <row r="64875" ht="12.8" customHeight="1" s="21"/>
-    <row r="64876" ht="12.8" customHeight="1" s="21"/>
-    <row r="64877" ht="12.8" customHeight="1" s="21"/>
-    <row r="64878" ht="12.8" customHeight="1" s="21"/>
-    <row r="64879" ht="12.8" customHeight="1" s="21"/>
-    <row r="64880" ht="12.8" customHeight="1" s="21"/>
-    <row r="64881" ht="12.8" customHeight="1" s="21"/>
-    <row r="64882" ht="12.8" customHeight="1" s="21"/>
-    <row r="64883" ht="12.8" customHeight="1" s="21"/>
-    <row r="64884" ht="12.8" customHeight="1" s="21"/>
-    <row r="64885" ht="12.8" customHeight="1" s="21"/>
-    <row r="64886" ht="12.8" customHeight="1" s="21"/>
-    <row r="64887" ht="12.8" customHeight="1" s="21"/>
-    <row r="64888" ht="12.8" customHeight="1" s="21"/>
-    <row r="64889" ht="12.8" customHeight="1" s="21"/>
-    <row r="64890" ht="12.8" customHeight="1" s="21"/>
-    <row r="64891" ht="12.8" customHeight="1" s="21"/>
-    <row r="64892" ht="12.8" customHeight="1" s="21"/>
-    <row r="64893" ht="12.8" customHeight="1" s="21"/>
-    <row r="64894" ht="12.8" customHeight="1" s="21"/>
-    <row r="64895" ht="12.8" customHeight="1" s="21"/>
-    <row r="64896" ht="12.8" customHeight="1" s="21"/>
-    <row r="64897" ht="12.8" customHeight="1" s="21"/>
-    <row r="64898" ht="12.8" customHeight="1" s="21"/>
-    <row r="64899" ht="12.8" customHeight="1" s="21"/>
-    <row r="64900" ht="12.8" customHeight="1" s="21"/>
-    <row r="64901" ht="12.8" customHeight="1" s="21"/>
-    <row r="64902" ht="12.8" customHeight="1" s="21"/>
-    <row r="64903" ht="12.8" customHeight="1" s="21"/>
-    <row r="64904" ht="12.8" customHeight="1" s="21"/>
-    <row r="64905" ht="12.8" customHeight="1" s="21"/>
-    <row r="64906" ht="12.8" customHeight="1" s="21"/>
-    <row r="64907" ht="12.8" customHeight="1" s="21"/>
-    <row r="64908" ht="12.8" customHeight="1" s="21"/>
-    <row r="64909" ht="12.8" customHeight="1" s="21"/>
-    <row r="64910" ht="12.8" customHeight="1" s="21"/>
-    <row r="64911" ht="12.8" customHeight="1" s="21"/>
-    <row r="64912" ht="12.8" customHeight="1" s="21"/>
-    <row r="64913" ht="12.8" customHeight="1" s="21"/>
-    <row r="64914" ht="12.8" customHeight="1" s="21"/>
-    <row r="64915" ht="12.8" customHeight="1" s="21"/>
-    <row r="64916" ht="12.8" customHeight="1" s="21"/>
-    <row r="64917" ht="12.8" customHeight="1" s="21"/>
-    <row r="64918" ht="12.8" customHeight="1" s="21"/>
-    <row r="64919" ht="12.8" customHeight="1" s="21"/>
-    <row r="64920" ht="12.8" customHeight="1" s="21"/>
-    <row r="64921" ht="12.8" customHeight="1" s="21"/>
-    <row r="64922" ht="12.8" customHeight="1" s="21"/>
-    <row r="64923" ht="12.8" customHeight="1" s="21"/>
-    <row r="64924" ht="12.8" customHeight="1" s="21"/>
-    <row r="64925" ht="12.8" customHeight="1" s="21"/>
-    <row r="64926" ht="12.8" customHeight="1" s="21"/>
-    <row r="64927" ht="12.8" customHeight="1" s="21"/>
-    <row r="64928" ht="12.8" customHeight="1" s="21"/>
-    <row r="64929" ht="12.8" customHeight="1" s="21"/>
-    <row r="64930" ht="12.8" customHeight="1" s="21"/>
-    <row r="64931" ht="12.8" customHeight="1" s="21"/>
-    <row r="64932" ht="12.8" customHeight="1" s="21"/>
-    <row r="64933" ht="12.8" customHeight="1" s="21"/>
-    <row r="64934" ht="12.8" customHeight="1" s="21"/>
-    <row r="64935" ht="12.8" customHeight="1" s="21"/>
-    <row r="64936" ht="12.8" customHeight="1" s="21"/>
-    <row r="64937" ht="12.8" customHeight="1" s="21"/>
-    <row r="64938" ht="12.8" customHeight="1" s="21"/>
-    <row r="64939" ht="12.8" customHeight="1" s="21"/>
-    <row r="64940" ht="12.8" customHeight="1" s="21"/>
-    <row r="64941" ht="12.8" customHeight="1" s="21"/>
-    <row r="64942" ht="12.8" customHeight="1" s="21"/>
-    <row r="64943" ht="12.8" customHeight="1" s="21"/>
-    <row r="64944" ht="12.8" customHeight="1" s="21"/>
-    <row r="64945" ht="12.8" customHeight="1" s="21"/>
-    <row r="64946" ht="12.8" customHeight="1" s="21"/>
-    <row r="64947" ht="12.8" customHeight="1" s="21"/>
-    <row r="64948" ht="12.8" customHeight="1" s="21"/>
-    <row r="64949" ht="12.8" customHeight="1" s="21"/>
-    <row r="64950" ht="12.8" customHeight="1" s="21"/>
-    <row r="64951" ht="12.8" customHeight="1" s="21"/>
-    <row r="64952" ht="12.8" customHeight="1" s="21"/>
-    <row r="64953" ht="12.8" customHeight="1" s="21"/>
-    <row r="64954" ht="12.8" customHeight="1" s="21"/>
-    <row r="64955" ht="12.8" customHeight="1" s="21"/>
-    <row r="64956" ht="12.8" customHeight="1" s="21"/>
-    <row r="64957" ht="12.8" customHeight="1" s="21"/>
-    <row r="64958" ht="12.8" customHeight="1" s="21"/>
-    <row r="64959" ht="12.8" customHeight="1" s="21"/>
-    <row r="64960" ht="12.8" customHeight="1" s="21"/>
-    <row r="64961" ht="12.8" customHeight="1" s="21"/>
-    <row r="64962" ht="12.8" customHeight="1" s="21"/>
-    <row r="64963" ht="12.8" customHeight="1" s="21"/>
-    <row r="64964" ht="12.8" customHeight="1" s="21"/>
-    <row r="64965" ht="12.8" customHeight="1" s="21"/>
-    <row r="64966" ht="12.8" customHeight="1" s="21"/>
-    <row r="64967" ht="12.8" customHeight="1" s="21"/>
-    <row r="64968" ht="12.8" customHeight="1" s="21"/>
-    <row r="64969" ht="12.8" customHeight="1" s="21"/>
-    <row r="64970" ht="12.8" customHeight="1" s="21"/>
-    <row r="64971" ht="12.8" customHeight="1" s="21"/>
-    <row r="64972" ht="12.8" customHeight="1" s="21"/>
-    <row r="64973" ht="12.8" customHeight="1" s="21"/>
-    <row r="64974" ht="12.8" customHeight="1" s="21"/>
-    <row r="64975" ht="12.8" customHeight="1" s="21"/>
-    <row r="64976" ht="12.8" customHeight="1" s="21"/>
-    <row r="64977" ht="12.8" customHeight="1" s="21"/>
-    <row r="64978" ht="12.8" customHeight="1" s="21"/>
-    <row r="64979" ht="12.8" customHeight="1" s="21"/>
-    <row r="64980" ht="12.8" customHeight="1" s="21"/>
-    <row r="64981" ht="12.8" customHeight="1" s="21"/>
-    <row r="64982" ht="12.8" customHeight="1" s="21"/>
-    <row r="64983" ht="12.8" customHeight="1" s="21"/>
-    <row r="64984" ht="12.8" customHeight="1" s="21"/>
-    <row r="64985" ht="12.8" customHeight="1" s="21"/>
-    <row r="64986" ht="12.8" customHeight="1" s="21"/>
-    <row r="64987" ht="12.8" customHeight="1" s="21"/>
-    <row r="64988" ht="12.8" customHeight="1" s="21"/>
-    <row r="64989" ht="12.8" customHeight="1" s="21"/>
-    <row r="64990" ht="12.8" customHeight="1" s="21"/>
-    <row r="64991" ht="12.8" customHeight="1" s="21"/>
-    <row r="64992" ht="12.8" customHeight="1" s="21"/>
-    <row r="64993" ht="12.8" customHeight="1" s="21"/>
-    <row r="64994" ht="12.8" customHeight="1" s="21"/>
-    <row r="64995" ht="12.8" customHeight="1" s="21"/>
-    <row r="64996" ht="12.8" customHeight="1" s="21"/>
-    <row r="64997" ht="12.8" customHeight="1" s="21"/>
-    <row r="64998" ht="12.8" customHeight="1" s="21"/>
-    <row r="64999" ht="12.8" customHeight="1" s="21"/>
-    <row r="65000" ht="12.8" customHeight="1" s="21"/>
-    <row r="65001" ht="12.8" customHeight="1" s="21"/>
-    <row r="65002" ht="12.8" customHeight="1" s="21"/>
-    <row r="65003" ht="12.8" customHeight="1" s="21"/>
-    <row r="65004" ht="12.8" customHeight="1" s="21"/>
-    <row r="65005" ht="12.8" customHeight="1" s="21"/>
-    <row r="65006" ht="12.8" customHeight="1" s="21"/>
-    <row r="65007" ht="12.8" customHeight="1" s="21"/>
-    <row r="65008" ht="12.8" customHeight="1" s="21"/>
-    <row r="65009" ht="12.8" customHeight="1" s="21"/>
-    <row r="65010" ht="12.8" customHeight="1" s="21"/>
-    <row r="65011" ht="12.8" customHeight="1" s="21"/>
-    <row r="65012" ht="12.8" customHeight="1" s="21"/>
-    <row r="65013" ht="12.8" customHeight="1" s="21"/>
-    <row r="65014" ht="12.8" customHeight="1" s="21"/>
-    <row r="65015" ht="12.8" customHeight="1" s="21"/>
-    <row r="65016" ht="12.8" customHeight="1" s="21"/>
-    <row r="65017" ht="12.8" customHeight="1" s="21"/>
-    <row r="65018" ht="12.8" customHeight="1" s="21"/>
-    <row r="65019" ht="12.8" customHeight="1" s="21"/>
-    <row r="65020" ht="12.8" customHeight="1" s="21"/>
-    <row r="65021" ht="12.8" customHeight="1" s="21"/>
-    <row r="65022" ht="12.8" customHeight="1" s="21"/>
-    <row r="65023" ht="12.8" customHeight="1" s="21"/>
-    <row r="65024" ht="12.8" customHeight="1" s="21"/>
-    <row r="65025" ht="12.8" customHeight="1" s="21"/>
-    <row r="65026" ht="12.8" customHeight="1" s="21"/>
-    <row r="65027" ht="12.8" customHeight="1" s="21"/>
-    <row r="65028" ht="12.8" customHeight="1" s="21"/>
-    <row r="65029" ht="12.8" customHeight="1" s="21"/>
-    <row r="65030" ht="12.8" customHeight="1" s="21"/>
-    <row r="65031" ht="12.8" customHeight="1" s="21"/>
-    <row r="65032" ht="12.8" customHeight="1" s="21"/>
-    <row r="65033" ht="12.8" customHeight="1" s="21"/>
-    <row r="65034" ht="12.8" customHeight="1" s="21"/>
-    <row r="65035" ht="12.8" customHeight="1" s="21"/>
-    <row r="65036" ht="12.8" customHeight="1" s="21"/>
-    <row r="65037" ht="12.8" customHeight="1" s="21"/>
-    <row r="65038" ht="12.8" customHeight="1" s="21"/>
-    <row r="65039" ht="12.8" customHeight="1" s="21"/>
-    <row r="65040" ht="12.8" customHeight="1" s="21"/>
-    <row r="65041" ht="12.8" customHeight="1" s="21"/>
-    <row r="65042" ht="12.8" customHeight="1" s="21"/>
-    <row r="65043" ht="12.8" customHeight="1" s="21"/>
-    <row r="65044" ht="12.8" customHeight="1" s="21"/>
-    <row r="65045" ht="12.8" customHeight="1" s="21"/>
-    <row r="65046" ht="12.8" customHeight="1" s="21"/>
-    <row r="65047" ht="12.8" customHeight="1" s="21"/>
-    <row r="65048" ht="12.8" customHeight="1" s="21"/>
-    <row r="65049" ht="12.8" customHeight="1" s="21"/>
-    <row r="65050" ht="12.8" customHeight="1" s="21"/>
-    <row r="65051" ht="12.8" customHeight="1" s="21"/>
-    <row r="65052" ht="12.8" customHeight="1" s="21"/>
-    <row r="65053" ht="12.8" customHeight="1" s="21"/>
-    <row r="65054" ht="12.8" customHeight="1" s="21"/>
-    <row r="65055" ht="12.8" customHeight="1" s="21"/>
-    <row r="65056" ht="12.8" customHeight="1" s="21"/>
-    <row r="65057" ht="12.8" customHeight="1" s="21"/>
-    <row r="65058" ht="12.8" customHeight="1" s="21"/>
-    <row r="65059" ht="12.8" customHeight="1" s="21"/>
-    <row r="65060" ht="12.8" customHeight="1" s="21"/>
-    <row r="65061" ht="12.8" customHeight="1" s="21"/>
-    <row r="65062" ht="12.8" customHeight="1" s="21"/>
-    <row r="65063" ht="12.8" customHeight="1" s="21"/>
-    <row r="65064" ht="12.8" customHeight="1" s="21"/>
-    <row r="65065" ht="12.8" customHeight="1" s="21"/>
-    <row r="65066" ht="12.8" customHeight="1" s="21"/>
-    <row r="65067" ht="12.8" customHeight="1" s="21"/>
-    <row r="65068" ht="12.8" customHeight="1" s="21"/>
-    <row r="65069" ht="12.8" customHeight="1" s="21"/>
-    <row r="65070" ht="12.8" customHeight="1" s="21"/>
-    <row r="65071" ht="12.8" customHeight="1" s="21"/>
-    <row r="65072" ht="12.8" customHeight="1" s="21"/>
-    <row r="65073" ht="12.8" customHeight="1" s="21"/>
-    <row r="65074" ht="12.8" customHeight="1" s="21"/>
-    <row r="65075" ht="12.8" customHeight="1" s="21"/>
-    <row r="65076" ht="12.8" customHeight="1" s="21"/>
-    <row r="65077" ht="12.8" customHeight="1" s="21"/>
-    <row r="65078" ht="12.8" customHeight="1" s="21"/>
-    <row r="65079" ht="12.8" customHeight="1" s="21"/>
-    <row r="65080" ht="12.8" customHeight="1" s="21"/>
-    <row r="65081" ht="12.8" customHeight="1" s="21"/>
-    <row r="65082" ht="12.8" customHeight="1" s="21"/>
-    <row r="65083" ht="12.8" customHeight="1" s="21"/>
-    <row r="65084" ht="12.8" customHeight="1" s="21"/>
-    <row r="65085" ht="12.8" customHeight="1" s="21"/>
-    <row r="65086" ht="12.8" customHeight="1" s="21"/>
-    <row r="65087" ht="12.8" customHeight="1" s="21"/>
-    <row r="65088" ht="12.8" customHeight="1" s="21"/>
-    <row r="65089" ht="12.8" customHeight="1" s="21"/>
-    <row r="65090" ht="12.8" customHeight="1" s="21"/>
-    <row r="65091" ht="12.8" customHeight="1" s="21"/>
-    <row r="65092" ht="12.8" customHeight="1" s="21"/>
-    <row r="65093" ht="12.8" customHeight="1" s="21"/>
-    <row r="65094" ht="12.8" customHeight="1" s="21"/>
-    <row r="65095" ht="12.8" customHeight="1" s="21"/>
-    <row r="65096" ht="12.8" customHeight="1" s="21"/>
-    <row r="65097" ht="12.8" customHeight="1" s="21"/>
-    <row r="65098" ht="12.8" customHeight="1" s="21"/>
-    <row r="65099" ht="12.8" customHeight="1" s="21"/>
-    <row r="65100" ht="12.8" customHeight="1" s="21"/>
-    <row r="65101" ht="12.8" customHeight="1" s="21"/>
-    <row r="65102" ht="12.8" customHeight="1" s="21"/>
-    <row r="65103" ht="12.8" customHeight="1" s="21"/>
-    <row r="65104" ht="12.8" customHeight="1" s="21"/>
-    <row r="65105" ht="12.8" customHeight="1" s="21"/>
-    <row r="65106" ht="12.8" customHeight="1" s="21"/>
-    <row r="65107" ht="12.8" customHeight="1" s="21"/>
-    <row r="65108" ht="12.8" customHeight="1" s="21"/>
-    <row r="65109" ht="12.8" customHeight="1" s="21"/>
-    <row r="65110" ht="12.8" customHeight="1" s="21"/>
-    <row r="65111" ht="12.8" customHeight="1" s="21"/>
-    <row r="65112" ht="12.8" customHeight="1" s="21"/>
-    <row r="65113" ht="12.8" customHeight="1" s="21"/>
-    <row r="65114" ht="12.8" customHeight="1" s="21"/>
-    <row r="65115" ht="12.8" customHeight="1" s="21"/>
-    <row r="65116" ht="12.8" customHeight="1" s="21"/>
-    <row r="65117" ht="12.8" customHeight="1" s="21"/>
-    <row r="65118" ht="12.8" customHeight="1" s="21"/>
-    <row r="65119" ht="12.8" customHeight="1" s="21"/>
-    <row r="65120" ht="12.8" customHeight="1" s="21"/>
-    <row r="65121" ht="12.8" customHeight="1" s="21"/>
-    <row r="65122" ht="12.8" customHeight="1" s="21"/>
-    <row r="65123" ht="12.8" customHeight="1" s="21"/>
-    <row r="65124" ht="12.8" customHeight="1" s="21"/>
-    <row r="65125" ht="12.8" customHeight="1" s="21"/>
-    <row r="65126" ht="12.8" customHeight="1" s="21"/>
-    <row r="65127" ht="12.8" customHeight="1" s="21"/>
-    <row r="65128" ht="12.8" customHeight="1" s="21"/>
-    <row r="65129" ht="12.8" customHeight="1" s="21"/>
-    <row r="65130" ht="12.8" customHeight="1" s="21"/>
-    <row r="65131" ht="12.8" customHeight="1" s="21"/>
-    <row r="65132" ht="12.8" customHeight="1" s="21"/>
-    <row r="65133" ht="12.8" customHeight="1" s="21"/>
-    <row r="65134" ht="12.8" customHeight="1" s="21"/>
-    <row r="65135" ht="12.8" customHeight="1" s="21"/>
-    <row r="65136" ht="12.8" customHeight="1" s="21"/>
-    <row r="65137" ht="12.8" customHeight="1" s="21"/>
-    <row r="65138" ht="12.8" customHeight="1" s="21"/>
-    <row r="65139" ht="12.8" customHeight="1" s="21"/>
-    <row r="65140" ht="12.8" customHeight="1" s="21"/>
-    <row r="65141" ht="12.8" customHeight="1" s="21"/>
-    <row r="65142" ht="12.8" customHeight="1" s="21"/>
-    <row r="65143" ht="12.8" customHeight="1" s="21"/>
-    <row r="65144" ht="12.8" customHeight="1" s="21"/>
-    <row r="65145" ht="12.8" customHeight="1" s="21"/>
-    <row r="65146" ht="12.8" customHeight="1" s="21"/>
-    <row r="65147" ht="12.8" customHeight="1" s="21"/>
-    <row r="65148" ht="12.8" customHeight="1" s="21"/>
-    <row r="65149" ht="12.8" customHeight="1" s="21"/>
-    <row r="65150" ht="12.8" customHeight="1" s="21"/>
-    <row r="65151" ht="12.8" customHeight="1" s="21"/>
-    <row r="65152" ht="12.8" customHeight="1" s="21"/>
-    <row r="65153" ht="12.8" customHeight="1" s="21"/>
-    <row r="65154" ht="12.8" customHeight="1" s="21"/>
-    <row r="65155" ht="12.8" customHeight="1" s="21"/>
-    <row r="65156" ht="12.8" customHeight="1" s="21"/>
-    <row r="65157" ht="12.8" customHeight="1" s="21"/>
-    <row r="65158" ht="12.8" customHeight="1" s="21"/>
-    <row r="65159" ht="12.8" customHeight="1" s="21"/>
-    <row r="65160" ht="12.8" customHeight="1" s="21"/>
-    <row r="65161" ht="12.8" customHeight="1" s="21"/>
-    <row r="65162" ht="12.8" customHeight="1" s="21"/>
-    <row r="65163" ht="12.8" customHeight="1" s="21"/>
-    <row r="65164" ht="12.8" customHeight="1" s="21"/>
-    <row r="65165" ht="12.8" customHeight="1" s="21"/>
-    <row r="65166" ht="12.8" customHeight="1" s="21"/>
-    <row r="65167" ht="12.8" customHeight="1" s="21"/>
-    <row r="65168" ht="12.8" customHeight="1" s="21"/>
-    <row r="65169" ht="12.8" customHeight="1" s="21"/>
-    <row r="65170" ht="12.8" customHeight="1" s="21"/>
-    <row r="65171" ht="12.8" customHeight="1" s="21"/>
-    <row r="65172" ht="12.8" customHeight="1" s="21"/>
-    <row r="65173" ht="12.8" customHeight="1" s="21"/>
-    <row r="65174" ht="12.8" customHeight="1" s="21"/>
-    <row r="65175" ht="12.8" customHeight="1" s="21"/>
-    <row r="65176" ht="12.8" customHeight="1" s="21"/>
-    <row r="65177" ht="12.8" customHeight="1" s="21"/>
-    <row r="65178" ht="12.8" customHeight="1" s="21"/>
-    <row r="65179" ht="12.8" customHeight="1" s="21"/>
-    <row r="65180" ht="12.8" customHeight="1" s="21"/>
-    <row r="65181" ht="12.8" customHeight="1" s="21"/>
-    <row r="65182" ht="12.8" customHeight="1" s="21"/>
-    <row r="65183" ht="12.8" customHeight="1" s="21"/>
-    <row r="65184" ht="12.8" customHeight="1" s="21"/>
-    <row r="65185" ht="12.8" customHeight="1" s="21"/>
-    <row r="65186" ht="12.8" customHeight="1" s="21"/>
-    <row r="65187" ht="12.8" customHeight="1" s="21"/>
-    <row r="65188" ht="12.8" customHeight="1" s="21"/>
-    <row r="65189" ht="12.8" customHeight="1" s="21"/>
-    <row r="65190" ht="12.8" customHeight="1" s="21"/>
-    <row r="65191" ht="12.8" customHeight="1" s="21"/>
-    <row r="65192" ht="12.8" customHeight="1" s="21"/>
-    <row r="65193" ht="12.8" customHeight="1" s="21"/>
-    <row r="65194" ht="12.8" customHeight="1" s="21"/>
-    <row r="65195" ht="12.8" customHeight="1" s="21"/>
-    <row r="65196" ht="12.8" customHeight="1" s="21"/>
-    <row r="65197" ht="12.8" customHeight="1" s="21"/>
-    <row r="65198" ht="12.8" customHeight="1" s="21"/>
-    <row r="65199" ht="12.8" customHeight="1" s="21"/>
-    <row r="65200" ht="12.8" customHeight="1" s="21"/>
-    <row r="65201" ht="12.8" customHeight="1" s="21"/>
-    <row r="65202" ht="12.8" customHeight="1" s="21"/>
-    <row r="65203" ht="12.8" customHeight="1" s="21"/>
-    <row r="65204" ht="12.8" customHeight="1" s="21"/>
-    <row r="65205" ht="12.8" customHeight="1" s="21"/>
-    <row r="65206" ht="12.8" customHeight="1" s="21"/>
-    <row r="65207" ht="12.8" customHeight="1" s="21"/>
-    <row r="65208" ht="12.8" customHeight="1" s="21"/>
-    <row r="65209" ht="12.8" customHeight="1" s="21"/>
-    <row r="65210" ht="12.8" customHeight="1" s="21"/>
-    <row r="65211" ht="12.8" customHeight="1" s="21"/>
-    <row r="65212" ht="12.8" customHeight="1" s="21"/>
-    <row r="65213" ht="12.8" customHeight="1" s="21"/>
-    <row r="65214" ht="12.8" customHeight="1" s="21"/>
-    <row r="65215" ht="12.8" customHeight="1" s="21"/>
-    <row r="65216" ht="12.8" customHeight="1" s="21"/>
-    <row r="65217" ht="12.8" customHeight="1" s="21"/>
-    <row r="65218" ht="12.8" customHeight="1" s="21"/>
-    <row r="65219" ht="12.8" customHeight="1" s="21"/>
-    <row r="65220" ht="12.8" customHeight="1" s="21"/>
-    <row r="65221" ht="12.8" customHeight="1" s="21"/>
-    <row r="65222" ht="12.8" customHeight="1" s="21"/>
-    <row r="65223" ht="12.8" customHeight="1" s="21"/>
-    <row r="65224" ht="12.8" customHeight="1" s="21"/>
-    <row r="65225" ht="12.8" customHeight="1" s="21"/>
-    <row r="65226" ht="12.8" customHeight="1" s="21"/>
-    <row r="65227" ht="12.8" customHeight="1" s="21"/>
-    <row r="65228" ht="12.8" customHeight="1" s="21"/>
-    <row r="65229" ht="12.8" customHeight="1" s="21"/>
-    <row r="65230" ht="12.8" customHeight="1" s="21"/>
-    <row r="65231" ht="12.8" customHeight="1" s="21"/>
-    <row r="65232" ht="12.8" customHeight="1" s="21"/>
-    <row r="65233" ht="12.8" customHeight="1" s="21"/>
-    <row r="65234" ht="12.8" customHeight="1" s="21"/>
-    <row r="65235" ht="12.8" customHeight="1" s="21"/>
-    <row r="65236" ht="12.8" customHeight="1" s="21"/>
-    <row r="65237" ht="12.8" customHeight="1" s="21"/>
-    <row r="65238" ht="12.8" customHeight="1" s="21"/>
-    <row r="65239" ht="12.8" customHeight="1" s="21"/>
-    <row r="65240" ht="12.8" customHeight="1" s="21"/>
-    <row r="65241" ht="12.8" customHeight="1" s="21"/>
-    <row r="65242" ht="12.8" customHeight="1" s="21"/>
-    <row r="65243" ht="12.8" customHeight="1" s="21"/>
-    <row r="65244" ht="12.8" customHeight="1" s="21"/>
-    <row r="65245" ht="12.8" customHeight="1" s="21"/>
-    <row r="65246" ht="12.8" customHeight="1" s="21"/>
-    <row r="65247" ht="12.8" customHeight="1" s="21"/>
-    <row r="65248" ht="12.8" customHeight="1" s="21"/>
-    <row r="65249" ht="12.8" customHeight="1" s="21"/>
-    <row r="65250" ht="12.8" customHeight="1" s="21"/>
-    <row r="65251" ht="12.8" customHeight="1" s="21"/>
-    <row r="65252" ht="12.8" customHeight="1" s="21"/>
-    <row r="65253" ht="12.8" customHeight="1" s="21"/>
-    <row r="65254" ht="12.8" customHeight="1" s="21"/>
-    <row r="65255" ht="12.8" customHeight="1" s="21"/>
-    <row r="65256" ht="12.8" customHeight="1" s="21"/>
-    <row r="65257" ht="12.8" customHeight="1" s="21"/>
-    <row r="65258" ht="12.8" customHeight="1" s="21"/>
-    <row r="65259" ht="12.8" customHeight="1" s="21"/>
-    <row r="65260" ht="12.8" customHeight="1" s="21"/>
-    <row r="65261" ht="12.8" customHeight="1" s="21"/>
-    <row r="65262" ht="12.8" customHeight="1" s="21"/>
-    <row r="65263" ht="12.8" customHeight="1" s="21"/>
-    <row r="65264" ht="12.8" customHeight="1" s="21"/>
-    <row r="65265" ht="12.8" customHeight="1" s="21"/>
-    <row r="65266" ht="12.8" customHeight="1" s="21"/>
-    <row r="65267" ht="12.8" customHeight="1" s="21"/>
-    <row r="65268" ht="12.8" customHeight="1" s="21"/>
-    <row r="65269" ht="12.8" customHeight="1" s="21"/>
-    <row r="65270" ht="12.8" customHeight="1" s="21"/>
-    <row r="65271" ht="12.8" customHeight="1" s="21"/>
-    <row r="65272" ht="12.8" customHeight="1" s="21"/>
-    <row r="65273" ht="12.8" customHeight="1" s="21"/>
-    <row r="65274" ht="12.8" customHeight="1" s="21"/>
-    <row r="65275" ht="12.8" customHeight="1" s="21"/>
-    <row r="65276" ht="12.8" customHeight="1" s="21"/>
-    <row r="65277" ht="12.8" customHeight="1" s="21"/>
-    <row r="65278" ht="12.8" customHeight="1" s="21"/>
-    <row r="65279" ht="12.8" customHeight="1" s="21"/>
-    <row r="65280" ht="12.8" customHeight="1" s="21"/>
-    <row r="65281" ht="12.8" customHeight="1" s="21"/>
-    <row r="65282" ht="12.8" customHeight="1" s="21"/>
-    <row r="65283" ht="12.8" customHeight="1" s="21"/>
-    <row r="65284" ht="12.8" customHeight="1" s="21"/>
-    <row r="65285" ht="12.8" customHeight="1" s="21"/>
-    <row r="65286" ht="12.8" customHeight="1" s="21"/>
-    <row r="65287" ht="12.8" customHeight="1" s="21"/>
-    <row r="65288" ht="12.8" customHeight="1" s="21"/>
-    <row r="65289" ht="12.8" customHeight="1" s="21"/>
-    <row r="65290" ht="12.8" customHeight="1" s="21"/>
-    <row r="65291" ht="12.8" customHeight="1" s="21"/>
-    <row r="65292" ht="12.8" customHeight="1" s="21"/>
-    <row r="65293" ht="12.8" customHeight="1" s="21"/>
-    <row r="65294" ht="12.8" customHeight="1" s="21"/>
-    <row r="65295" ht="12.8" customHeight="1" s="21"/>
-    <row r="65296" ht="12.8" customHeight="1" s="21"/>
-    <row r="65297" ht="12.8" customHeight="1" s="21"/>
-    <row r="65298" ht="12.8" customHeight="1" s="21"/>
-    <row r="65299" ht="12.8" customHeight="1" s="21"/>
-    <row r="65300" ht="12.8" customHeight="1" s="21"/>
-    <row r="65301" ht="12.8" customHeight="1" s="21"/>
-    <row r="65302" ht="12.8" customHeight="1" s="21"/>
-    <row r="65303" ht="12.8" customHeight="1" s="21"/>
-    <row r="65304" ht="12.8" customHeight="1" s="21"/>
-    <row r="65305" ht="12.8" customHeight="1" s="21"/>
-    <row r="65306" ht="12.8" customHeight="1" s="21"/>
-    <row r="65307" ht="12.8" customHeight="1" s="21"/>
-    <row r="65308" ht="12.8" customHeight="1" s="21"/>
-    <row r="65309" ht="12.8" customHeight="1" s="21"/>
-    <row r="65310" ht="12.8" customHeight="1" s="21"/>
-    <row r="65311" ht="12.8" customHeight="1" s="21"/>
-    <row r="65312" ht="12.8" customHeight="1" s="21"/>
-    <row r="65313" ht="12.8" customHeight="1" s="21"/>
-    <row r="65314" ht="12.8" customHeight="1" s="21"/>
-    <row r="65315" ht="12.8" customHeight="1" s="21"/>
-    <row r="65316" ht="12.8" customHeight="1" s="21"/>
-    <row r="65317" ht="12.8" customHeight="1" s="21"/>
-    <row r="65318" ht="12.8" customHeight="1" s="21"/>
-    <row r="65319" ht="12.8" customHeight="1" s="21"/>
-    <row r="65320" ht="12.8" customHeight="1" s="21"/>
-    <row r="65321" ht="12.8" customHeight="1" s="21"/>
-    <row r="65322" ht="12.8" customHeight="1" s="21"/>
-    <row r="65323" ht="12.8" customHeight="1" s="21"/>
-    <row r="65324" ht="12.8" customHeight="1" s="21"/>
-    <row r="65325" ht="12.8" customHeight="1" s="21"/>
-    <row r="65326" ht="12.8" customHeight="1" s="21"/>
-    <row r="65327" ht="12.8" customHeight="1" s="21"/>
-    <row r="65328" ht="12.8" customHeight="1" s="21"/>
-    <row r="65329" ht="12.8" customHeight="1" s="21"/>
-    <row r="65330" ht="12.8" customHeight="1" s="21"/>
-    <row r="65331" ht="12.8" customHeight="1" s="21"/>
-    <row r="65332" ht="12.8" customHeight="1" s="21"/>
-    <row r="65333" ht="12.8" customHeight="1" s="21"/>
-    <row r="65334" ht="12.8" customHeight="1" s="21"/>
-    <row r="65335" ht="12.8" customHeight="1" s="21"/>
-    <row r="65336" ht="12.8" customHeight="1" s="21"/>
-    <row r="65337" ht="12.8" customHeight="1" s="21"/>
-    <row r="65338" ht="12.8" customHeight="1" s="21"/>
-    <row r="65339" ht="12.8" customHeight="1" s="21"/>
-    <row r="65340" ht="12.8" customHeight="1" s="21"/>
-    <row r="65341" ht="12.8" customHeight="1" s="21"/>
-    <row r="65342" ht="12.8" customHeight="1" s="21"/>
-    <row r="65343" ht="12.8" customHeight="1" s="21"/>
-    <row r="65344" ht="12.8" customHeight="1" s="21"/>
-    <row r="65345" ht="12.8" customHeight="1" s="21"/>
-    <row r="65346" ht="12.8" customHeight="1" s="21"/>
-    <row r="65347" ht="12.8" customHeight="1" s="21"/>
-    <row r="65348" ht="12.8" customHeight="1" s="21"/>
-    <row r="65349" ht="12.8" customHeight="1" s="21"/>
-    <row r="65350" ht="12.8" customHeight="1" s="21"/>
-    <row r="65351" ht="12.8" customHeight="1" s="21"/>
-    <row r="65352" ht="12.8" customHeight="1" s="21"/>
-    <row r="65353" ht="12.8" customHeight="1" s="21"/>
-    <row r="65354" ht="12.8" customHeight="1" s="21"/>
-    <row r="65355" ht="12.8" customHeight="1" s="21"/>
-    <row r="65356" ht="12.8" customHeight="1" s="21"/>
-    <row r="65357" ht="12.8" customHeight="1" s="21"/>
-    <row r="65358" ht="12.8" customHeight="1" s="21"/>
-    <row r="65359" ht="12.8" customHeight="1" s="21"/>
-    <row r="65360" ht="12.8" customHeight="1" s="21"/>
-    <row r="65361" ht="12.8" customHeight="1" s="21"/>
-    <row r="65362" ht="12.8" customHeight="1" s="21"/>
-    <row r="65363" ht="12.8" customHeight="1" s="21"/>
-    <row r="65364" ht="12.8" customHeight="1" s="21"/>
-    <row r="65365" ht="12.8" customHeight="1" s="21"/>
-    <row r="65366" ht="12.8" customHeight="1" s="21"/>
-    <row r="65367" ht="12.8" customHeight="1" s="21"/>
-    <row r="65368" ht="12.8" customHeight="1" s="21"/>
-    <row r="65369" ht="12.8" customHeight="1" s="21"/>
-    <row r="65370" ht="12.8" customHeight="1" s="21"/>
-    <row r="65371" ht="12.8" customHeight="1" s="21"/>
-    <row r="65372" ht="12.8" customHeight="1" s="21"/>
-    <row r="65373" ht="12.8" customHeight="1" s="21"/>
-    <row r="65374" ht="12.8" customHeight="1" s="21"/>
-    <row r="65375" ht="12.8" customHeight="1" s="21"/>
-    <row r="65376" ht="12.8" customHeight="1" s="21"/>
-    <row r="65377" ht="12.8" customHeight="1" s="21"/>
-    <row r="65378" ht="12.8" customHeight="1" s="21"/>
-    <row r="65379" ht="12.8" customHeight="1" s="21"/>
-    <row r="65380" ht="12.8" customHeight="1" s="21"/>
-    <row r="65381" ht="12.8" customHeight="1" s="21"/>
-    <row r="65382" ht="12.8" customHeight="1" s="21"/>
-    <row r="65383" ht="12.8" customHeight="1" s="21"/>
-    <row r="65384" ht="12.8" customHeight="1" s="21"/>
-    <row r="65385" ht="12.8" customHeight="1" s="21"/>
-    <row r="65386" ht="12.8" customHeight="1" s="21"/>
-    <row r="65387" ht="12.8" customHeight="1" s="21"/>
-    <row r="65388" ht="12.8" customHeight="1" s="21"/>
-    <row r="65389" ht="12.8" customHeight="1" s="21"/>
-    <row r="65390" ht="12.8" customHeight="1" s="21"/>
-    <row r="65391" ht="12.8" customHeight="1" s="21"/>
-    <row r="65392" ht="12.8" customHeight="1" s="21"/>
-    <row r="65393" ht="12.8" customHeight="1" s="21"/>
-    <row r="65394" ht="12.8" customHeight="1" s="21"/>
-    <row r="65395" ht="12.8" customHeight="1" s="21"/>
-    <row r="65396" ht="12.8" customHeight="1" s="21"/>
-    <row r="65397" ht="12.8" customHeight="1" s="21"/>
-    <row r="65398" ht="12.8" customHeight="1" s="21"/>
-    <row r="65399" ht="12.8" customHeight="1" s="21"/>
-    <row r="65400" ht="12.8" customHeight="1" s="21"/>
-    <row r="65401" ht="12.8" customHeight="1" s="21"/>
-    <row r="65402" ht="12.8" customHeight="1" s="21"/>
-    <row r="65403" ht="12.8" customHeight="1" s="21"/>
-    <row r="65404" ht="12.8" customHeight="1" s="21"/>
-    <row r="65405" ht="12.8" customHeight="1" s="21"/>
-    <row r="65406" ht="12.8" customHeight="1" s="21"/>
-    <row r="65407" ht="12.8" customHeight="1" s="21"/>
-    <row r="65408" ht="12.8" customHeight="1" s="21"/>
-    <row r="65409" ht="12.8" customHeight="1" s="21"/>
-    <row r="65410" ht="12.8" customHeight="1" s="21"/>
-    <row r="65411" ht="12.8" customHeight="1" s="21"/>
-    <row r="65412" ht="12.8" customHeight="1" s="21"/>
-    <row r="65413" ht="12.8" customHeight="1" s="21"/>
-    <row r="65414" ht="12.8" customHeight="1" s="21"/>
-    <row r="65415" ht="12.8" customHeight="1" s="21"/>
-    <row r="65416" ht="12.8" customHeight="1" s="21"/>
-    <row r="65417" ht="12.8" customHeight="1" s="21"/>
-    <row r="65418" ht="12.8" customHeight="1" s="21"/>
-    <row r="65419" ht="12.8" customHeight="1" s="21"/>
-    <row r="65420" ht="12.8" customHeight="1" s="21"/>
-    <row r="65421" ht="12.8" customHeight="1" s="21"/>
-    <row r="65422" ht="12.8" customHeight="1" s="21"/>
-    <row r="65423" ht="12.8" customHeight="1" s="21"/>
-    <row r="65424" ht="12.8" customHeight="1" s="21"/>
-    <row r="65425" ht="12.8" customHeight="1" s="21"/>
-    <row r="65426" ht="12.8" customHeight="1" s="21"/>
-    <row r="65427" ht="12.8" customHeight="1" s="21"/>
-    <row r="65428" ht="12.8" customHeight="1" s="21"/>
-    <row r="65429" ht="12.8" customHeight="1" s="21"/>
-    <row r="65430" ht="12.8" customHeight="1" s="21"/>
-    <row r="65431" ht="12.8" customHeight="1" s="21"/>
-    <row r="65432" ht="12.8" customHeight="1" s="21"/>
-    <row r="65433" ht="12.8" customHeight="1" s="21"/>
-    <row r="65434" ht="12.8" customHeight="1" s="21"/>
-    <row r="65435" ht="12.8" customHeight="1" s="21"/>
-    <row r="65436" ht="12.8" customHeight="1" s="21"/>
-    <row r="65437" ht="12.8" customHeight="1" s="21"/>
-    <row r="65438" ht="12.8" customHeight="1" s="21"/>
-    <row r="65439" ht="12.8" customHeight="1" s="21"/>
-    <row r="65440" ht="12.8" customHeight="1" s="21"/>
-    <row r="65441" ht="12.8" customHeight="1" s="21"/>
-    <row r="65442" ht="12.8" customHeight="1" s="21"/>
-    <row r="65443" ht="12.8" customHeight="1" s="21"/>
-    <row r="65444" ht="12.8" customHeight="1" s="21"/>
-    <row r="65445" ht="12.8" customHeight="1" s="21"/>
-    <row r="65446" ht="12.8" customHeight="1" s="21"/>
-    <row r="65447" ht="12.8" customHeight="1" s="21"/>
-    <row r="65448" ht="12.8" customHeight="1" s="21"/>
-    <row r="65449" ht="12.8" customHeight="1" s="21"/>
-    <row r="65450" ht="12.8" customHeight="1" s="21"/>
-    <row r="65451" ht="12.8" customHeight="1" s="21"/>
-    <row r="65452" ht="12.8" customHeight="1" s="21"/>
-    <row r="65453" ht="12.8" customHeight="1" s="21"/>
-    <row r="65454" ht="12.8" customHeight="1" s="21"/>
-    <row r="65455" ht="12.8" customHeight="1" s="21"/>
-    <row r="65456" ht="12.8" customHeight="1" s="21"/>
-    <row r="65457" ht="12.8" customHeight="1" s="21"/>
-    <row r="65458" ht="12.8" customHeight="1" s="21"/>
-    <row r="65459" ht="12.8" customHeight="1" s="21"/>
-    <row r="65460" ht="12.8" customHeight="1" s="21"/>
-    <row r="65461" ht="12.8" customHeight="1" s="21"/>
-    <row r="65462" ht="12.8" customHeight="1" s="21"/>
-    <row r="65463" ht="12.8" customHeight="1" s="21"/>
-    <row r="65464" ht="12.8" customHeight="1" s="21"/>
-    <row r="65465" ht="12.8" customHeight="1" s="21"/>
-    <row r="65466" ht="12.8" customHeight="1" s="21"/>
-    <row r="65467" ht="12.8" customHeight="1" s="21"/>
-    <row r="65468" ht="12.8" customHeight="1" s="21"/>
-    <row r="65469" ht="12.8" customHeight="1" s="21"/>
-    <row r="65470" ht="12.8" customHeight="1" s="21"/>
-    <row r="65471" ht="12.8" customHeight="1" s="21"/>
-    <row r="65472" ht="12.8" customHeight="1" s="21"/>
-    <row r="65473" ht="12.8" customHeight="1" s="21"/>
-    <row r="65474" ht="12.8" customHeight="1" s="21"/>
-    <row r="65475" ht="12.8" customHeight="1" s="21"/>
-    <row r="65476" ht="12.8" customHeight="1" s="21"/>
-    <row r="65477" ht="12.8" customHeight="1" s="21"/>
-    <row r="65478" ht="12.8" customHeight="1" s="21"/>
-    <row r="65479" ht="12.8" customHeight="1" s="21"/>
-    <row r="65480" ht="12.8" customHeight="1" s="21"/>
-    <row r="65481" ht="12.8" customHeight="1" s="21"/>
-    <row r="65482" ht="12.8" customHeight="1" s="21"/>
-    <row r="65483" ht="12.8" customHeight="1" s="21"/>
-    <row r="65484" ht="12.8" customHeight="1" s="21"/>
-    <row r="65485" ht="12.8" customHeight="1" s="21"/>
-    <row r="65486" ht="12.8" customHeight="1" s="21"/>
-    <row r="65487" ht="12.8" customHeight="1" s="21"/>
-    <row r="65488" ht="12.8" customHeight="1" s="21"/>
-    <row r="65489" ht="12.8" customHeight="1" s="21"/>
-    <row r="65490" ht="12.8" customHeight="1" s="21"/>
-    <row r="65491" ht="12.8" customHeight="1" s="21"/>
-    <row r="65492" ht="12.8" customHeight="1" s="21"/>
-    <row r="65493" ht="12.8" customHeight="1" s="21"/>
-    <row r="65494" ht="12.8" customHeight="1" s="21"/>
-    <row r="65495" ht="12.8" customHeight="1" s="21"/>
-    <row r="65496" ht="12.8" customHeight="1" s="21"/>
-    <row r="65497" ht="12.8" customHeight="1" s="21"/>
-    <row r="65498" ht="12.8" customHeight="1" s="21"/>
-    <row r="65499" ht="12.8" customHeight="1" s="21"/>
-    <row r="65500" ht="12.8" customHeight="1" s="21"/>
-    <row r="65501" ht="12.8" customHeight="1" s="21"/>
-    <row r="65502" ht="12.8" customHeight="1" s="21"/>
-    <row r="65503" ht="12.8" customHeight="1" s="21"/>
-    <row r="65504" ht="12.8" customHeight="1" s="21"/>
-    <row r="65505" ht="12.8" customHeight="1" s="21"/>
-    <row r="65506" ht="12.8" customHeight="1" s="21"/>
-    <row r="65507" ht="12.8" customHeight="1" s="21"/>
-    <row r="65508" ht="12.8" customHeight="1" s="21"/>
-    <row r="65509" ht="12.8" customHeight="1" s="21"/>
-    <row r="65510" ht="12.8" customHeight="1" s="21"/>
-    <row r="65511" ht="12.8" customHeight="1" s="21"/>
-    <row r="65512" ht="12.8" customHeight="1" s="21"/>
-    <row r="65513" ht="12.8" customHeight="1" s="21"/>
-    <row r="65514" ht="12.8" customHeight="1" s="21"/>
-    <row r="65515" ht="12.8" customHeight="1" s="21"/>
-    <row r="65516" ht="12.8" customHeight="1" s="21"/>
-    <row r="65517" ht="12.8" customHeight="1" s="21"/>
-    <row r="65518" ht="12.8" customHeight="1" s="21"/>
-    <row r="65519" ht="12.8" customHeight="1" s="21"/>
-    <row r="65520" ht="12.8" customHeight="1" s="21"/>
-    <row r="65521" ht="12.8" customHeight="1" s="21"/>
-    <row r="65522" ht="12.8" customHeight="1" s="21"/>
-    <row r="65523" ht="12.8" customHeight="1" s="21"/>
-    <row r="65524" ht="12.8" customHeight="1" s="21"/>
-    <row r="65525" ht="12.8" customHeight="1" s="21"/>
-    <row r="65526" ht="12.8" customHeight="1" s="21"/>
-    <row r="65527" ht="12.8" customHeight="1" s="21"/>
-    <row r="65528" ht="12.8" customHeight="1" s="21"/>
-    <row r="65529" ht="12.8" customHeight="1" s="21"/>
-    <row r="65530" ht="12.8" customHeight="1" s="21"/>
-    <row r="65531" ht="12.8" customHeight="1" s="21"/>
-    <row r="65532" ht="12.8" customHeight="1" s="21"/>
-    <row r="65533" ht="12.8" customHeight="1" s="21"/>
-    <row r="65534" ht="12.8" customHeight="1" s="21"/>
-    <row r="65535" ht="12.8" customHeight="1" s="21"/>
     <row r="1048576" ht="12.8" customHeight="1" s="21"/>
   </sheetData>
   <printOptions horizontalCentered="1" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
@@ -9338,11 +7877,11 @@
   </sheetPr>
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="12.01953125" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.07421875" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="11.08" customWidth="1" style="18" min="6" max="6"/>
     <col width="11.52" customWidth="1" style="18" min="947" max="1024"/>
@@ -10380,7 +8919,7 @@
       <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData>
     <row r="1" ht="16.05" customHeight="1" s="21">
       <c r="A1" s="18" t="inlineStr">
@@ -10928,7 +9467,7 @@
       <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData>
     <row r="1" ht="16.05" customHeight="1" s="21">
       <c r="A1" s="18" t="inlineStr">
@@ -11476,7 +10015,7 @@
       <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData>
     <row r="1" ht="16.05" customHeight="1" s="21">
       <c r="A1" s="18" t="inlineStr">
@@ -12024,7 +10563,7 @@
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="11.31" customWidth="1" style="18" min="1" max="2"/>
     <col width="11.52" customWidth="1" style="18" min="998" max="1024"/>
@@ -12142,7 +10681,7 @@
       <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="11.31" customWidth="1" style="18" min="1" max="3"/>
     <col width="21.53" customWidth="1" style="18" min="4" max="4"/>

</xml_diff>

<commit_message>
feat(commands) : add the command cutsendmail to cut a file in multiple tabs which are eventually sent by mail to their owner.
</commit_message>
<xml_diff>
--- a/fichiers_xls/test.xlsx
+++ b/fichiers_xls/test.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="sheet1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Feuille2" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Feuille3" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Feuille4" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Feuille5" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Feuille5bis" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="color_line" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="cutinparts" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="cutinpartsbis" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="delete_lines" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="delete_lines_bis" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Feuille2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Feuille3" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Feuille4" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Feuille5" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Feuille5bis" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="color_line" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="cutinparts" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="cutinpartsbis" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="delete_lines" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="delete_lines_bis" sheetId="11" state="visible" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName name="_xlfn_T_TEST" hidden="0" function="0" vbProcedure="0">NA()</definedName>
@@ -361,14 +361,14 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0"/>
+          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:pPr>
               <a:defRPr sz="1400" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
@@ -401,8 +401,8 @@
       </layout>
       <overlay val="0"/>
       <spPr>
-        <a:noFill/>
-        <a:ln w="0">
+        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="0">
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
@@ -440,10 +440,10 @@
             </strRef>
           </tx>
           <spPr>
-            <a:solidFill>
+            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:srgbClr val="5b9bd5"/>
             </a:solidFill>
-            <a:ln w="0">
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="0">
               <a:noFill/>
               <a:prstDash val="solid"/>
             </a:ln>
@@ -451,9 +451,9 @@
           <invertIfNegative val="0"/>
           <dLbls>
             <txPr>
-              <a:bodyPr wrap="square"/>
-              <a:lstStyle/>
-              <a:p>
+              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square"/>
+              <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:pPr>
                   <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
@@ -606,7 +606,7 @@
         <minorTickMark val="none"/>
         <tickLblPos val="nextTo"/>
         <spPr>
-          <a:ln w="0">
+          <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="0">
             <a:solidFill>
               <a:srgbClr val="c0c0c0"/>
             </a:solidFill>
@@ -614,9 +614,9 @@
           </a:ln>
         </spPr>
         <txPr>
-          <a:bodyPr rot="-5400000"/>
-          <a:lstStyle/>
-          <a:p>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="-5400000"/>
+          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:pPr>
               <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
@@ -647,7 +647,7 @@
         <axPos val="l"/>
         <majorGridlines>
           <spPr>
-            <a:ln w="0">
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="0">
               <a:solidFill>
                 <a:srgbClr val="c0c0c0"/>
               </a:solidFill>
@@ -660,15 +660,15 @@
         <minorTickMark val="none"/>
         <tickLblPos val="nextTo"/>
         <spPr>
-          <a:ln w="0">
+          <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="0">
             <a:noFill/>
             <a:prstDash val="solid"/>
           </a:ln>
         </spPr>
         <txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:pPr>
               <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
@@ -691,10 +691,10 @@
     <dispBlanksAs val="gap"/>
   </chart>
   <spPr>
-    <a:solidFill>
+    <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
       <a:srgbClr val="ffffff"/>
     </a:solidFill>
-    <a:ln w="0">
+    <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="0">
       <a:solidFill>
         <a:srgbClr val="c0c0c0"/>
       </a:solidFill>
@@ -705,14 +705,14 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0"/>
+          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:pPr>
               <a:defRPr sz="1400" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
@@ -745,8 +745,8 @@
       </layout>
       <overlay val="0"/>
       <spPr>
-        <a:noFill/>
-        <a:ln w="0">
+        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="0">
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
@@ -784,10 +784,10 @@
             </strRef>
           </tx>
           <spPr>
-            <a:solidFill>
+            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:srgbClr val="5b9bd5"/>
             </a:solidFill>
-            <a:ln w="0">
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="0">
               <a:noFill/>
               <a:prstDash val="solid"/>
             </a:ln>
@@ -795,9 +795,9 @@
           <invertIfNegative val="0"/>
           <dLbls>
             <txPr>
-              <a:bodyPr wrap="square"/>
-              <a:lstStyle/>
-              <a:p>
+              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square"/>
+              <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:pPr>
                   <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
@@ -950,7 +950,7 @@
         <minorTickMark val="none"/>
         <tickLblPos val="nextTo"/>
         <spPr>
-          <a:ln w="0">
+          <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="0">
             <a:solidFill>
               <a:srgbClr val="c0c0c0"/>
             </a:solidFill>
@@ -958,9 +958,9 @@
           </a:ln>
         </spPr>
         <txPr>
-          <a:bodyPr rot="-5400000"/>
-          <a:lstStyle/>
-          <a:p>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="-5400000"/>
+          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:pPr>
               <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
@@ -991,7 +991,7 @@
         <axPos val="l"/>
         <majorGridlines>
           <spPr>
-            <a:ln w="0">
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="0">
               <a:solidFill>
                 <a:srgbClr val="c0c0c0"/>
               </a:solidFill>
@@ -1004,15 +1004,15 @@
         <minorTickMark val="none"/>
         <tickLblPos val="nextTo"/>
         <spPr>
-          <a:ln w="0">
+          <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="0">
             <a:noFill/>
             <a:prstDash val="solid"/>
           </a:ln>
         </spPr>
         <txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:pPr>
               <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
@@ -1035,10 +1035,10 @@
     <dispBlanksAs val="gap"/>
   </chart>
   <spPr>
-    <a:solidFill>
+    <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
       <a:srgbClr val="ffffff"/>
     </a:solidFill>
-    <a:ln w="0">
+    <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="0">
       <a:solidFill>
         <a:srgbClr val="c0c0c0"/>
       </a:solidFill>
@@ -1049,14 +1049,14 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0"/>
+          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:pPr>
               <a:defRPr sz="1400" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
@@ -1089,8 +1089,8 @@
       </layout>
       <overlay val="0"/>
       <spPr>
-        <a:noFill/>
-        <a:ln w="0">
+        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="0">
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
@@ -1129,10 +1129,10 @@
             </strRef>
           </tx>
           <spPr>
-            <a:solidFill>
+            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:srgbClr val="5b9bd5"/>
             </a:solidFill>
-            <a:ln w="0">
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="0">
               <a:noFill/>
               <a:prstDash val="solid"/>
             </a:ln>
@@ -1140,9 +1140,9 @@
           <invertIfNegative val="0"/>
           <dLbls>
             <txPr>
-              <a:bodyPr wrap="square"/>
-              <a:lstStyle/>
-              <a:p>
+              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square"/>
+              <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:pPr>
                   <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
@@ -1295,7 +1295,7 @@
         <minorTickMark val="none"/>
         <tickLblPos val="nextTo"/>
         <spPr>
-          <a:ln w="0">
+          <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="0">
             <a:solidFill>
               <a:srgbClr val="c0c0c0"/>
             </a:solidFill>
@@ -1303,9 +1303,9 @@
           </a:ln>
         </spPr>
         <txPr>
-          <a:bodyPr rot="-5400000"/>
-          <a:lstStyle/>
-          <a:p>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="-5400000"/>
+          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:pPr>
               <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
@@ -1336,7 +1336,7 @@
         <axPos val="l"/>
         <majorGridlines>
           <spPr>
-            <a:ln w="0">
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="0">
               <a:solidFill>
                 <a:srgbClr val="c0c0c0"/>
               </a:solidFill>
@@ -1349,15 +1349,15 @@
         <minorTickMark val="none"/>
         <tickLblPos val="nextTo"/>
         <spPr>
-          <a:ln w="0">
+          <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="0">
             <a:noFill/>
             <a:prstDash val="solid"/>
           </a:ln>
         </spPr>
         <txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:pPr>
               <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
@@ -1380,10 +1380,10 @@
     <dispBlanksAs val="gap"/>
   </chart>
   <spPr>
-    <a:solidFill>
+    <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
       <a:srgbClr val="ffffff"/>
     </a:solidFill>
-    <a:ln w="0">
+    <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="0">
       <a:solidFill>
         <a:srgbClr val="c0c0c0"/>
       </a:solidFill>
@@ -1394,14 +1394,14 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0"/>
+          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:pPr>
               <a:defRPr sz="1400" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
@@ -1434,8 +1434,8 @@
       </layout>
       <overlay val="0"/>
       <spPr>
-        <a:noFill/>
-        <a:ln w="0">
+        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="0">
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
@@ -1474,10 +1474,10 @@
             </strRef>
           </tx>
           <spPr>
-            <a:solidFill>
+            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:srgbClr val="5b9bd5"/>
             </a:solidFill>
-            <a:ln w="0">
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="0">
               <a:noFill/>
               <a:prstDash val="solid"/>
             </a:ln>
@@ -1485,9 +1485,9 @@
           <invertIfNegative val="0"/>
           <dLbls>
             <txPr>
-              <a:bodyPr wrap="square"/>
-              <a:lstStyle/>
-              <a:p>
+              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square"/>
+              <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:pPr>
                   <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
@@ -1640,7 +1640,7 @@
         <minorTickMark val="none"/>
         <tickLblPos val="nextTo"/>
         <spPr>
-          <a:ln w="0">
+          <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="0">
             <a:solidFill>
               <a:srgbClr val="c0c0c0"/>
             </a:solidFill>
@@ -1648,9 +1648,9 @@
           </a:ln>
         </spPr>
         <txPr>
-          <a:bodyPr rot="-5400000"/>
-          <a:lstStyle/>
-          <a:p>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="-5400000"/>
+          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:pPr>
               <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
@@ -1681,7 +1681,7 @@
         <axPos val="l"/>
         <majorGridlines>
           <spPr>
-            <a:ln w="0">
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="0">
               <a:solidFill>
                 <a:srgbClr val="c0c0c0"/>
               </a:solidFill>
@@ -1694,15 +1694,15 @@
         <minorTickMark val="none"/>
         <tickLblPos val="nextTo"/>
         <spPr>
-          <a:ln w="0">
+          <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="0">
             <a:noFill/>
             <a:prstDash val="solid"/>
           </a:ln>
         </spPr>
         <txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:pPr>
               <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
@@ -1725,10 +1725,10 @@
     <dispBlanksAs val="gap"/>
   </chart>
   <spPr>
-    <a:solidFill>
+    <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
       <a:srgbClr val="ffffff"/>
     </a:solidFill>
-    <a:ln w="0">
+    <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="0">
       <a:solidFill>
         <a:srgbClr val="c0c0c0"/>
       </a:solidFill>
@@ -1739,7 +1739,7 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <twoCellAnchor editAs="oneCell">
     <from>
       <col>99</col>
@@ -1759,9 +1759,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId1"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -1771,7 +1771,7 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <twoCellAnchor editAs="oneCell">
     <from>
       <col>94</col>
@@ -1791,9 +1791,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId1"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -1803,7 +1803,7 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <twoCellAnchor editAs="oneCell">
     <from>
       <col>101</col>
@@ -1823,9 +1823,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId1"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -1835,7 +1835,7 @@
 </file>
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <twoCellAnchor editAs="oneCell">
     <from>
       <col>101</col>
@@ -1855,9 +1855,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId1"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -2150,7 +2150,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr filterMode="0">
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
@@ -7163,7 +7163,7 @@
     <firstHeader/>
     <firstFooter/>
   </headerFooter>
-  <drawing r:id="rId1"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -8908,7 +8908,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr filterMode="0">
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
@@ -9451,12 +9451,12 @@
     <firstHeader/>
     <firstFooter/>
   </headerFooter>
-  <drawing r:id="rId1"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr filterMode="0">
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
@@ -9999,12 +9999,12 @@
     <firstHeader/>
     <firstFooter/>
   </headerFooter>
-  <drawing r:id="rId1"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr filterMode="0">
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
@@ -10547,7 +10547,7 @@
     <firstHeader/>
     <firstFooter/>
   </headerFooter>
-  <drawing r:id="rId1"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
feat(module_pour_excel, xlspython) : addition of file functions to merge the same cells on all files and to copy formulas from the first tab.
</commit_message>
<xml_diff>
--- a/fichiers_xls/test.xlsx
+++ b/fichiers_xls/test.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -395,8 +395,8 @@
           <yMode val="edge"/>
           <wMode val="factor"/>
           <hMode val="factor"/>
-          <x val="0.30458577090017"/>
-          <y val="0.0263457884737175"/>
+          <x val="0.304922118380062"/>
+          <y val="0.0272565922920892"/>
         </manualLayout>
       </layout>
       <overlay val="0"/>
@@ -415,10 +415,10 @@
           <yMode val="edge"/>
           <wMode val="factor"/>
           <hMode val="factor"/>
-          <x val="0.0128326099264012"/>
-          <y val="0.125142495250158"/>
-          <w val="0.965402277159213"/>
-          <h val="0.860291323622546"/>
+          <x val="0.0127102803738318"/>
+          <y val="0.12525354969574"/>
+          <w val="0.964922118380062"/>
+          <h val="0.859279918864097"/>
         </manualLayout>
       </layout>
       <barChart>
@@ -591,11 +591,11 @@
         </ser>
         <gapWidth val="219"/>
         <overlap val="-27"/>
-        <axId val="60210764"/>
-        <axId val="39655215"/>
+        <axId val="38660563"/>
+        <axId val="4767489"/>
       </barChart>
       <catAx>
-        <axId val="60210764"/>
+        <axId val="38660563"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
@@ -630,7 +630,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="39655215"/>
+        <crossAx val="4767489"/>
         <crossesAt val="0"/>
         <auto val="1"/>
         <lblAlgn val="ctr"/>
@@ -638,7 +638,7 @@
         <noMultiLvlLbl val="0"/>
       </catAx>
       <valAx>
-        <axId val="39655215"/>
+        <axId val="4767489"/>
         <scaling>
           <orientation val="minMax"/>
           <max val="100"/>
@@ -682,7 +682,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="60210764"/>
+        <crossAx val="38660563"/>
         <crossesAt val="1"/>
         <crossBetween val="midCat"/>
       </valAx>
@@ -739,8 +739,8 @@
           <yMode val="edge"/>
           <wMode val="factor"/>
           <hMode val="factor"/>
-          <x val="0.304590060145616"/>
-          <y val="0.0263457884737175"/>
+          <x val="0.304847419314329"/>
+          <y val="0.0272565922920892"/>
         </manualLayout>
       </layout>
       <overlay val="0"/>
@@ -759,10 +759,10 @@
           <yMode val="edge"/>
           <wMode val="factor"/>
           <hMode val="factor"/>
-          <x val="0.012852168407724"/>
-          <y val="0.125142495250158"/>
-          <w val="0.965115542893321"/>
-          <h val="0.860291323622546"/>
+          <x val="0.0127464523420821"/>
+          <y val="0.12525354969574"/>
+          <w val="0.964586211226925"/>
+          <h val="0.859279918864097"/>
         </manualLayout>
       </layout>
       <barChart>
@@ -935,11 +935,11 @@
         </ser>
         <gapWidth val="219"/>
         <overlap val="-27"/>
-        <axId val="16185274"/>
-        <axId val="62137394"/>
+        <axId val="98788891"/>
+        <axId val="3515034"/>
       </barChart>
       <catAx>
-        <axId val="16185274"/>
+        <axId val="98788891"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
@@ -974,7 +974,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="62137394"/>
+        <crossAx val="3515034"/>
         <crossesAt val="0"/>
         <auto val="1"/>
         <lblAlgn val="ctr"/>
@@ -982,7 +982,7 @@
         <noMultiLvlLbl val="0"/>
       </catAx>
       <valAx>
-        <axId val="62137394"/>
+        <axId val="3515034"/>
         <scaling>
           <orientation val="minMax"/>
           <max val="100"/>
@@ -1026,7 +1026,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="16185274"/>
+        <crossAx val="98788891"/>
         <crossesAt val="1"/>
         <crossBetween val="midCat"/>
       </valAx>
@@ -1083,8 +1083,8 @@
           <yMode val="edge"/>
           <wMode val="factor"/>
           <hMode val="factor"/>
-          <x val="0.304697391744746"/>
-          <y val="0.0264724509183027"/>
+          <x val="0.304973000125581"/>
+          <y val="0.0273833671399594"/>
         </manualLayout>
       </layout>
       <overlay val="0"/>
@@ -1104,10 +1104,10 @@
           <yMode val="edge"/>
           <wMode val="factor"/>
           <hMode val="factor"/>
-          <x val="0.0523550265890099"/>
-          <y val="0.145408486383787"/>
-          <w val="0.926373765510256"/>
-          <h val="0.819886003799873"/>
+          <x val="0.0523044078864749"/>
+          <y val="0.14553752535497"/>
+          <w val="0.926095692578174"/>
+          <h val="0.818838742393509"/>
         </manualLayout>
       </layout>
       <barChart>
@@ -1280,11 +1280,11 @@
         </ser>
         <gapWidth val="219"/>
         <overlap val="-27"/>
-        <axId val="42916953"/>
-        <axId val="10666216"/>
+        <axId val="82133774"/>
+        <axId val="91640293"/>
       </barChart>
       <catAx>
-        <axId val="42916953"/>
+        <axId val="82133774"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
@@ -1319,7 +1319,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="10666216"/>
+        <crossAx val="91640293"/>
         <crosses val="autoZero"/>
         <auto val="1"/>
         <lblAlgn val="ctr"/>
@@ -1327,7 +1327,7 @@
         <noMultiLvlLbl val="0"/>
       </catAx>
       <valAx>
-        <axId val="10666216"/>
+        <axId val="91640293"/>
         <scaling>
           <orientation val="minMax"/>
           <max val="100"/>
@@ -1371,7 +1371,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="42916953"/>
+        <crossAx val="82133774"/>
         <crossesAt val="1"/>
         <crossBetween val="midCat"/>
       </valAx>
@@ -1428,8 +1428,8 @@
           <yMode val="edge"/>
           <wMode val="factor"/>
           <hMode val="factor"/>
-          <x val="0.304760698911117"/>
-          <y val="0.0265991133628879"/>
+          <x val="0.305035790531207"/>
+          <y val="0.0275101419878296"/>
         </manualLayout>
       </layout>
       <overlay val="0"/>
@@ -1449,10 +1449,10 @@
           <yMode val="edge"/>
           <wMode val="factor"/>
           <hMode val="factor"/>
-          <x val="0.0523550265890099"/>
-          <y val="0.145408486383787"/>
-          <w val="0.926373765510256"/>
-          <h val="0.819886003799873"/>
+          <x val="0.0523044078864749"/>
+          <y val="0.14553752535497"/>
+          <w val="0.926095692578174"/>
+          <h val="0.818838742393509"/>
         </manualLayout>
       </layout>
       <barChart>
@@ -1625,11 +1625,11 @@
         </ser>
         <gapWidth val="219"/>
         <overlap val="-27"/>
-        <axId val="67993797"/>
-        <axId val="68842535"/>
+        <axId val="99313391"/>
+        <axId val="53093549"/>
       </barChart>
       <catAx>
-        <axId val="67993797"/>
+        <axId val="99313391"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
@@ -1664,7 +1664,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="68842535"/>
+        <crossAx val="53093549"/>
         <crosses val="autoZero"/>
         <auto val="1"/>
         <lblAlgn val="ctr"/>
@@ -1672,7 +1672,7 @@
         <noMultiLvlLbl val="0"/>
       </catAx>
       <valAx>
-        <axId val="68842535"/>
+        <axId val="53093549"/>
         <scaling>
           <orientation val="minMax"/>
           <max val="100"/>
@@ -1716,7 +1716,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="67993797"/>
+        <crossAx val="99313391"/>
         <crossesAt val="1"/>
         <crossBetween val="midCat"/>
       </valAx>
@@ -1749,9 +1749,9 @@
     </from>
     <to>
       <col>106</col>
-      <colOff>38520</colOff>
+      <colOff>36000</colOff>
       <row>30</row>
-      <rowOff>131040</rowOff>
+      <rowOff>128520</rowOff>
     </to>
     <graphicFrame>
       <nvGraphicFramePr>
@@ -1781,9 +1781,9 @@
     </from>
     <to>
       <col>100</col>
-      <colOff>689040</colOff>
+      <colOff>686520</colOff>
       <row>30</row>
-      <rowOff>130680</rowOff>
+      <rowOff>128160</rowOff>
     </to>
     <graphicFrame>
       <nvGraphicFramePr>
@@ -1813,9 +1813,9 @@
     </from>
     <to>
       <col>107</col>
-      <colOff>689040</colOff>
+      <colOff>686520</colOff>
       <row>30</row>
-      <rowOff>129960</rowOff>
+      <rowOff>127440</rowOff>
     </to>
     <graphicFrame>
       <nvGraphicFramePr>
@@ -1845,9 +1845,9 @@
     </from>
     <to>
       <col>107</col>
-      <colOff>689040</colOff>
+      <colOff>686520</colOff>
       <row>30</row>
-      <rowOff>129960</rowOff>
+      <rowOff>127440</rowOff>
     </to>
     <graphicFrame>
       <nvGraphicFramePr>
@@ -2157,11 +2157,11 @@
   </sheetPr>
   <dimension ref="A1:DJ14"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="J1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="J1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.54296875" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col width="16.2" customWidth="1" style="18" min="6" max="6"/>
     <col width="14.38" customWidth="1" style="19" min="7" max="7"/>
@@ -7175,11 +7175,11 @@
   </sheetPr>
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col width="11.54" customWidth="1" style="18" min="1" max="1024"/>
   </cols>
@@ -7504,6 +7504,10 @@
     </row>
     <row r="13" ht="12.8" customHeight="1" s="21"/>
     <row r="14" ht="12.8" customHeight="1" s="21"/>
+    <row r="15" ht="12.8" customHeight="1" s="21"/>
+    <row r="16" ht="12.8" customHeight="1" s="21"/>
+    <row r="17" ht="12.8" customHeight="1" s="21"/>
+    <row r="18" ht="12.8" customHeight="1" s="21"/>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -7528,10 +7532,10 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col width="11.54" customWidth="1" style="18" min="1" max="1024"/>
   </cols>
@@ -7881,7 +7885,7 @@
       <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="12.07421875" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.19140625" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col width="11.08" customWidth="1" style="18" min="6" max="6"/>
     <col width="11.52" customWidth="1" style="18" min="947" max="1024"/>
@@ -8115,7 +8119,7 @@
       <selection pane="topLeft" activeCell="I22" activeCellId="0" sqref="I22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col width="11.54" customWidth="1" style="18" min="1" max="1024"/>
   </cols>
@@ -8517,7 +8521,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col width="11.54" customWidth="1" style="18" min="1" max="1024"/>
   </cols>
@@ -8919,7 +8923,7 @@
       <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.95703125" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData>
     <row r="1" ht="16.05" customHeight="1" s="21">
       <c r="A1" s="18" t="inlineStr">
@@ -9467,7 +9471,7 @@
       <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.95703125" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData>
     <row r="1" ht="16.05" customHeight="1" s="21">
       <c r="A1" s="18" t="inlineStr">
@@ -10015,7 +10019,7 @@
       <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.95703125" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData>
     <row r="1" ht="16.05" customHeight="1" s="21">
       <c r="A1" s="18" t="inlineStr">
@@ -10563,7 +10567,7 @@
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col width="11.31" customWidth="1" style="18" min="1" max="2"/>
     <col width="11.52" customWidth="1" style="18" min="998" max="1024"/>
@@ -10681,7 +10685,7 @@
       <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col width="11.31" customWidth="1" style="18" min="1" max="3"/>
     <col width="21.53" customWidth="1" style="18" min="4" max="4"/>

</xml_diff>

<commit_message>
feat(utils,tests) : addition of methods to update the formula of cells when a row or a column is inserted or deleted
</commit_message>
<xml_diff>
--- a/fichiers_xls/test.xlsx
+++ b/fichiers_xls/test.xlsx
@@ -395,8 +395,8 @@
           <yMode val="edge"/>
           <wMode val="factor"/>
           <hMode val="factor"/>
-          <x val="0.304922118380062"/>
-          <y val="0.0272565922920892"/>
+          <x val="0.304962331112633"/>
+          <y val="0.0273868391023203"/>
         </manualLayout>
       </layout>
       <overlay val="0"/>
@@ -415,10 +415,10 @@
           <yMode val="edge"/>
           <wMode val="factor"/>
           <hMode val="factor"/>
-          <x val="0.0127102803738318"/>
-          <y val="0.12525354969574"/>
-          <w val="0.964922118380062"/>
-          <h val="0.859279918864097"/>
+          <x val="0.0127015752443808"/>
+          <y val="0.125269430708761"/>
+          <w val="0.964883880206712"/>
+          <h val="0.8591352859135289"/>
         </manualLayout>
       </layout>
       <barChart>
@@ -591,11 +591,11 @@
         </ser>
         <gapWidth val="219"/>
         <overlap val="-27"/>
-        <axId val="38660563"/>
-        <axId val="4767489"/>
+        <axId val="81793939"/>
+        <axId val="72976670"/>
       </barChart>
       <catAx>
-        <axId val="38660563"/>
+        <axId val="81793939"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
@@ -630,7 +630,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="4767489"/>
+        <crossAx val="72976670"/>
         <crossesAt val="0"/>
         <auto val="1"/>
         <lblAlgn val="ctr"/>
@@ -638,7 +638,7 @@
         <noMultiLvlLbl val="0"/>
       </catAx>
       <valAx>
-        <axId val="4767489"/>
+        <axId val="72976670"/>
         <scaling>
           <orientation val="minMax"/>
           <max val="100"/>
@@ -682,7 +682,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="38660563"/>
+        <crossAx val="81793939"/>
         <crossesAt val="1"/>
         <crossBetween val="midCat"/>
       </valAx>
@@ -739,8 +739,8 @@
           <yMode val="edge"/>
           <wMode val="factor"/>
           <hMode val="factor"/>
-          <x val="0.304847419314329"/>
-          <y val="0.0272565922920892"/>
+          <x val="0.304860457823769"/>
+          <y val="0.0273868391023203"/>
         </manualLayout>
       </layout>
       <overlay val="0"/>
@@ -759,10 +759,10 @@
           <yMode val="edge"/>
           <wMode val="factor"/>
           <hMode val="factor"/>
-          <x val="0.0127464523420821"/>
-          <y val="0.12525354969574"/>
-          <w val="0.964586211226925"/>
-          <h val="0.859279918864097"/>
+          <x val="0.0127312637190342"/>
+          <y val="0.125269430708761"/>
+          <w val="0.964502978990279"/>
+          <h val="0.8591352859135289"/>
         </manualLayout>
       </layout>
       <barChart>
@@ -935,11 +935,11 @@
         </ser>
         <gapWidth val="219"/>
         <overlap val="-27"/>
-        <axId val="98788891"/>
-        <axId val="3515034"/>
+        <axId val="80877132"/>
+        <axId val="52049170"/>
       </barChart>
       <catAx>
-        <axId val="98788891"/>
+        <axId val="80877132"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
@@ -974,7 +974,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="3515034"/>
+        <crossAx val="52049170"/>
         <crossesAt val="0"/>
         <auto val="1"/>
         <lblAlgn val="ctr"/>
@@ -982,7 +982,7 @@
         <noMultiLvlLbl val="0"/>
       </catAx>
       <valAx>
-        <axId val="3515034"/>
+        <axId val="52049170"/>
         <scaling>
           <orientation val="minMax"/>
           <max val="100"/>
@@ -1026,7 +1026,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="98788891"/>
+        <crossAx val="80877132"/>
         <crossesAt val="1"/>
         <crossBetween val="midCat"/>
       </valAx>
@@ -1083,8 +1083,8 @@
           <yMode val="edge"/>
           <wMode val="factor"/>
           <hMode val="factor"/>
-          <x val="0.304973000125581"/>
-          <y val="0.0273833671399594"/>
+          <x val="0.305029474476358"/>
+          <y val="0.0275136300240903"/>
         </manualLayout>
       </layout>
       <overlay val="0"/>
@@ -1104,10 +1104,10 @@
           <yMode val="edge"/>
           <wMode val="factor"/>
           <hMode val="factor"/>
-          <x val="0.0523044078864749"/>
-          <y val="0.14553752535497"/>
-          <w val="0.926095692578174"/>
-          <h val="0.818838742393509"/>
+          <x val="0.0523015176219742"/>
+          <y val="0.145555978191961"/>
+          <w val="0.926062962498432"/>
+          <h val="0.818688981868898"/>
         </manualLayout>
       </layout>
       <barChart>
@@ -1280,11 +1280,11 @@
         </ser>
         <gapWidth val="219"/>
         <overlap val="-27"/>
-        <axId val="82133774"/>
-        <axId val="91640293"/>
+        <axId val="89348863"/>
+        <axId val="82001105"/>
       </barChart>
       <catAx>
-        <axId val="82133774"/>
+        <axId val="89348863"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
@@ -1319,7 +1319,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="91640293"/>
+        <crossAx val="82001105"/>
         <crosses val="autoZero"/>
         <auto val="1"/>
         <lblAlgn val="ctr"/>
@@ -1327,7 +1327,7 @@
         <noMultiLvlLbl val="0"/>
       </catAx>
       <valAx>
-        <axId val="91640293"/>
+        <axId val="82001105"/>
         <scaling>
           <orientation val="minMax"/>
           <max val="100"/>
@@ -1371,7 +1371,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="82133774"/>
+        <crossAx val="89348863"/>
         <crossesAt val="1"/>
         <crossBetween val="midCat"/>
       </valAx>
@@ -1428,8 +1428,8 @@
           <yMode val="edge"/>
           <wMode val="factor"/>
           <hMode val="factor"/>
-          <x val="0.305035790531207"/>
-          <y val="0.0275101419878296"/>
+          <x val="0.305092186128183"/>
+          <y val="0.0276404209458603"/>
         </manualLayout>
       </layout>
       <overlay val="0"/>
@@ -1449,10 +1449,10 @@
           <yMode val="edge"/>
           <wMode val="factor"/>
           <hMode val="factor"/>
-          <x val="0.0523044078864749"/>
-          <y val="0.14553752535497"/>
-          <w val="0.926095692578174"/>
-          <h val="0.818838742393509"/>
+          <x val="0.0523015176219742"/>
+          <y val="0.145555978191961"/>
+          <w val="0.926062962498432"/>
+          <h val="0.818688981868898"/>
         </manualLayout>
       </layout>
       <barChart>
@@ -1625,11 +1625,11 @@
         </ser>
         <gapWidth val="219"/>
         <overlap val="-27"/>
-        <axId val="99313391"/>
-        <axId val="53093549"/>
+        <axId val="93897720"/>
+        <axId val="5572710"/>
       </barChart>
       <catAx>
-        <axId val="99313391"/>
+        <axId val="93897720"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
@@ -1664,7 +1664,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="53093549"/>
+        <crossAx val="5572710"/>
         <crosses val="autoZero"/>
         <auto val="1"/>
         <lblAlgn val="ctr"/>
@@ -1672,7 +1672,7 @@
         <noMultiLvlLbl val="0"/>
       </catAx>
       <valAx>
-        <axId val="53093549"/>
+        <axId val="5572710"/>
         <scaling>
           <orientation val="minMax"/>
           <max val="100"/>
@@ -1716,7 +1716,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="99313391"/>
+        <crossAx val="93897720"/>
         <crossesAt val="1"/>
         <crossBetween val="midCat"/>
       </valAx>
@@ -1749,9 +1749,9 @@
     </from>
     <to>
       <col>106</col>
-      <colOff>36000</colOff>
+      <colOff>35640</colOff>
       <row>30</row>
-      <rowOff>128520</rowOff>
+      <rowOff>128160</rowOff>
     </to>
     <graphicFrame>
       <nvGraphicFramePr>
@@ -1781,9 +1781,9 @@
     </from>
     <to>
       <col>100</col>
-      <colOff>686520</colOff>
+      <colOff>686160</colOff>
       <row>30</row>
-      <rowOff>128160</rowOff>
+      <rowOff>127800</rowOff>
     </to>
     <graphicFrame>
       <nvGraphicFramePr>
@@ -1813,9 +1813,9 @@
     </from>
     <to>
       <col>107</col>
-      <colOff>686520</colOff>
+      <colOff>686160</colOff>
       <row>30</row>
-      <rowOff>127440</rowOff>
+      <rowOff>127080</rowOff>
     </to>
     <graphicFrame>
       <nvGraphicFramePr>
@@ -1845,9 +1845,9 @@
     </from>
     <to>
       <col>107</col>
-      <colOff>686520</colOff>
+      <colOff>686160</colOff>
       <row>30</row>
-      <rowOff>127440</rowOff>
+      <rowOff>127080</rowOff>
     </to>
     <graphicFrame>
       <nvGraphicFramePr>
@@ -2161,7 +2161,7 @@
       <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col width="16.2" customWidth="1" style="18" min="6" max="6"/>
     <col width="14.38" customWidth="1" style="19" min="7" max="7"/>
@@ -7176,7 +7176,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7508,6 +7508,8 @@
     <row r="16" ht="12.8" customHeight="1" s="21"/>
     <row r="17" ht="12.8" customHeight="1" s="21"/>
     <row r="18" ht="12.8" customHeight="1" s="21"/>
+    <row r="19" ht="12.8" customHeight="1" s="21"/>
+    <row r="20" ht="12.8" customHeight="1" s="21"/>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -7885,7 +7887,7 @@
       <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="12.19140625" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.2109375" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col width="11.08" customWidth="1" style="18" min="6" max="6"/>
     <col width="11.52" customWidth="1" style="18" min="947" max="1024"/>
@@ -8923,7 +8925,7 @@
       <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.95703125" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.9765625" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData>
     <row r="1" ht="16.05" customHeight="1" s="21">
       <c r="A1" s="18" t="inlineStr">
@@ -9471,7 +9473,7 @@
       <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.95703125" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.9765625" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData>
     <row r="1" ht="16.05" customHeight="1" s="21">
       <c r="A1" s="18" t="inlineStr">
@@ -10019,7 +10021,7 @@
       <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.95703125" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.9765625" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData>
     <row r="1" ht="16.05" customHeight="1" s="21">
       <c r="A1" s="18" t="inlineStr">
@@ -10567,7 +10569,7 @@
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col width="11.31" customWidth="1" style="18" min="1" max="2"/>
     <col width="11.52" customWidth="1" style="18" min="998" max="1024"/>
@@ -10685,7 +10687,7 @@
       <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col width="11.31" customWidth="1" style="18" min="1" max="3"/>
     <col width="21.53" customWidth="1" style="18" min="4" max="4"/>

</xml_diff>

<commit_message>
factor(all): delete the label boolean, the columns must now be entered by their letters
</commit_message>
<xml_diff>
--- a/fichiers_xls/test.xlsx
+++ b/fichiers_xls/test.xlsx
@@ -8790,7 +8790,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
@@ -8824,6 +8824,16 @@
       </c>
       <c r="E1" s="18" t="inlineStr">
         <is>
+          <t>Prénom</t>
+        </is>
+      </c>
+      <c r="F1" s="18" t="inlineStr">
+        <is>
+          <t>Note/10,00</t>
+        </is>
+      </c>
+      <c r="G1" s="18" t="inlineStr">
+        <is>
           <t>Temps utilisé</t>
         </is>
       </c>
@@ -8849,7 +8859,17 @@
           <t>Terminé</t>
         </is>
       </c>
-      <c r="E2" s="23" t="inlineStr">
+      <c r="E2" s="18" t="inlineStr">
+        <is>
+          <t>Houzefa</t>
+        </is>
+      </c>
+      <c r="F2" s="18" t="inlineStr">
+        <is>
+          <t>7,83</t>
+        </is>
+      </c>
+      <c r="G2" s="23" t="inlineStr">
         <is>
           <t>5 min 49 s</t>
         </is>
@@ -8876,7 +8896,17 @@
           <t>Terminé</t>
         </is>
       </c>
-      <c r="E3" s="23" t="inlineStr">
+      <c r="E3" s="18" t="inlineStr">
+        <is>
+          <t>Yasmine</t>
+        </is>
+      </c>
+      <c r="F3" s="18" t="inlineStr">
+        <is>
+          <t>7,83</t>
+        </is>
+      </c>
+      <c r="G3" s="23" t="inlineStr">
         <is>
           <t>7 min 22 s</t>
         </is>
@@ -8903,7 +8933,17 @@
           <t>Terminé</t>
         </is>
       </c>
-      <c r="E4" s="23" t="inlineStr">
+      <c r="E4" s="18" t="inlineStr">
+        <is>
+          <t>Zina</t>
+        </is>
+      </c>
+      <c r="F4" s="18" t="inlineStr">
+        <is>
+          <t>7,28</t>
+        </is>
+      </c>
+      <c r="G4" s="23" t="inlineStr">
         <is>
           <t>5 min 15 s</t>
         </is>
@@ -8930,7 +8970,17 @@
           <t>Terminé</t>
         </is>
       </c>
-      <c r="E5" s="23" t="inlineStr">
+      <c r="E5" s="18" t="inlineStr">
+        <is>
+          <t>Aboubaker</t>
+        </is>
+      </c>
+      <c r="F5" s="18" t="inlineStr">
+        <is>
+          <t>7,98</t>
+        </is>
+      </c>
+      <c r="G5" s="23" t="inlineStr">
         <is>
           <t>7 min 57 s</t>
         </is>
@@ -8957,7 +9007,17 @@
           <t>Terminé</t>
         </is>
       </c>
-      <c r="E6" s="23" t="inlineStr">
+      <c r="E6" s="18" t="inlineStr">
+        <is>
+          <t>Yasmine</t>
+        </is>
+      </c>
+      <c r="F6" s="18" t="inlineStr">
+        <is>
+          <t>7,83</t>
+        </is>
+      </c>
+      <c r="G6" s="23" t="inlineStr">
         <is>
           <t>7 min 44 s</t>
         </is>
@@ -8984,7 +9044,17 @@
           <t>Terminé</t>
         </is>
       </c>
-      <c r="E7" s="26" t="inlineStr">
+      <c r="E7" s="18" t="inlineStr">
+        <is>
+          <t>Hassan Mahamat</t>
+        </is>
+      </c>
+      <c r="F7" s="18" t="inlineStr">
+        <is>
+          <t>7,52</t>
+        </is>
+      </c>
+      <c r="G7" s="26" t="inlineStr">
         <is>
           <t>23 min 37 s</t>
         </is>
@@ -9011,7 +9081,17 @@
           <t>Terminé</t>
         </is>
       </c>
-      <c r="E8" s="23" t="inlineStr">
+      <c r="E8" s="18" t="inlineStr">
+        <is>
+          <t>Yacine</t>
+        </is>
+      </c>
+      <c r="F8" s="18" t="inlineStr">
+        <is>
+          <t>8,07</t>
+        </is>
+      </c>
+      <c r="G8" s="23" t="inlineStr">
         <is>
           <t>4 min 17 s</t>
         </is>
@@ -9038,7 +9118,17 @@
           <t>Terminé</t>
         </is>
       </c>
-      <c r="E9" s="23" t="inlineStr">
+      <c r="E9" s="18" t="inlineStr">
+        <is>
+          <t>Paola</t>
+        </is>
+      </c>
+      <c r="F9" s="18" t="inlineStr">
+        <is>
+          <t>7,16</t>
+        </is>
+      </c>
+      <c r="G9" s="23" t="inlineStr">
         <is>
           <t>8 min 33 s</t>
         </is>
@@ -9065,7 +9155,17 @@
           <t>Terminé</t>
         </is>
       </c>
-      <c r="E10" s="23" t="inlineStr">
+      <c r="E10" s="35" t="inlineStr">
+        <is>
+          <t>Rodolphe</t>
+        </is>
+      </c>
+      <c r="F10" s="18" t="inlineStr">
+        <is>
+          <t>8,88</t>
+        </is>
+      </c>
+      <c r="G10" s="23" t="inlineStr">
         <is>
           <t>15 min 32 s</t>
         </is>
@@ -9092,7 +9192,17 @@
           <t>Terminé</t>
         </is>
       </c>
-      <c r="E11" s="23" t="inlineStr">
+      <c r="E11" s="18" t="inlineStr">
+        <is>
+          <t>Nouh</t>
+        </is>
+      </c>
+      <c r="F11" s="18" t="inlineStr">
+        <is>
+          <t>7,35</t>
+        </is>
+      </c>
+      <c r="G11" s="23" t="inlineStr">
         <is>
           <t>9 min 27 s</t>
         </is>
@@ -9119,7 +9229,17 @@
           <t>Terminé</t>
         </is>
       </c>
-      <c r="E12" s="23" t="inlineStr">
+      <c r="E12" s="18" t="inlineStr">
+        <is>
+          <t>Iness</t>
+        </is>
+      </c>
+      <c r="F12" s="18" t="inlineStr">
+        <is>
+          <t>6,51</t>
+        </is>
+      </c>
+      <c r="G12" s="23" t="inlineStr">
         <is>
           <t>10 min 33 s</t>
         </is>
@@ -9146,7 +9266,17 @@
           <t>Terminé</t>
         </is>
       </c>
-      <c r="E13" s="23" t="inlineStr">
+      <c r="E13" s="18" t="inlineStr">
+        <is>
+          <t>Zakaria</t>
+        </is>
+      </c>
+      <c r="F13" s="18" t="inlineStr">
+        <is>
+          <t>7,70</t>
+        </is>
+      </c>
+      <c r="G13" s="23" t="inlineStr">
         <is>
           <t>9 min 14 s</t>
         </is>
@@ -9173,7 +9303,17 @@
           <t>Terminé</t>
         </is>
       </c>
-      <c r="E14" s="26" t="inlineStr">
+      <c r="E14" s="35" t="inlineStr">
+        <is>
+          <t>Christian</t>
+        </is>
+      </c>
+      <c r="F14" s="18" t="inlineStr">
+        <is>
+          <t>6,72</t>
+        </is>
+      </c>
+      <c r="G14" s="26" t="inlineStr">
         <is>
           <t>21 min 49 s</t>
         </is>

</xml_diff>

<commit_message>
feat(module_pour_excel, xlspython): change colgetbegin in colgetpart
</commit_message>
<xml_diff>
--- a/fichiers_xls/test.xlsx
+++ b/fichiers_xls/test.xlsx
@@ -91,7 +91,7 @@
       <sz val="11"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill/>
     </fill>
@@ -163,6 +163,11 @@
         <fgColor rgb="00ff2112"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0000a933"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -183,7 +188,7 @@
     <xf numFmtId="42" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
@@ -300,6 +305,10 @@
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -477,7 +486,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:t/>
+                  <a:t>None</a:t>
                 </a:r>
               </a:p>
             </txPr>
@@ -640,7 +649,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
           </a:p>
         </txPr>
@@ -692,7 +701,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
           </a:p>
         </txPr>
@@ -821,7 +830,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:t/>
+                  <a:t>None</a:t>
                 </a:r>
               </a:p>
             </txPr>
@@ -984,7 +993,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
           </a:p>
         </txPr>
@@ -1036,7 +1045,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
           </a:p>
         </txPr>
@@ -1166,7 +1175,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:t/>
+                  <a:t>None</a:t>
                 </a:r>
               </a:p>
             </txPr>
@@ -1329,7 +1338,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
           </a:p>
         </txPr>
@@ -1381,7 +1390,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
           </a:p>
         </txPr>
@@ -1511,7 +1520,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:t/>
+                  <a:t>None</a:t>
                 </a:r>
               </a:p>
             </txPr>
@@ -1674,7 +1683,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
           </a:p>
         </txPr>
@@ -1726,7 +1735,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
           </a:p>
         </txPr>
@@ -10101,37 +10110,37 @@
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1" s="22">
-      <c r="A4" s="36" t="inlineStr">
+      <c r="A4" s="41" t="inlineStr">
         <is>
           <t>Abbas</t>
         </is>
       </c>
-      <c r="B4" s="36" t="inlineStr">
+      <c r="B4" s="41" t="inlineStr">
         <is>
           <t>Zina</t>
         </is>
       </c>
-      <c r="C4" s="36" t="inlineStr">
+      <c r="C4" s="41" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="D4" s="36" t="inlineStr">
+      <c r="D4" s="41" t="inlineStr">
         <is>
           <t>Terminé</t>
         </is>
       </c>
-      <c r="E4" s="36" t="inlineStr">
+      <c r="E4" s="41" t="inlineStr">
         <is>
           <t>Zina</t>
         </is>
       </c>
-      <c r="F4" s="36" t="inlineStr">
+      <c r="F4" s="41" t="inlineStr">
         <is>
           <t>7,28</t>
         </is>
       </c>
-      <c r="G4" s="36" t="inlineStr">
+      <c r="G4" s="41" t="inlineStr">
         <is>
           <t>5 min 15 s</t>
         </is>
@@ -10212,37 +10221,37 @@
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1" s="22">
-      <c r="A7" s="36" t="inlineStr">
+      <c r="A7" s="41" t="inlineStr">
         <is>
           <t>Abdelgow</t>
         </is>
       </c>
-      <c r="B7" s="36" t="inlineStr">
+      <c r="B7" s="41" t="inlineStr">
         <is>
           <t>Hassan Mahamat</t>
         </is>
       </c>
-      <c r="C7" s="36" t="inlineStr">
+      <c r="C7" s="41" t="inlineStr">
         <is>
           <t>hassan-mahamat.abdelgow@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D7" s="36" t="inlineStr">
+      <c r="D7" s="41" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="E7" s="36" t="inlineStr">
+      <c r="E7" s="41" t="inlineStr">
         <is>
           <t>Hassan Mahamat</t>
         </is>
       </c>
-      <c r="F7" s="36" t="inlineStr">
+      <c r="F7" s="41" t="inlineStr">
         <is>
           <t>7,52</t>
         </is>
       </c>
-      <c r="G7" s="36" t="inlineStr">
+      <c r="G7" s="41" t="inlineStr">
         <is>
           <t>23 min 37 s</t>
         </is>
@@ -10323,37 +10332,37 @@
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1" s="22">
-      <c r="A10" s="36" t="inlineStr">
+      <c r="A10" s="41" t="inlineStr">
         <is>
           <t>Abi Rizk</t>
         </is>
       </c>
-      <c r="B10" s="36" t="inlineStr">
+      <c r="B10" s="41" t="inlineStr">
         <is>
           <t>Rodolphe</t>
         </is>
       </c>
-      <c r="C10" s="36" t="inlineStr">
+      <c r="C10" s="41" t="inlineStr">
         <is>
           <t>rodolphe.abi-rizk@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D10" s="36" t="inlineStr">
+      <c r="D10" s="41" t="inlineStr">
         <is>
           <t>Terminé</t>
         </is>
       </c>
-      <c r="E10" s="36" t="inlineStr">
+      <c r="E10" s="41" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="F10" s="36" t="inlineStr">
+      <c r="F10" s="41" t="inlineStr">
         <is>
           <t>8,88</t>
         </is>
       </c>
-      <c r="G10" s="36" t="inlineStr">
+      <c r="G10" s="41" t="inlineStr">
         <is>
           <t>15 min 32 s</t>
         </is>
@@ -10397,37 +10406,37 @@
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1" s="22">
-      <c r="A12" s="36" t="inlineStr">
+      <c r="A12" s="41" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="B12" s="36" t="inlineStr">
+      <c r="B12" s="41" t="inlineStr">
         <is>
           <t>Iness</t>
         </is>
       </c>
-      <c r="C12" s="36" t="inlineStr">
+      <c r="C12" s="41" t="inlineStr">
         <is>
           <t>iness.abdenbaoui@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D12" s="36" t="inlineStr">
+      <c r="D12" s="41" t="inlineStr">
         <is>
           <t>Terminé</t>
         </is>
       </c>
-      <c r="E12" s="36" t="inlineStr">
+      <c r="E12" s="41" t="inlineStr">
         <is>
           <t>Iness</t>
         </is>
       </c>
-      <c r="F12" s="36" t="inlineStr">
+      <c r="F12" s="41" t="inlineStr">
         <is>
           <t>6,51</t>
         </is>
       </c>
-      <c r="G12" s="36" t="inlineStr">
+      <c r="G12" s="41" t="inlineStr">
         <is>
           <t>10 min 33 s</t>
         </is>
@@ -10471,37 +10480,37 @@
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1" s="22">
-      <c r="A14" s="37" t="inlineStr">
+      <c r="A14" s="41" t="inlineStr">
         <is>
           <t>Abi Rizk</t>
         </is>
       </c>
-      <c r="B14" s="37" t="inlineStr">
+      <c r="B14" s="41" t="inlineStr">
         <is>
           <t>Christian</t>
         </is>
       </c>
-      <c r="C14" s="37" t="inlineStr">
+      <c r="C14" s="41" t="inlineStr">
         <is>
           <t>christian.abi-rizk@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D14" s="37" t="inlineStr">
+      <c r="D14" s="41" t="inlineStr">
         <is>
           <t>Terminé</t>
         </is>
       </c>
-      <c r="E14" s="37" t="inlineStr">
+      <c r="E14" s="41" t="inlineStr">
         <is>
           <t>Christian</t>
         </is>
       </c>
-      <c r="F14" s="37" t="inlineStr">
+      <c r="F14" s="41" t="inlineStr">
         <is>
           <t>+</t>
         </is>
       </c>
-      <c r="G14" s="37" t="inlineStr">
+      <c r="G14" s="41" t="inlineStr">
         <is>
           <t>21 min 49 s</t>
         </is>

</xml_diff>

<commit_message>
feat(utils, module_pour_excel): add display_running_infos with an estimation of remaining time for all functions acting on several files or several tabs
</commit_message>
<xml_diff>
--- a/fichiers_xls/test.xlsx
+++ b/fichiers_xls/test.xlsx
@@ -91,7 +91,7 @@
       <sz val="11"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill/>
     </fill>
@@ -168,6 +168,11 @@
         <fgColor rgb="0000a933"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00ff2211"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -188,7 +193,7 @@
     <xf numFmtId="42" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
@@ -309,6 +314,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -2500,7 +2508,7 @@
           <t>paola.aatif-mieulet@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D2" s="38" t="inlineStr">
+      <c r="D2" s="42" t="inlineStr">
         <is>
           <t>Terminé</t>
         </is>
@@ -2819,7 +2827,7 @@
           <t>zina.abbas@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D3" s="38" t="inlineStr">
+      <c r="D3" s="42" t="inlineStr">
         <is>
           <t>Terminé</t>
         </is>
@@ -3140,7 +3148,7 @@
           <t>aboubaker.abdallah@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D4" s="38" t="inlineStr">
+      <c r="D4" s="42" t="inlineStr">
         <is>
           <t>Terminé</t>
         </is>
@@ -3459,7 +3467,7 @@
           <t>yasmine.abdel-moneim@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D5" s="38" t="inlineStr">
+      <c r="D5" s="42" t="inlineStr">
         <is>
           <t>Terminé</t>
         </is>
@@ -3883,7 +3891,7 @@
           <t>yasmine.abdelali@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D6" s="38" t="inlineStr">
+      <c r="D6" s="42" t="inlineStr">
         <is>
           <t>Terminé</t>
         </is>
@@ -4307,7 +4315,7 @@
           <t>hassan-mahamat.abdelgow@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D7" s="38" t="inlineStr">
+      <c r="D7" s="42" t="inlineStr">
         <is>
           <t>Terminé</t>
         </is>
@@ -4627,7 +4635,7 @@
           <t>nouh.abdelhadi@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D8" s="38" t="inlineStr">
+      <c r="D8" s="42" t="inlineStr">
         <is>
           <t>Terminé</t>
         </is>
@@ -4946,7 +4954,7 @@
           <t>yacine.abdelkarim@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D9" s="38" t="inlineStr">
+      <c r="D9" s="42" t="inlineStr">
         <is>
           <t>Terminé</t>
         </is>
@@ -5267,7 +5275,7 @@
           <t>iness.abdenbaoui@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D10" s="38" t="inlineStr">
+      <c r="D10" s="42" t="inlineStr">
         <is>
           <t>Terminé</t>
         </is>
@@ -5752,7 +5760,7 @@
           <t>houzefa.abdulhoussen@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D11" s="38" t="inlineStr">
+      <c r="D11" s="42" t="inlineStr">
         <is>
           <t>Terminé</t>
         </is>
@@ -6173,7 +6181,7 @@
           <t>20221641@etud.univ-evry.fr</t>
         </is>
       </c>
-      <c r="D12" s="38" t="inlineStr">
+      <c r="D12" s="42" t="inlineStr">
         <is>
           <t>Terminé</t>
         </is>
@@ -6494,7 +6502,7 @@
           <t>rodolphe.abi-rizk@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D13" s="38" t="inlineStr">
+      <c r="D13" s="42" t="inlineStr">
         <is>
           <t>Terminé</t>
         </is>
@@ -6814,7 +6822,7 @@
           <t>christian.abi-rizk@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D14" s="38" t="inlineStr">
+      <c r="D14" s="42" t="inlineStr">
         <is>
           <t>Terminé</t>
         </is>

</xml_diff>

<commit_message>
factor(one_file_one_tab): end factorisation of InsertController methods
</commit_message>
<xml_diff>
--- a/fichiers_xls/test.xlsx
+++ b/fichiers_xls/test.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="11" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -18,6 +18,8 @@
     <sheet name="cutinpartsbis" sheetId="9" state="visible" r:id="rId9"/>
     <sheet name="delete_lines" sheetId="10" state="visible" r:id="rId10"/>
     <sheet name="delete_lines_bis" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="time_min" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="time_min_expected" sheetId="13" state="visible" r:id="rId13"/>
   </sheets>
   <definedNames>
     <definedName name="_xlfn_T_TEST" hidden="0" function="0" vbProcedure="0">NA()</definedName>
@@ -424,8 +426,8 @@
           <yMode val="edge"/>
           <wMode val="factor"/>
           <hMode val="factor"/>
-          <x val="0.305385862111956"/>
-          <y val="0.0300204394481349"/>
+          <x val="0.305519176800748"/>
+          <y val="0.0309423347398031"/>
         </manualLayout>
       </layout>
       <overlay val="0"/>
@@ -444,10 +446,10 @@
           <yMode val="edge"/>
           <wMode val="factor"/>
           <hMode val="factor"/>
-          <x val="0.0127166188754519"/>
-          <y val="0.125574859478794"/>
-          <w val="0.963595561650667"/>
-          <h val="0.856285130301482"/>
+          <x val="0.0127221702525725"/>
+          <y val="0.125687252269531"/>
+          <w val="0.963143124415341"/>
+          <h val="0.85526147551464"/>
         </manualLayout>
       </layout>
       <barChart>
@@ -620,11 +622,11 @@
         </ser>
         <gapWidth val="219"/>
         <overlap val="-27"/>
-        <axId val="25103631"/>
-        <axId val="97802298"/>
+        <axId val="46191872"/>
+        <axId val="29177310"/>
       </barChart>
       <catAx>
-        <axId val="25103631"/>
+        <axId val="46191872"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
@@ -659,7 +661,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="97802298"/>
+        <crossAx val="29177310"/>
         <crossesAt val="0"/>
         <auto val="1"/>
         <lblAlgn val="ctr"/>
@@ -667,7 +669,7 @@
         <noMultiLvlLbl val="0"/>
       </catAx>
       <valAx>
-        <axId val="97802298"/>
+        <axId val="29177310"/>
         <scaling>
           <orientation val="minMax"/>
           <max val="100"/>
@@ -711,7 +713,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="25103631"/>
+        <crossAx val="46191872"/>
         <crossesAt val="1"/>
         <crossBetween val="midCat"/>
       </valAx>
@@ -768,8 +770,8 @@
           <yMode val="edge"/>
           <wMode val="factor"/>
           <hMode val="factor"/>
-          <x val="0.305243328100471"/>
-          <y val="0.0300204394481349"/>
+          <x val="0.305377559994974"/>
+          <y val="0.0309423347398031"/>
         </manualLayout>
       </layout>
       <overlay val="0"/>
@@ -788,10 +790,10 @@
           <yMode val="edge"/>
           <wMode val="factor"/>
           <hMode val="factor"/>
-          <x val="0.0127472527472527"/>
-          <y val="0.125574859478794"/>
-          <w val="0.96320251177394"/>
-          <h val="0.856285130301482"/>
+          <x val="0.0127528583992964"/>
+          <y val="0.125687252269531"/>
+          <w val="0.962746576203041"/>
+          <h val="0.85526147551464"/>
         </manualLayout>
       </layout>
       <barChart>
@@ -964,11 +966,11 @@
         </ser>
         <gapWidth val="219"/>
         <overlap val="-27"/>
-        <axId val="76034018"/>
-        <axId val="12270066"/>
+        <axId val="5370765"/>
+        <axId val="32017228"/>
       </barChart>
       <catAx>
-        <axId val="76034018"/>
+        <axId val="5370765"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
@@ -1003,7 +1005,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="12270066"/>
+        <crossAx val="32017228"/>
         <crossesAt val="0"/>
         <auto val="1"/>
         <lblAlgn val="ctr"/>
@@ -1011,7 +1013,7 @@
         <noMultiLvlLbl val="0"/>
       </catAx>
       <valAx>
-        <axId val="12270066"/>
+        <axId val="32017228"/>
         <scaling>
           <orientation val="minMax"/>
           <max val="100"/>
@@ -1055,7 +1057,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="76034018"/>
+        <crossAx val="5370765"/>
         <crossesAt val="1"/>
         <crossBetween val="midCat"/>
       </valAx>
@@ -1112,8 +1114,8 @@
           <yMode val="edge"/>
           <wMode val="factor"/>
           <hMode val="factor"/>
-          <x val="0.305412532964963"/>
-          <y val="0.030148185998978"/>
+          <x val="0.305546830831082"/>
+          <y val="0.0310701956271577"/>
         </manualLayout>
       </layout>
       <overlay val="0"/>
@@ -1133,10 +1135,10 @@
           <yMode val="edge"/>
           <wMode val="factor"/>
           <hMode val="factor"/>
-          <x val="0.052367198292101"/>
-          <y val="0.145886561062851"/>
-          <w val="0.924714303654402"/>
-          <h val="0.815661727133367"/>
+          <x val="0.0523902255166782"/>
+          <y val="0.146017133358906"/>
+          <w val="0.9242414724543"/>
+          <h val="0.814601713335891"/>
         </manualLayout>
       </layout>
       <barChart>
@@ -1309,11 +1311,11 @@
         </ser>
         <gapWidth val="219"/>
         <overlap val="-27"/>
-        <axId val="47487803"/>
-        <axId val="16667942"/>
+        <axId val="27704434"/>
+        <axId val="65417075"/>
       </barChart>
       <catAx>
-        <axId val="47487803"/>
+        <axId val="27704434"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
@@ -1348,7 +1350,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="16667942"/>
+        <crossAx val="65417075"/>
         <crosses val="autoZero"/>
         <auto val="1"/>
         <lblAlgn val="ctr"/>
@@ -1356,7 +1358,7 @@
         <noMultiLvlLbl val="0"/>
       </catAx>
       <valAx>
-        <axId val="16667942"/>
+        <axId val="65417075"/>
         <scaling>
           <orientation val="minMax"/>
           <max val="100"/>
@@ -1400,7 +1402,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="47487803"/>
+        <crossAx val="27704434"/>
         <crossesAt val="1"/>
         <crossBetween val="midCat"/>
       </valAx>
@@ -1457,8 +1459,8 @@
           <yMode val="edge"/>
           <wMode val="factor"/>
           <hMode val="factor"/>
-          <x val="0.305475323370589"/>
-          <y val="0.0302759325498212"/>
+          <x val="0.305609648847289"/>
+          <y val="0.0311980565145122"/>
         </manualLayout>
       </layout>
       <overlay val="0"/>
@@ -1478,10 +1480,10 @@
           <yMode val="edge"/>
           <wMode val="factor"/>
           <hMode val="factor"/>
-          <x val="0.052367198292101"/>
-          <y val="0.145886561062851"/>
-          <w val="0.924714303654402"/>
-          <h val="0.815661727133367"/>
+          <x val="0.0523902255166782"/>
+          <y val="0.146017133358906"/>
+          <w val="0.9242414724543"/>
+          <h val="0.814601713335891"/>
         </manualLayout>
       </layout>
       <barChart>
@@ -1654,11 +1656,11 @@
         </ser>
         <gapWidth val="219"/>
         <overlap val="-27"/>
-        <axId val="727618"/>
-        <axId val="1132976"/>
+        <axId val="65124397"/>
+        <axId val="8457015"/>
       </barChart>
       <catAx>
-        <axId val="727618"/>
+        <axId val="65124397"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
@@ -1693,7 +1695,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="1132976"/>
+        <crossAx val="8457015"/>
         <crosses val="autoZero"/>
         <auto val="1"/>
         <lblAlgn val="ctr"/>
@@ -1701,7 +1703,7 @@
         <noMultiLvlLbl val="0"/>
       </catAx>
       <valAx>
-        <axId val="1132976"/>
+        <axId val="8457015"/>
         <scaling>
           <orientation val="minMax"/>
           <max val="100"/>
@@ -1745,7 +1747,1042 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="727618"/>
+        <crossAx val="65124397"/>
+        <crossesAt val="1"/>
+        <crossBetween val="midCat"/>
+      </valAx>
+    </plotArea>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+  <spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="0">
+      <a:solidFill>
+        <a:srgbClr val="c0c0c0"/>
+      </a:solidFill>
+      <a:prstDash val="solid"/>
+    </a:ln>
+  </spPr>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" strike="noStrike" spc="-1">
+                <a:solidFill>
+                  <a:srgbClr val="333333"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr sz="1400" b="0" strike="noStrike" spc="-1">
+                <a:solidFill>
+                  <a:srgbClr val="333333"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+              </a:rPr>
+              <a:t>taux réussite ( %) par question</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+      <layout>
+        <manualLayout>
+          <xMode val="edge"/>
+          <yMode val="edge"/>
+          <wMode val="factor"/>
+          <hMode val="factor"/>
+          <x val="0.30550320392009"/>
+          <y val="0.0311980565145122"/>
+        </manualLayout>
+      </layout>
+      <overlay val="0"/>
+      <spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </title>
+    <plotArea>
+      <layout>
+        <manualLayout>
+          <layoutTarget val="inner"/>
+          <xMode val="edge"/>
+          <yMode val="edge"/>
+          <wMode val="factor"/>
+          <hMode val="factor"/>
+          <x val="0.0483729111697449"/>
+          <y val="0.146017133358906"/>
+          <w val="0.9271265234325921"/>
+          <h val="0.814473852448536"/>
+        </manualLayout>
+      </layout>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <varyColors val="0"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>time_min!$AS$13:$AS$13</f>
+              <strCache>
+                <ptCount val="1"/>
+                <pt idx="0">
+                  <v>None</v>
+                </pt>
+              </strCache>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:solidFill>
+              <a:srgbClr val="5b9bd5"/>
+            </a:solidFill>
+            <a:ln w="0">
+              <a:noFill/>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <invertIfNegative val="0"/>
+          <dLbls>
+            <txPr>
+              <a:bodyPr wrap="square"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:t>None</a:t>
+                </a:r>
+              </a:p>
+            </txPr>
+            <dLblPos val="outEnd"/>
+            <showLegendKey val="0"/>
+            <showVal val="0"/>
+            <showCatName val="0"/>
+            <showSerName val="0"/>
+            <showPercent val="0"/>
+            <showLeaderLines val="1"/>
+          </dLbls>
+          <cat>
+            <strRef>
+              <f>time_min!$AT$12:$BY$12</f>
+              <strCache>
+                <ptCount val="32"/>
+                <pt idx="0">
+                  <v>None</v>
+                </pt>
+                <pt idx="1">
+                  <v>None</v>
+                </pt>
+                <pt idx="2">
+                  <v>None</v>
+                </pt>
+                <pt idx="3">
+                  <v>None</v>
+                </pt>
+                <pt idx="4">
+                  <v>None</v>
+                </pt>
+                <pt idx="5">
+                  <v>None</v>
+                </pt>
+                <pt idx="6">
+                  <v>None</v>
+                </pt>
+                <pt idx="7">
+                  <v>None</v>
+                </pt>
+                <pt idx="8">
+                  <v>None</v>
+                </pt>
+                <pt idx="9">
+                  <v>None</v>
+                </pt>
+                <pt idx="10">
+                  <v>None</v>
+                </pt>
+                <pt idx="11">
+                  <v>None</v>
+                </pt>
+                <pt idx="12">
+                  <v>None</v>
+                </pt>
+                <pt idx="13">
+                  <v>None</v>
+                </pt>
+                <pt idx="14">
+                  <v>None</v>
+                </pt>
+                <pt idx="15">
+                  <v>None</v>
+                </pt>
+                <pt idx="16">
+                  <v>None</v>
+                </pt>
+                <pt idx="17">
+                  <v>None</v>
+                </pt>
+                <pt idx="18">
+                  <v>None</v>
+                </pt>
+                <pt idx="19">
+                  <v>None</v>
+                </pt>
+                <pt idx="20">
+                  <v>None</v>
+                </pt>
+                <pt idx="21">
+                  <v>None</v>
+                </pt>
+                <pt idx="22">
+                  <v>None</v>
+                </pt>
+                <pt idx="23">
+                  <v>None</v>
+                </pt>
+                <pt idx="24">
+                  <v>None</v>
+                </pt>
+                <pt idx="25">
+                  <v>None</v>
+                </pt>
+                <pt idx="26">
+                  <v>None</v>
+                </pt>
+                <pt idx="27">
+                  <v>None</v>
+                </pt>
+                <pt idx="28">
+                  <v>None</v>
+                </pt>
+                <pt idx="29">
+                  <v>None</v>
+                </pt>
+                <pt idx="30">
+                  <v>None</v>
+                </pt>
+                <pt idx="31">
+                  <v>None</v>
+                </pt>
+              </strCache>
+            </strRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>time_min!$AT$13:$BY$13</f>
+              <numCache>
+                <formatCode>General</formatCode>
+                <ptCount val="32"/>
+              </numCache>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="219"/>
+        <overlap val="-27"/>
+        <axId val="16514139"/>
+        <axId val="92265786"/>
+      </barChart>
+      <catAx>
+        <axId val="16514139"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <delete val="0"/>
+        <axPos val="b"/>
+        <numFmt formatCode="General" sourceLinked="0"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <tickLblPos val="nextTo"/>
+        <spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="c0c0c0"/>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+          </a:ln>
+        </spPr>
+        <txPr>
+          <a:bodyPr rot="-5400000"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
+                <a:solidFill>
+                  <a:srgbClr val="333333"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:t>None</a:t>
+            </a:r>
+          </a:p>
+        </txPr>
+        <crossAx val="92265786"/>
+        <crosses val="autoZero"/>
+        <auto val="1"/>
+        <lblAlgn val="ctr"/>
+        <lblOffset val="100"/>
+        <noMultiLvlLbl val="0"/>
+      </catAx>
+      <valAx>
+        <axId val="92265786"/>
+        <scaling>
+          <orientation val="minMax"/>
+          <max val="100"/>
+        </scaling>
+        <delete val="0"/>
+        <axPos val="l"/>
+        <majorGridlines>
+          <spPr>
+            <a:ln w="0">
+              <a:solidFill>
+                <a:srgbClr val="c0c0c0"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+        </majorGridlines>
+        <numFmt formatCode="0" sourceLinked="0"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <tickLblPos val="nextTo"/>
+        <spPr>
+          <a:ln w="0">
+            <a:noFill/>
+            <a:prstDash val="solid"/>
+          </a:ln>
+        </spPr>
+        <txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
+                <a:solidFill>
+                  <a:srgbClr val="333333"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:t>None</a:t>
+            </a:r>
+          </a:p>
+        </txPr>
+        <crossAx val="16514139"/>
+        <crossesAt val="1"/>
+        <crossBetween val="midCat"/>
+      </valAx>
+    </plotArea>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+  <spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="0">
+      <a:solidFill>
+        <a:srgbClr val="c0c0c0"/>
+      </a:solidFill>
+      <a:prstDash val="solid"/>
+    </a:ln>
+  </spPr>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" strike="noStrike" spc="-1">
+                <a:solidFill>
+                  <a:srgbClr val="333333"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr sz="1400" b="0" strike="noStrike" spc="-1">
+                <a:solidFill>
+                  <a:srgbClr val="333333"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+              </a:rPr>
+              <a:t>taux réussite ( %) par question</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+      <layout>
+        <manualLayout>
+          <xMode val="edge"/>
+          <yMode val="edge"/>
+          <wMode val="factor"/>
+          <hMode val="factor"/>
+          <x val="0.30550320392009"/>
+          <y val="0.0311858316221766"/>
+        </manualLayout>
+      </layout>
+      <overlay val="0"/>
+      <spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </title>
+    <plotArea>
+      <layout>
+        <manualLayout>
+          <layoutTarget val="inner"/>
+          <xMode val="edge"/>
+          <yMode val="edge"/>
+          <wMode val="factor"/>
+          <hMode val="factor"/>
+          <x val="0.0483729111697449"/>
+          <y val="0.145918891170431"/>
+          <w val="0.9271265234325921"/>
+          <h val="0.8145533880903491"/>
+        </manualLayout>
+      </layout>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <varyColors val="0"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>time_min_expected!$AW$13</f>
+              <strCache>
+                <ptCount val="1"/>
+                <pt idx="0">
+                  <v>None</v>
+                </pt>
+              </strCache>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:solidFill>
+              <a:srgbClr val="5b9bd5"/>
+            </a:solidFill>
+            <a:ln w="0">
+              <a:noFill/>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <invertIfNegative val="0"/>
+          <dLbls>
+            <txPr>
+              <a:bodyPr wrap="square"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:t>None</a:t>
+                </a:r>
+              </a:p>
+            </txPr>
+            <dLblPos val="outEnd"/>
+            <showLegendKey val="0"/>
+            <showVal val="0"/>
+            <showCatName val="0"/>
+            <showSerName val="0"/>
+            <showPercent val="0"/>
+            <showLeaderLines val="1"/>
+          </dLbls>
+          <cat>
+            <strRef>
+              <f>time_min_expected!$AX$12:$CC$12</f>
+              <strCache>
+                <ptCount val="32"/>
+                <pt idx="0">
+                  <v>None</v>
+                </pt>
+                <pt idx="1">
+                  <v>None</v>
+                </pt>
+                <pt idx="2">
+                  <v>None</v>
+                </pt>
+                <pt idx="3">
+                  <v>None</v>
+                </pt>
+                <pt idx="4">
+                  <v>None</v>
+                </pt>
+                <pt idx="5">
+                  <v>None</v>
+                </pt>
+                <pt idx="6">
+                  <v>None</v>
+                </pt>
+                <pt idx="7">
+                  <v>None</v>
+                </pt>
+                <pt idx="8">
+                  <v>None</v>
+                </pt>
+                <pt idx="9">
+                  <v>None</v>
+                </pt>
+                <pt idx="10">
+                  <v>None</v>
+                </pt>
+                <pt idx="11">
+                  <v>None</v>
+                </pt>
+                <pt idx="12">
+                  <v>None</v>
+                </pt>
+                <pt idx="13">
+                  <v>None</v>
+                </pt>
+                <pt idx="14">
+                  <v>None</v>
+                </pt>
+                <pt idx="15">
+                  <v>None</v>
+                </pt>
+                <pt idx="16">
+                  <v>None</v>
+                </pt>
+                <pt idx="17">
+                  <v>None</v>
+                </pt>
+                <pt idx="18">
+                  <v>None</v>
+                </pt>
+                <pt idx="19">
+                  <v>None</v>
+                </pt>
+                <pt idx="20">
+                  <v>None</v>
+                </pt>
+                <pt idx="21">
+                  <v>None</v>
+                </pt>
+                <pt idx="22">
+                  <v>None</v>
+                </pt>
+                <pt idx="23">
+                  <v>None</v>
+                </pt>
+                <pt idx="24">
+                  <v>None</v>
+                </pt>
+                <pt idx="25">
+                  <v>None</v>
+                </pt>
+                <pt idx="26">
+                  <v>None</v>
+                </pt>
+                <pt idx="27">
+                  <v>None</v>
+                </pt>
+                <pt idx="28">
+                  <v>None</v>
+                </pt>
+                <pt idx="29">
+                  <v>None</v>
+                </pt>
+                <pt idx="30">
+                  <v>None</v>
+                </pt>
+                <pt idx="31">
+                  <v>None</v>
+                </pt>
+              </strCache>
+            </strRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>time_min_expected!$AX$13:$CC$13</f>
+              <numCache>
+                <formatCode>General</formatCode>
+                <ptCount val="32"/>
+              </numCache>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="219"/>
+        <overlap val="-27"/>
+        <axId val="87775539"/>
+        <axId val="12380380"/>
+      </barChart>
+      <catAx>
+        <axId val="87775539"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <delete val="0"/>
+        <axPos val="b"/>
+        <numFmt formatCode="General" sourceLinked="0"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <tickLblPos val="nextTo"/>
+        <spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="c0c0c0"/>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+          </a:ln>
+        </spPr>
+        <txPr>
+          <a:bodyPr rot="-5400000"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
+                <a:solidFill>
+                  <a:srgbClr val="333333"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:t>None</a:t>
+            </a:r>
+          </a:p>
+        </txPr>
+        <crossAx val="12380380"/>
+        <crosses val="autoZero"/>
+        <auto val="1"/>
+        <lblAlgn val="ctr"/>
+        <lblOffset val="100"/>
+        <noMultiLvlLbl val="0"/>
+      </catAx>
+      <valAx>
+        <axId val="12380380"/>
+        <scaling>
+          <orientation val="minMax"/>
+          <max val="100"/>
+        </scaling>
+        <delete val="0"/>
+        <axPos val="l"/>
+        <majorGridlines>
+          <spPr>
+            <a:ln w="0">
+              <a:solidFill>
+                <a:srgbClr val="c0c0c0"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+        </majorGridlines>
+        <numFmt formatCode="0" sourceLinked="0"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <tickLblPos val="nextTo"/>
+        <spPr>
+          <a:ln w="0">
+            <a:noFill/>
+            <a:prstDash val="solid"/>
+          </a:ln>
+        </spPr>
+        <txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
+                <a:solidFill>
+                  <a:srgbClr val="333333"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:t>None</a:t>
+            </a:r>
+          </a:p>
+        </txPr>
+        <crossAx val="87775539"/>
+        <crossesAt val="1"/>
+        <crossBetween val="midCat"/>
+      </valAx>
+    </plotArea>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+  <spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="0">
+      <a:solidFill>
+        <a:srgbClr val="c0c0c0"/>
+      </a:solidFill>
+      <a:prstDash val="solid"/>
+    </a:ln>
+  </spPr>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" strike="noStrike" spc="-1">
+                <a:solidFill>
+                  <a:srgbClr val="333333"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr sz="1400" b="0" strike="noStrike" spc="-1">
+                <a:solidFill>
+                  <a:srgbClr val="333333"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+              </a:rPr>
+              <a:t>taux réussite ( %) par question</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+      <layout>
+        <manualLayout>
+          <xMode val="edge"/>
+          <yMode val="edge"/>
+          <wMode val="factor"/>
+          <hMode val="factor"/>
+          <x val="0.305628847845207"/>
+          <y val="0.0314425051334702"/>
+        </manualLayout>
+      </layout>
+      <overlay val="0"/>
+      <spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </title>
+    <plotArea>
+      <layout>
+        <manualLayout>
+          <layoutTarget val="inner"/>
+          <xMode val="edge"/>
+          <yMode val="edge"/>
+          <wMode val="factor"/>
+          <hMode val="factor"/>
+          <x val="0.0483729111697449"/>
+          <y val="0.145918891170431"/>
+          <w val="0.9271265234325921"/>
+          <h val="0.8145533880903491"/>
+        </manualLayout>
+      </layout>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <varyColors val="0"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>time_min_expected!$AW$13</f>
+              <strCache>
+                <ptCount val="1"/>
+                <pt idx="0">
+                  <v>None</v>
+                </pt>
+              </strCache>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:solidFill>
+              <a:srgbClr val="5b9bd5"/>
+            </a:solidFill>
+            <a:ln w="0">
+              <a:noFill/>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <invertIfNegative val="0"/>
+          <dLbls>
+            <txPr>
+              <a:bodyPr wrap="square"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:t>None</a:t>
+                </a:r>
+              </a:p>
+            </txPr>
+            <dLblPos val="outEnd"/>
+            <showLegendKey val="0"/>
+            <showVal val="0"/>
+            <showCatName val="0"/>
+            <showSerName val="0"/>
+            <showPercent val="0"/>
+            <showLeaderLines val="1"/>
+          </dLbls>
+          <cat>
+            <strRef>
+              <f>time_min_expected!$AX$12:$CC$12</f>
+              <strCache>
+                <ptCount val="32"/>
+                <pt idx="0">
+                  <v>None</v>
+                </pt>
+                <pt idx="1">
+                  <v>None</v>
+                </pt>
+                <pt idx="2">
+                  <v>None</v>
+                </pt>
+                <pt idx="3">
+                  <v>None</v>
+                </pt>
+                <pt idx="4">
+                  <v>None</v>
+                </pt>
+                <pt idx="5">
+                  <v>None</v>
+                </pt>
+                <pt idx="6">
+                  <v>None</v>
+                </pt>
+                <pt idx="7">
+                  <v>None</v>
+                </pt>
+                <pt idx="8">
+                  <v>None</v>
+                </pt>
+                <pt idx="9">
+                  <v>None</v>
+                </pt>
+                <pt idx="10">
+                  <v>None</v>
+                </pt>
+                <pt idx="11">
+                  <v>None</v>
+                </pt>
+                <pt idx="12">
+                  <v>None</v>
+                </pt>
+                <pt idx="13">
+                  <v>None</v>
+                </pt>
+                <pt idx="14">
+                  <v>None</v>
+                </pt>
+                <pt idx="15">
+                  <v>None</v>
+                </pt>
+                <pt idx="16">
+                  <v>None</v>
+                </pt>
+                <pt idx="17">
+                  <v>None</v>
+                </pt>
+                <pt idx="18">
+                  <v>None</v>
+                </pt>
+                <pt idx="19">
+                  <v>None</v>
+                </pt>
+                <pt idx="20">
+                  <v>None</v>
+                </pt>
+                <pt idx="21">
+                  <v>None</v>
+                </pt>
+                <pt idx="22">
+                  <v>None</v>
+                </pt>
+                <pt idx="23">
+                  <v>None</v>
+                </pt>
+                <pt idx="24">
+                  <v>None</v>
+                </pt>
+                <pt idx="25">
+                  <v>None</v>
+                </pt>
+                <pt idx="26">
+                  <v>None</v>
+                </pt>
+                <pt idx="27">
+                  <v>None</v>
+                </pt>
+                <pt idx="28">
+                  <v>None</v>
+                </pt>
+                <pt idx="29">
+                  <v>None</v>
+                </pt>
+                <pt idx="30">
+                  <v>None</v>
+                </pt>
+                <pt idx="31">
+                  <v>None</v>
+                </pt>
+              </strCache>
+            </strRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>time_min_expected!$AX$13:$CC$13</f>
+              <numCache>
+                <formatCode>General</formatCode>
+                <ptCount val="32"/>
+              </numCache>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="219"/>
+        <overlap val="-27"/>
+        <axId val="98824304"/>
+        <axId val="88787689"/>
+      </barChart>
+      <catAx>
+        <axId val="98824304"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <delete val="0"/>
+        <axPos val="b"/>
+        <numFmt formatCode="General" sourceLinked="0"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <tickLblPos val="nextTo"/>
+        <spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="c0c0c0"/>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+          </a:ln>
+        </spPr>
+        <txPr>
+          <a:bodyPr rot="-5400000"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
+                <a:solidFill>
+                  <a:srgbClr val="333333"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:t>None</a:t>
+            </a:r>
+          </a:p>
+        </txPr>
+        <crossAx val="88787689"/>
+        <crosses val="autoZero"/>
+        <auto val="1"/>
+        <lblAlgn val="ctr"/>
+        <lblOffset val="100"/>
+        <noMultiLvlLbl val="0"/>
+      </catAx>
+      <valAx>
+        <axId val="88787689"/>
+        <scaling>
+          <orientation val="minMax"/>
+          <max val="100"/>
+        </scaling>
+        <delete val="0"/>
+        <axPos val="l"/>
+        <majorGridlines>
+          <spPr>
+            <a:ln w="0">
+              <a:solidFill>
+                <a:srgbClr val="c0c0c0"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+        </majorGridlines>
+        <numFmt formatCode="0" sourceLinked="0"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <tickLblPos val="nextTo"/>
+        <spPr>
+          <a:ln w="0">
+            <a:noFill/>
+            <a:prstDash val="solid"/>
+          </a:ln>
+        </spPr>
+        <txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
+                <a:solidFill>
+                  <a:srgbClr val="333333"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:t>None</a:t>
+            </a:r>
+          </a:p>
+        </txPr>
+        <crossAx val="98824304"/>
         <crossesAt val="1"/>
         <crossBetween val="midCat"/>
       </valAx>
@@ -1778,9 +2815,9 @@
     </from>
     <to>
       <col>99</col>
-      <colOff>207360</colOff>
+      <colOff>204840</colOff>
       <row>30</row>
-      <rowOff>120960</rowOff>
+      <rowOff>118440</rowOff>
     </to>
     <graphicFrame>
       <nvGraphicFramePr>
@@ -1810,9 +2847,9 @@
     </from>
     <to>
       <col>76</col>
-      <colOff>678960</colOff>
+      <colOff>676440</colOff>
       <row>30</row>
-      <rowOff>120600</rowOff>
+      <rowOff>118080</rowOff>
     </to>
     <graphicFrame>
       <nvGraphicFramePr>
@@ -1842,9 +2879,9 @@
     </from>
     <to>
       <col>107</col>
-      <colOff>678960</colOff>
+      <colOff>676440</colOff>
       <row>30</row>
-      <rowOff>119880</rowOff>
+      <rowOff>117360</rowOff>
     </to>
     <graphicFrame>
       <nvGraphicFramePr>
@@ -1874,9 +2911,9 @@
     </from>
     <to>
       <col>107</col>
-      <colOff>678960</colOff>
+      <colOff>676440</colOff>
       <row>30</row>
-      <rowOff>119880</rowOff>
+      <rowOff>117360</rowOff>
     </to>
     <graphicFrame>
       <nvGraphicFramePr>
@@ -1887,6 +2924,97 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </twoCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <twoCellAnchor editAs="oneCell">
+    <from>
+      <col>66</col>
+      <colOff>9720</colOff>
+      <row>13</row>
+      <rowOff>93600</rowOff>
+    </from>
+    <to>
+      <col>72</col>
+      <colOff>676440</colOff>
+      <row>30</row>
+      <rowOff>155880</rowOff>
+    </to>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </twoCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <twoCellAnchor editAs="oneCell">
+    <from>
+      <col>70</col>
+      <colOff>9720</colOff>
+      <row>13</row>
+      <rowOff>93600</rowOff>
+    </from>
+    <to>
+      <col>76</col>
+      <colOff>676440</colOff>
+      <row>30</row>
+      <rowOff>145440</rowOff>
+    </to>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </twoCellAnchor>
+  <twoCellAnchor editAs="oneCell">
+    <from>
+      <col>70</col>
+      <colOff>9720</colOff>
+      <row>13</row>
+      <rowOff>93600</rowOff>
+    </from>
+    <to>
+      <col>76</col>
+      <colOff>676440</colOff>
+      <row>30</row>
+      <rowOff>145440</rowOff>
+    </to>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="2" name="Chart 2"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -7853,6 +8981,366 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr filterMode="0">
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr fitToPage="0"/>
+  </sheetPr>
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.9765625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col width="11.53" customWidth="1" style="38" min="16357" max="16384"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="15.75" customHeight="1" s="23">
+      <c r="A1" s="38" t="inlineStr">
+        <is>
+          <t>Nom</t>
+        </is>
+      </c>
+      <c r="B1" s="38" t="inlineStr">
+        <is>
+          <t>Prénom</t>
+        </is>
+      </c>
+      <c r="C1" s="38" t="inlineStr">
+        <is>
+          <t>Adresse de courriel</t>
+        </is>
+      </c>
+      <c r="D1" s="38" t="inlineStr">
+        <is>
+          <t>État</t>
+        </is>
+      </c>
+      <c r="E1" s="38" t="inlineStr">
+        <is>
+          <t>Temps utilisé</t>
+        </is>
+      </c>
+      <c r="F1" s="38" t="n"/>
+    </row>
+    <row r="2" ht="15.75" customHeight="1" s="23">
+      <c r="A2" s="38" t="inlineStr">
+        <is>
+          <t>Abdulhoussen</t>
+        </is>
+      </c>
+      <c r="B2" s="38" t="inlineStr">
+        <is>
+          <t>Houzefa</t>
+        </is>
+      </c>
+      <c r="C2" s="38" t="inlineStr">
+        <is>
+          <t>houzefa.abdulhoussen@universite-paris-saclay.fr</t>
+        </is>
+      </c>
+      <c r="D2" s="38" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="E2" s="26" t="inlineStr">
+        <is>
+          <t>5 min 49 s</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" ht="15.75" customHeight="1" s="23">
+      <c r="A3" s="38" t="inlineStr">
+        <is>
+          <t>Abdel Moneim</t>
+        </is>
+      </c>
+      <c r="B3" s="38" t="inlineStr">
+        <is>
+          <t>Yasmine</t>
+        </is>
+      </c>
+      <c r="C3" s="38" t="inlineStr">
+        <is>
+          <t>yasmine.abdel-moneim@universite-paris-saclay.fr</t>
+        </is>
+      </c>
+      <c r="D3" s="38" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="E3" s="26" t="inlineStr">
+        <is>
+          <t>7 min</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="15.75" customHeight="1" s="23">
+      <c r="A4" s="38" t="inlineStr">
+        <is>
+          <t>Abbas</t>
+        </is>
+      </c>
+      <c r="B4" s="38" t="inlineStr">
+        <is>
+          <t>Zina</t>
+        </is>
+      </c>
+      <c r="C4" s="38" t="inlineStr">
+        <is>
+          <t>zina.abbas@universite-paris-saclay.fr</t>
+        </is>
+      </c>
+      <c r="D4" s="38" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="E4" s="26" t="inlineStr">
+        <is>
+          <t>1 jour 5 heures</t>
+        </is>
+      </c>
+      <c r="F4" s="38" t="n"/>
+    </row>
+    <row r="5" ht="15.75" customHeight="1" s="23">
+      <c r="A5" s="38" t="inlineStr">
+        <is>
+          <t>Abdallah</t>
+        </is>
+      </c>
+      <c r="B5" s="38" t="inlineStr">
+        <is>
+          <t>Aboubaker</t>
+        </is>
+      </c>
+      <c r="C5" s="38" t="inlineStr">
+        <is>
+          <t>aboubaker.abdallah@universite-paris-saclay.fr</t>
+        </is>
+      </c>
+      <c r="D5" s="38" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="E5" s="26" t="inlineStr">
+        <is>
+          <t>2 jours 10 min</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentOddEven="0" differentFirst="0">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12 &amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12 Page &amp;P</oddFooter>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr filterMode="0">
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr fitToPage="0"/>
+  </sheetPr>
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.9765625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col width="11.53" customWidth="1" style="38" min="16361" max="16384"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="15.75" customHeight="1" s="23">
+      <c r="A1" s="38" t="inlineStr">
+        <is>
+          <t>Nom</t>
+        </is>
+      </c>
+      <c r="B1" s="38" t="inlineStr">
+        <is>
+          <t>Prénom</t>
+        </is>
+      </c>
+      <c r="C1" s="38" t="inlineStr">
+        <is>
+          <t>Adresse de courriel</t>
+        </is>
+      </c>
+      <c r="D1" s="38" t="inlineStr">
+        <is>
+          <t>État</t>
+        </is>
+      </c>
+      <c r="E1" s="38" t="inlineStr">
+        <is>
+          <t>Temps utilisé</t>
+        </is>
+      </c>
+      <c r="F1" s="38" t="n"/>
+    </row>
+    <row r="2" ht="15.75" customHeight="1" s="23">
+      <c r="A2" s="38" t="inlineStr">
+        <is>
+          <t>Abdulhoussen</t>
+        </is>
+      </c>
+      <c r="B2" s="38" t="inlineStr">
+        <is>
+          <t>Houzefa</t>
+        </is>
+      </c>
+      <c r="C2" s="38" t="inlineStr">
+        <is>
+          <t>houzefa.abdulhoussen@universite-paris-saclay.fr</t>
+        </is>
+      </c>
+      <c r="D2" s="38" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="E2" s="26" t="inlineStr">
+        <is>
+          <t>5 min 49 s</t>
+        </is>
+      </c>
+      <c r="F2" s="38" t="inlineStr">
+        <is>
+          <t>5,82</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" ht="15.75" customHeight="1" s="23">
+      <c r="A3" s="38" t="inlineStr">
+        <is>
+          <t>Abdel Moneim</t>
+        </is>
+      </c>
+      <c r="B3" s="38" t="inlineStr">
+        <is>
+          <t>Yasmine</t>
+        </is>
+      </c>
+      <c r="C3" s="38" t="inlineStr">
+        <is>
+          <t>yasmine.abdel-moneim@universite-paris-saclay.fr</t>
+        </is>
+      </c>
+      <c r="D3" s="38" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="E3" s="26" t="inlineStr">
+        <is>
+          <t>7 min</t>
+        </is>
+      </c>
+      <c r="F3" s="38" t="inlineStr">
+        <is>
+          <t>7,0</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="15.75" customHeight="1" s="23">
+      <c r="A4" s="38" t="inlineStr">
+        <is>
+          <t>Abbas</t>
+        </is>
+      </c>
+      <c r="B4" s="38" t="inlineStr">
+        <is>
+          <t>Zina</t>
+        </is>
+      </c>
+      <c r="C4" s="38" t="inlineStr">
+        <is>
+          <t>zina.abbas@universite-paris-saclay.fr</t>
+        </is>
+      </c>
+      <c r="D4" s="38" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="E4" s="26" t="inlineStr">
+        <is>
+          <t>1 jour 5 heures</t>
+        </is>
+      </c>
+      <c r="F4" s="38" t="inlineStr">
+        <is>
+          <t>1740,0</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="15.75" customHeight="1" s="23">
+      <c r="A5" s="38" t="inlineStr">
+        <is>
+          <t>Abdallah</t>
+        </is>
+      </c>
+      <c r="B5" s="38" t="inlineStr">
+        <is>
+          <t>Aboubaker</t>
+        </is>
+      </c>
+      <c r="C5" s="38" t="inlineStr">
+        <is>
+          <t>aboubaker.abdallah@universite-paris-saclay.fr</t>
+        </is>
+      </c>
+      <c r="D5" s="38" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="E5" s="26" t="inlineStr">
+        <is>
+          <t>2 jours 10 min</t>
+        </is>
+      </c>
+      <c r="F5" s="38" t="inlineStr">
+        <is>
+          <t>2890,0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048576" ht="12.75" customHeight="1" s="23"/>
+  </sheetData>
+  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentOddEven="0" differentFirst="0">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12 &amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12 Page &amp;P</oddFooter>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr filterMode="0">
@@ -8899,8 +10387,8 @@
   </sheetPr>
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="11.9765625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
factor(path.py): end of refactoring controller functions
</commit_message>
<xml_diff>
--- a/fichiers_xls/test.xlsx
+++ b/fichiers_xls/test.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="11" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -426,8 +426,8 @@
           <yMode val="edge"/>
           <wMode val="factor"/>
           <hMode val="factor"/>
-          <x val="0.305519176800748"/>
-          <y val="0.0309423347398031"/>
+          <x val="0.305538231258576"/>
+          <y val="0.031074168797954"/>
         </manualLayout>
       </layout>
       <overlay val="0"/>
@@ -446,10 +446,10 @@
           <yMode val="edge"/>
           <wMode val="factor"/>
           <hMode val="factor"/>
-          <x val="0.0127221702525725"/>
-          <y val="0.125687252269531"/>
-          <w val="0.963143124415341"/>
-          <h val="0.85526147551464"/>
+          <x val="0.012722963702133"/>
+          <y val="0.125703324808184"/>
+          <w val="0.963078458276163"/>
+          <h val="0.855115089514067"/>
         </manualLayout>
       </layout>
       <barChart>
@@ -461,7 +461,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>Feuille5!$AW$13:$AW$13</f>
+              <f>Feuille5!$AS$13:$AS$13</f>
               <strCache>
                 <ptCount val="1"/>
                 <pt idx="0">
@@ -508,7 +508,7 @@
           </dLbls>
           <cat>
             <strRef>
-              <f>Feuille5!$AX$12:$CC$12</f>
+              <f>Feuille5!$AT$12:$BY$12</f>
               <strCache>
                 <ptCount val="32"/>
                 <pt idx="0">
@@ -612,7 +612,7 @@
           </cat>
           <val>
             <numRef>
-              <f>Feuille5!$AX$13:$CC$13</f>
+              <f>Feuille5!$AT$13:$BY$13</f>
               <numCache>
                 <formatCode>General</formatCode>
                 <ptCount val="32"/>
@@ -622,11 +622,11 @@
         </ser>
         <gapWidth val="219"/>
         <overlap val="-27"/>
-        <axId val="46191872"/>
-        <axId val="29177310"/>
+        <axId val="84471571"/>
+        <axId val="11320165"/>
       </barChart>
       <catAx>
-        <axId val="46191872"/>
+        <axId val="84471571"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
@@ -661,7 +661,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="29177310"/>
+        <crossAx val="11320165"/>
         <crossesAt val="0"/>
         <auto val="1"/>
         <lblAlgn val="ctr"/>
@@ -669,7 +669,7 @@
         <noMultiLvlLbl val="0"/>
       </catAx>
       <valAx>
-        <axId val="29177310"/>
+        <axId val="11320165"/>
         <scaling>
           <orientation val="minMax"/>
           <max val="100"/>
@@ -713,7 +713,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="46191872"/>
+        <crossAx val="84471571"/>
         <crossesAt val="1"/>
         <crossBetween val="midCat"/>
       </valAx>
@@ -770,8 +770,8 @@
           <yMode val="edge"/>
           <wMode val="factor"/>
           <hMode val="factor"/>
-          <x val="0.305377559994974"/>
-          <y val="0.0309423347398031"/>
+          <x val="0.305396745617893"/>
+          <y val="0.031074168797954"/>
         </manualLayout>
       </layout>
       <overlay val="0"/>
@@ -790,10 +790,10 @@
           <yMode val="edge"/>
           <wMode val="factor"/>
           <hMode val="factor"/>
-          <x val="0.0127528583992964"/>
-          <y val="0.125687252269531"/>
-          <w val="0.962746576203041"/>
-          <h val="0.85526147551464"/>
+          <x val="0.0127536596092228"/>
+          <y val="0.125703324808184"/>
+          <w val="0.962681409813407"/>
+          <h val="0.855115089514067"/>
         </manualLayout>
       </layout>
       <barChart>
@@ -805,7 +805,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>Feuille5!$AW$13:$AW$13</f>
+              <f>Feuille5!$AS$13:$AS$13</f>
               <strCache>
                 <ptCount val="1"/>
                 <pt idx="0">
@@ -852,7 +852,7 @@
           </dLbls>
           <cat>
             <strRef>
-              <f>Feuille5!$AX$12:$CC$12</f>
+              <f>Feuille5!$AT$12:$BY$12</f>
               <strCache>
                 <ptCount val="32"/>
                 <pt idx="0">
@@ -956,7 +956,7 @@
           </cat>
           <val>
             <numRef>
-              <f>Feuille5!$AX$13:$CC$13</f>
+              <f>Feuille5!$AT$13:$BY$13</f>
               <numCache>
                 <formatCode>General</formatCode>
                 <ptCount val="32"/>
@@ -966,11 +966,11 @@
         </ser>
         <gapWidth val="219"/>
         <overlap val="-27"/>
-        <axId val="5370765"/>
-        <axId val="32017228"/>
+        <axId val="81245660"/>
+        <axId val="46782103"/>
       </barChart>
       <catAx>
-        <axId val="5370765"/>
+        <axId val="81245660"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
@@ -1005,7 +1005,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="32017228"/>
+        <crossAx val="46782103"/>
         <crossesAt val="0"/>
         <auto val="1"/>
         <lblAlgn val="ctr"/>
@@ -1013,7 +1013,7 @@
         <noMultiLvlLbl val="0"/>
       </catAx>
       <valAx>
-        <axId val="32017228"/>
+        <axId val="46782103"/>
         <scaling>
           <orientation val="minMax"/>
           <max val="100"/>
@@ -1057,7 +1057,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="5370765"/>
+        <crossAx val="81245660"/>
         <crossesAt val="1"/>
         <crossBetween val="midCat"/>
       </valAx>
@@ -1114,8 +1114,8 @@
           <yMode val="edge"/>
           <wMode val="factor"/>
           <hMode val="factor"/>
-          <x val="0.305546830831082"/>
-          <y val="0.0310701956271577"/>
+          <x val="0.305566025882649"/>
+          <y val="0.0312020460358056"/>
         </manualLayout>
       </layout>
       <overlay val="0"/>
@@ -1135,10 +1135,10 @@
           <yMode val="edge"/>
           <wMode val="factor"/>
           <hMode val="factor"/>
-          <x val="0.0523902255166782"/>
-          <y val="0.146017133358906"/>
-          <w val="0.9242414724543"/>
-          <h val="0.814601713335891"/>
+          <x val="0.052393516773464"/>
+          <y val="0.146035805626598"/>
+          <w val="0.924173891192361"/>
+          <h val="0.814450127877238"/>
         </manualLayout>
       </layout>
       <barChart>
@@ -1311,11 +1311,11 @@
         </ser>
         <gapWidth val="219"/>
         <overlap val="-27"/>
-        <axId val="27704434"/>
-        <axId val="65417075"/>
+        <axId val="41299039"/>
+        <axId val="63796112"/>
       </barChart>
       <catAx>
-        <axId val="27704434"/>
+        <axId val="41299039"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
@@ -1350,7 +1350,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="65417075"/>
+        <crossAx val="63796112"/>
         <crosses val="autoZero"/>
         <auto val="1"/>
         <lblAlgn val="ctr"/>
@@ -1358,7 +1358,7 @@
         <noMultiLvlLbl val="0"/>
       </catAx>
       <valAx>
-        <axId val="65417075"/>
+        <axId val="63796112"/>
         <scaling>
           <orientation val="minMax"/>
           <max val="100"/>
@@ -1402,7 +1402,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="27704434"/>
+        <crossAx val="41299039"/>
         <crossesAt val="1"/>
         <crossBetween val="midCat"/>
       </valAx>
@@ -1459,8 +1459,8 @@
           <yMode val="edge"/>
           <wMode val="factor"/>
           <hMode val="factor"/>
-          <x val="0.305609648847289"/>
-          <y val="0.0311980565145122"/>
+          <x val="0.305628847845207"/>
+          <y val="0.0313299232736573"/>
         </manualLayout>
       </layout>
       <overlay val="0"/>
@@ -1480,10 +1480,10 @@
           <yMode val="edge"/>
           <wMode val="factor"/>
           <hMode val="factor"/>
-          <x val="0.0523902255166782"/>
-          <y val="0.146017133358906"/>
-          <w val="0.9242414724543"/>
-          <h val="0.814601713335891"/>
+          <x val="0.052393516773464"/>
+          <y val="0.146035805626598"/>
+          <w val="0.924173891192361"/>
+          <h val="0.814450127877238"/>
         </manualLayout>
       </layout>
       <barChart>
@@ -1656,11 +1656,11 @@
         </ser>
         <gapWidth val="219"/>
         <overlap val="-27"/>
-        <axId val="65124397"/>
-        <axId val="8457015"/>
+        <axId val="35133032"/>
+        <axId val="71765336"/>
       </barChart>
       <catAx>
-        <axId val="65124397"/>
+        <axId val="35133032"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
@@ -1695,7 +1695,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="8457015"/>
+        <crossAx val="71765336"/>
         <crosses val="autoZero"/>
         <auto val="1"/>
         <lblAlgn val="ctr"/>
@@ -1703,7 +1703,7 @@
         <noMultiLvlLbl val="0"/>
       </catAx>
       <valAx>
-        <axId val="8457015"/>
+        <axId val="71765336"/>
         <scaling>
           <orientation val="minMax"/>
           <max val="100"/>
@@ -1747,7 +1747,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="65124397"/>
+        <crossAx val="35133032"/>
         <crossesAt val="1"/>
         <crossBetween val="midCat"/>
       </valAx>
@@ -1804,8 +1804,8 @@
           <yMode val="edge"/>
           <wMode val="factor"/>
           <hMode val="factor"/>
-          <x val="0.30550320392009"/>
-          <y val="0.0311980565145122"/>
+          <x val="0.305522397436703"/>
+          <y val="0.0313299232736573"/>
         </manualLayout>
       </layout>
       <overlay val="0"/>
@@ -1825,10 +1825,10 @@
           <yMode val="edge"/>
           <wMode val="factor"/>
           <hMode val="factor"/>
-          <x val="0.0483729111697449"/>
-          <y val="0.146017133358906"/>
-          <w val="0.9271265234325921"/>
-          <h val="0.814473852448536"/>
+          <x val="0.0483759502418798"/>
+          <y val="0.146035805626598"/>
+          <w val="0.92705911918075"/>
+          <h val="0.814322250639386"/>
         </manualLayout>
       </layout>
       <barChart>
@@ -2001,11 +2001,11 @@
         </ser>
         <gapWidth val="219"/>
         <overlap val="-27"/>
-        <axId val="16514139"/>
-        <axId val="92265786"/>
+        <axId val="53306918"/>
+        <axId val="89418232"/>
       </barChart>
       <catAx>
-        <axId val="16514139"/>
+        <axId val="53306918"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
@@ -2040,7 +2040,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="92265786"/>
+        <crossAx val="89418232"/>
         <crosses val="autoZero"/>
         <auto val="1"/>
         <lblAlgn val="ctr"/>
@@ -2048,7 +2048,7 @@
         <noMultiLvlLbl val="0"/>
       </catAx>
       <valAx>
-        <axId val="92265786"/>
+        <axId val="89418232"/>
         <scaling>
           <orientation val="minMax"/>
           <max val="100"/>
@@ -2092,7 +2092,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="16514139"/>
+        <crossAx val="53306918"/>
         <crossesAt val="1"/>
         <crossBetween val="midCat"/>
       </valAx>
@@ -2149,8 +2149,8 @@
           <yMode val="edge"/>
           <wMode val="factor"/>
           <hMode val="factor"/>
-          <x val="0.30550320392009"/>
-          <y val="0.0311858316221766"/>
+          <x val="0.305522397436703"/>
+          <y val="0.0313181876524195"/>
         </manualLayout>
       </layout>
       <overlay val="0"/>
@@ -2170,10 +2170,10 @@
           <yMode val="edge"/>
           <wMode val="factor"/>
           <hMode val="factor"/>
-          <x val="0.0483729111697449"/>
-          <y val="0.145918891170431"/>
-          <w val="0.9271265234325921"/>
-          <h val="0.8145533880903491"/>
+          <x val="0.0483759502418798"/>
+          <y val="0.145937620331151"/>
+          <w val="0.92705911918075"/>
+          <h val="0.81440123219099"/>
         </manualLayout>
       </layout>
       <barChart>
@@ -2346,11 +2346,11 @@
         </ser>
         <gapWidth val="219"/>
         <overlap val="-27"/>
-        <axId val="87775539"/>
-        <axId val="12380380"/>
+        <axId val="83668030"/>
+        <axId val="76635886"/>
       </barChart>
       <catAx>
-        <axId val="87775539"/>
+        <axId val="83668030"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
@@ -2385,7 +2385,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="12380380"/>
+        <crossAx val="76635886"/>
         <crosses val="autoZero"/>
         <auto val="1"/>
         <lblAlgn val="ctr"/>
@@ -2393,7 +2393,7 @@
         <noMultiLvlLbl val="0"/>
       </catAx>
       <valAx>
-        <axId val="12380380"/>
+        <axId val="76635886"/>
         <scaling>
           <orientation val="minMax"/>
           <max val="100"/>
@@ -2437,7 +2437,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="87775539"/>
+        <crossAx val="83668030"/>
         <crossesAt val="1"/>
         <crossBetween val="midCat"/>
       </valAx>
@@ -2494,8 +2494,8 @@
           <yMode val="edge"/>
           <wMode val="factor"/>
           <hMode val="factor"/>
-          <x val="0.305628847845207"/>
-          <y val="0.0314425051334702"/>
+          <x val="0.305648049255513"/>
+          <y val="0.0315748941085868"/>
         </manualLayout>
       </layout>
       <overlay val="0"/>
@@ -2515,10 +2515,10 @@
           <yMode val="edge"/>
           <wMode val="factor"/>
           <hMode val="factor"/>
-          <x val="0.0483729111697449"/>
-          <y val="0.145918891170431"/>
-          <w val="0.9271265234325921"/>
-          <h val="0.8145533880903491"/>
+          <x val="0.0483759502418798"/>
+          <y val="0.145937620331151"/>
+          <w val="0.92705911918075"/>
+          <h val="0.81440123219099"/>
         </manualLayout>
       </layout>
       <barChart>
@@ -2691,11 +2691,11 @@
         </ser>
         <gapWidth val="219"/>
         <overlap val="-27"/>
-        <axId val="98824304"/>
-        <axId val="88787689"/>
+        <axId val="36938005"/>
+        <axId val="11693007"/>
       </barChart>
       <catAx>
-        <axId val="98824304"/>
+        <axId val="36938005"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
@@ -2730,7 +2730,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="88787689"/>
+        <crossAx val="11693007"/>
         <crosses val="autoZero"/>
         <auto val="1"/>
         <lblAlgn val="ctr"/>
@@ -2738,7 +2738,7 @@
         <noMultiLvlLbl val="0"/>
       </catAx>
       <valAx>
-        <axId val="88787689"/>
+        <axId val="11693007"/>
         <scaling>
           <orientation val="minMax"/>
           <max val="100"/>
@@ -2782,7 +2782,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="98824304"/>
+        <crossAx val="36938005"/>
         <crossesAt val="1"/>
         <crossBetween val="midCat"/>
       </valAx>
@@ -2815,9 +2815,9 @@
     </from>
     <to>
       <col>99</col>
-      <colOff>204840</colOff>
+      <colOff>204480</colOff>
       <row>30</row>
-      <rowOff>118440</rowOff>
+      <rowOff>118080</rowOff>
     </to>
     <graphicFrame>
       <nvGraphicFramePr>
@@ -2840,16 +2840,16 @@
 <wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <twoCellAnchor editAs="oneCell">
     <from>
-      <col>70</col>
+      <col>66</col>
       <colOff>9720</colOff>
       <row>13</row>
       <rowOff>93600</rowOff>
     </from>
     <to>
-      <col>76</col>
-      <colOff>676440</colOff>
+      <col>72</col>
+      <colOff>676080</colOff>
       <row>30</row>
-      <rowOff>118080</rowOff>
+      <rowOff>117720</rowOff>
     </to>
     <graphicFrame>
       <nvGraphicFramePr>
@@ -2879,9 +2879,9 @@
     </from>
     <to>
       <col>107</col>
-      <colOff>676440</colOff>
+      <colOff>676080</colOff>
       <row>30</row>
-      <rowOff>117360</rowOff>
+      <rowOff>117000</rowOff>
     </to>
     <graphicFrame>
       <nvGraphicFramePr>
@@ -2911,9 +2911,9 @@
     </from>
     <to>
       <col>107</col>
-      <colOff>676440</colOff>
+      <colOff>676080</colOff>
       <row>30</row>
-      <rowOff>117360</rowOff>
+      <rowOff>117000</rowOff>
     </to>
     <graphicFrame>
       <nvGraphicFramePr>
@@ -2943,9 +2943,9 @@
     </from>
     <to>
       <col>72</col>
-      <colOff>676440</colOff>
+      <colOff>676080</colOff>
       <row>30</row>
-      <rowOff>155880</rowOff>
+      <rowOff>155520</rowOff>
     </to>
     <graphicFrame>
       <nvGraphicFramePr>
@@ -2975,9 +2975,9 @@
     </from>
     <to>
       <col>76</col>
-      <colOff>676440</colOff>
+      <colOff>676080</colOff>
       <row>30</row>
-      <rowOff>145440</rowOff>
+      <rowOff>145080</rowOff>
     </to>
     <graphicFrame>
       <nvGraphicFramePr>
@@ -3002,9 +3002,9 @@
     </from>
     <to>
       <col>76</col>
-      <colOff>676440</colOff>
+      <colOff>676080</colOff>
       <row>30</row>
-      <rowOff>145440</rowOff>
+      <rowOff>145080</rowOff>
     </to>
     <graphicFrame>
       <nvGraphicFramePr>
@@ -8987,9 +8987,9 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
@@ -9024,7 +9024,7 @@
           <t>Temps utilisé</t>
         </is>
       </c>
-      <c r="F1" s="38" t="n"/>
+      <c r="H1" s="38" t="n"/>
     </row>
     <row r="2" ht="15.75" customHeight="1" s="23">
       <c r="A2" s="38" t="inlineStr">
@@ -9052,6 +9052,16 @@
           <t>5 min 49 s</t>
         </is>
       </c>
+      <c r="F2" s="38" t="inlineStr">
+        <is>
+          <t>5,82</t>
+        </is>
+      </c>
+      <c r="G2" s="38" t="inlineStr">
+        <is>
+          <t>5,82</t>
+        </is>
+      </c>
     </row>
     <row r="3" ht="15.75" customHeight="1" s="23">
       <c r="A3" s="38" t="inlineStr">
@@ -9079,6 +9089,16 @@
           <t>7 min</t>
         </is>
       </c>
+      <c r="F3" s="38" t="inlineStr">
+        <is>
+          <t>7,0</t>
+        </is>
+      </c>
+      <c r="G3" s="38" t="inlineStr">
+        <is>
+          <t>7,0</t>
+        </is>
+      </c>
     </row>
     <row r="4" ht="15.75" customHeight="1" s="23">
       <c r="A4" s="38" t="inlineStr">
@@ -9106,7 +9126,17 @@
           <t>1 jour 5 heures</t>
         </is>
       </c>
-      <c r="F4" s="38" t="n"/>
+      <c r="F4" s="38" t="inlineStr">
+        <is>
+          <t>1740,0</t>
+        </is>
+      </c>
+      <c r="G4" s="38" t="inlineStr">
+        <is>
+          <t>1740,0</t>
+        </is>
+      </c>
+      <c r="H4" s="38" t="n"/>
     </row>
     <row r="5" ht="15.75" customHeight="1" s="23">
       <c r="A5" s="38" t="inlineStr">
@@ -9132,6 +9162,16 @@
       <c r="E5" s="26" t="inlineStr">
         <is>
           <t>2 jours 10 min</t>
+        </is>
+      </c>
+      <c r="F5" s="38" t="inlineStr">
+        <is>
+          <t>2890,0</t>
+        </is>
+      </c>
+      <c r="G5" s="38" t="inlineStr">
+        <is>
+          <t>2890,0</t>
         </is>
       </c>
     </row>
@@ -9347,7 +9387,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
@@ -9370,7 +9410,7 @@
           <t>Le cerveau est constitué uniquement de neurones</t>
         </is>
       </c>
-      <c r="H1" s="24" t="inlineStr">
+      <c r="J1" s="24" t="inlineStr">
         <is>
           <t>accuracy_Q27</t>
         </is>
@@ -9388,6 +9428,12 @@
       <c r="H2" s="38" t="n">
         <v>1</v>
       </c>
+      <c r="I2" s="38" t="n">
+        <v>1</v>
+      </c>
+      <c r="J2" s="38" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" ht="12.75" customHeight="1" s="23">
       <c r="F3" s="38" t="inlineStr">
@@ -9401,6 +9447,12 @@
       <c r="H3" s="38" t="n">
         <v>1</v>
       </c>
+      <c r="I3" s="38" t="n">
+        <v>1</v>
+      </c>
+      <c r="J3" s="38" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" ht="12.75" customHeight="1" s="23">
       <c r="C4" s="38" t="inlineStr">
@@ -9419,6 +9471,12 @@
       <c r="H4" s="38" t="n">
         <v>1</v>
       </c>
+      <c r="I4" s="38" t="n">
+        <v>1</v>
+      </c>
+      <c r="J4" s="38" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" ht="12.75" customHeight="1" s="23">
       <c r="F5" s="38" t="inlineStr">
@@ -9432,6 +9490,12 @@
       <c r="H5" s="38" t="n">
         <v>1</v>
       </c>
+      <c r="I5" s="38" t="n">
+        <v>1</v>
+      </c>
+      <c r="J5" s="38" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" ht="12.75" customHeight="1" s="23">
       <c r="B6" s="38" t="inlineStr">
@@ -9450,6 +9514,12 @@
       <c r="H6" s="38" t="n">
         <v>1</v>
       </c>
+      <c r="I6" s="38" t="n">
+        <v>1</v>
+      </c>
+      <c r="J6" s="38" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" ht="12.75" customHeight="1" s="23">
       <c r="B7" s="38" t="inlineStr">
@@ -9468,6 +9538,12 @@
       <c r="H7" s="38" t="n">
         <v>1</v>
       </c>
+      <c r="I7" s="38" t="n">
+        <v>1</v>
+      </c>
+      <c r="J7" s="38" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" ht="12.75" customHeight="1" s="23">
       <c r="F8" s="38" t="inlineStr">
@@ -9481,6 +9557,12 @@
       <c r="H8" s="38" t="n">
         <v>0</v>
       </c>
+      <c r="I8" s="38" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" s="38" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" ht="12.75" customHeight="1" s="23">
       <c r="F9" s="38" t="inlineStr">
@@ -9494,6 +9576,12 @@
       <c r="H9" s="38" t="n">
         <v>1</v>
       </c>
+      <c r="I9" s="38" t="n">
+        <v>1</v>
+      </c>
+      <c r="J9" s="38" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" ht="12.75" customHeight="1" s="23">
       <c r="F10" s="38" t="inlineStr">
@@ -9507,6 +9595,12 @@
       <c r="H10" s="38" t="n">
         <v>0</v>
       </c>
+      <c r="I10" s="38" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" s="38" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" ht="12.75" customHeight="1" s="23">
       <c r="F11" s="38" t="inlineStr">
@@ -9520,6 +9614,12 @@
       <c r="H11" s="38" t="n">
         <v>1</v>
       </c>
+      <c r="I11" s="38" t="n">
+        <v>1</v>
+      </c>
+      <c r="J11" s="38" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" ht="12.75" customHeight="1" s="23">
       <c r="F12" s="38" t="inlineStr">
@@ -9533,6 +9633,12 @@
       <c r="H12" s="38" t="n">
         <v>1</v>
       </c>
+      <c r="I12" s="38" t="n">
+        <v>1</v>
+      </c>
+      <c r="J12" s="38" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" ht="12.75" customHeight="1" s="23">
       <c r="F13" s="38" t="inlineStr">
@@ -9546,6 +9652,12 @@
       <c r="H13" s="38" t="n">
         <v>1</v>
       </c>
+      <c r="I13" s="38" t="n">
+        <v>1</v>
+      </c>
+      <c r="J13" s="38" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" ht="12.75" customHeight="1" s="23">
       <c r="F14" s="38" t="inlineStr">
@@ -9557,6 +9669,12 @@
         <v>1</v>
       </c>
       <c r="H14" s="38" t="n">
+        <v>1</v>
+      </c>
+      <c r="I14" s="38" t="n">
+        <v>1</v>
+      </c>
+      <c r="J14" s="38" t="n">
         <v>1</v>
       </c>
     </row>
@@ -10388,12 +10506,12 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="11.9765625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col width="11.53" customWidth="1" style="38" min="16361" max="16384"/>
+    <col width="11.53" customWidth="1" style="38" min="16357" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1" s="23">
@@ -11903,15 +12021,15 @@
   </sheetPr>
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="11.9140625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col width="11.31" customWidth="1" style="38" min="1" max="2"/>
-    <col width="11.52" customWidth="1" style="38" min="980" max="1006"/>
-    <col width="11.53" customWidth="1" style="38" min="16367" max="16384"/>
+    <col width="11.52" customWidth="1" style="38" min="974" max="1000"/>
+    <col width="11.53" customWidth="1" style="38" min="16361" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1" s="23">

</xml_diff>

<commit_message>
factor(tests_for_factorise): add an AssertIdentical class
</commit_message>
<xml_diff>
--- a/fichiers_xls/test.xlsx
+++ b/fichiers_xls/test.xlsx
@@ -9387,7 +9387,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
@@ -9410,7 +9410,7 @@
           <t>Le cerveau est constitué uniquement de neurones</t>
         </is>
       </c>
-      <c r="J1" s="24" t="inlineStr">
+      <c r="N1" s="24" t="inlineStr">
         <is>
           <t>accuracy_Q27</t>
         </is>
@@ -9434,6 +9434,18 @@
       <c r="J2" s="38" t="n">
         <v>1</v>
       </c>
+      <c r="K2" s="38" t="n">
+        <v>1</v>
+      </c>
+      <c r="L2" s="38" t="n">
+        <v>1</v>
+      </c>
+      <c r="M2" s="38" t="n">
+        <v>1</v>
+      </c>
+      <c r="N2" s="38" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" ht="12.75" customHeight="1" s="23">
       <c r="F3" s="38" t="inlineStr">
@@ -9453,6 +9465,18 @@
       <c r="J3" s="38" t="n">
         <v>1</v>
       </c>
+      <c r="K3" s="38" t="n">
+        <v>1</v>
+      </c>
+      <c r="L3" s="38" t="n">
+        <v>1</v>
+      </c>
+      <c r="M3" s="38" t="n">
+        <v>1</v>
+      </c>
+      <c r="N3" s="38" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" ht="12.75" customHeight="1" s="23">
       <c r="C4" s="38" t="inlineStr">
@@ -9477,6 +9501,18 @@
       <c r="J4" s="38" t="n">
         <v>1</v>
       </c>
+      <c r="K4" s="38" t="n">
+        <v>1</v>
+      </c>
+      <c r="L4" s="38" t="n">
+        <v>1</v>
+      </c>
+      <c r="M4" s="38" t="n">
+        <v>1</v>
+      </c>
+      <c r="N4" s="38" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" ht="12.75" customHeight="1" s="23">
       <c r="F5" s="38" t="inlineStr">
@@ -9496,6 +9532,18 @@
       <c r="J5" s="38" t="n">
         <v>1</v>
       </c>
+      <c r="K5" s="38" t="n">
+        <v>1</v>
+      </c>
+      <c r="L5" s="38" t="n">
+        <v>1</v>
+      </c>
+      <c r="M5" s="38" t="n">
+        <v>1</v>
+      </c>
+      <c r="N5" s="38" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" ht="12.75" customHeight="1" s="23">
       <c r="B6" s="38" t="inlineStr">
@@ -9520,6 +9568,18 @@
       <c r="J6" s="38" t="n">
         <v>1</v>
       </c>
+      <c r="K6" s="38" t="n">
+        <v>1</v>
+      </c>
+      <c r="L6" s="38" t="n">
+        <v>1</v>
+      </c>
+      <c r="M6" s="38" t="n">
+        <v>1</v>
+      </c>
+      <c r="N6" s="38" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" ht="12.75" customHeight="1" s="23">
       <c r="B7" s="38" t="inlineStr">
@@ -9544,6 +9604,18 @@
       <c r="J7" s="38" t="n">
         <v>1</v>
       </c>
+      <c r="K7" s="38" t="n">
+        <v>1</v>
+      </c>
+      <c r="L7" s="38" t="n">
+        <v>1</v>
+      </c>
+      <c r="M7" s="38" t="n">
+        <v>1</v>
+      </c>
+      <c r="N7" s="38" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" ht="12.75" customHeight="1" s="23">
       <c r="F8" s="38" t="inlineStr">
@@ -9563,6 +9635,18 @@
       <c r="J8" s="38" t="n">
         <v>0</v>
       </c>
+      <c r="K8" s="38" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" s="38" t="n">
+        <v>0</v>
+      </c>
+      <c r="M8" s="38" t="n">
+        <v>0</v>
+      </c>
+      <c r="N8" s="38" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" ht="12.75" customHeight="1" s="23">
       <c r="F9" s="38" t="inlineStr">
@@ -9582,6 +9666,18 @@
       <c r="J9" s="38" t="n">
         <v>1</v>
       </c>
+      <c r="K9" s="38" t="n">
+        <v>1</v>
+      </c>
+      <c r="L9" s="38" t="n">
+        <v>1</v>
+      </c>
+      <c r="M9" s="38" t="n">
+        <v>1</v>
+      </c>
+      <c r="N9" s="38" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" ht="12.75" customHeight="1" s="23">
       <c r="F10" s="38" t="inlineStr">
@@ -9601,6 +9697,18 @@
       <c r="J10" s="38" t="n">
         <v>0</v>
       </c>
+      <c r="K10" s="38" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" s="38" t="n">
+        <v>0</v>
+      </c>
+      <c r="M10" s="38" t="n">
+        <v>0</v>
+      </c>
+      <c r="N10" s="38" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" ht="12.75" customHeight="1" s="23">
       <c r="F11" s="38" t="inlineStr">
@@ -9620,6 +9728,18 @@
       <c r="J11" s="38" t="n">
         <v>1</v>
       </c>
+      <c r="K11" s="38" t="n">
+        <v>1</v>
+      </c>
+      <c r="L11" s="38" t="n">
+        <v>1</v>
+      </c>
+      <c r="M11" s="38" t="n">
+        <v>1</v>
+      </c>
+      <c r="N11" s="38" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" ht="12.75" customHeight="1" s="23">
       <c r="F12" s="38" t="inlineStr">
@@ -9639,6 +9759,18 @@
       <c r="J12" s="38" t="n">
         <v>1</v>
       </c>
+      <c r="K12" s="38" t="n">
+        <v>1</v>
+      </c>
+      <c r="L12" s="38" t="n">
+        <v>1</v>
+      </c>
+      <c r="M12" s="38" t="n">
+        <v>1</v>
+      </c>
+      <c r="N12" s="38" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" ht="12.75" customHeight="1" s="23">
       <c r="F13" s="38" t="inlineStr">
@@ -9658,6 +9790,18 @@
       <c r="J13" s="38" t="n">
         <v>1</v>
       </c>
+      <c r="K13" s="38" t="n">
+        <v>1</v>
+      </c>
+      <c r="L13" s="38" t="n">
+        <v>1</v>
+      </c>
+      <c r="M13" s="38" t="n">
+        <v>1</v>
+      </c>
+      <c r="N13" s="38" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" ht="12.75" customHeight="1" s="23">
       <c r="F14" s="38" t="inlineStr">
@@ -9675,6 +9819,18 @@
         <v>1</v>
       </c>
       <c r="J14" s="38" t="n">
+        <v>1</v>
+      </c>
+      <c r="K14" s="38" t="n">
+        <v>1</v>
+      </c>
+      <c r="L14" s="38" t="n">
+        <v>1</v>
+      </c>
+      <c r="M14" s="38" t="n">
+        <v>1</v>
+      </c>
+      <c r="N14" s="38" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
factor(tests_for_factorise): add TestStr and TestTabUpdate classes and finish TestColumnInsertion class
</commit_message>
<xml_diff>
--- a/fichiers_xls/test.xlsx
+++ b/fichiers_xls/test.xlsx
@@ -9487,7 +9487,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
@@ -9511,7 +9511,7 @@
           <t>Le cerveau est constitué uniquement de neurones</t>
         </is>
       </c>
-      <c r="K1" s="24" t="inlineStr">
+      <c r="M1" s="24" t="inlineStr">
         <is>
           <t>accuracy_Q27</t>
         </is>
@@ -9538,6 +9538,12 @@
       <c r="K2" s="20" t="n">
         <v>1</v>
       </c>
+      <c r="L2" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="M2" s="20" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" ht="12.75" customHeight="1" s="23">
       <c r="F3" s="20" t="inlineStr">
@@ -9560,6 +9566,12 @@
       <c r="K3" s="20" t="n">
         <v>1</v>
       </c>
+      <c r="L3" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="M3" s="20" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" ht="12.75" customHeight="1" s="23">
       <c r="C4" s="20" t="inlineStr">
@@ -9587,6 +9599,12 @@
       <c r="K4" s="20" t="n">
         <v>1</v>
       </c>
+      <c r="L4" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="M4" s="20" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" ht="12.75" customHeight="1" s="23">
       <c r="F5" s="20" t="inlineStr">
@@ -9609,6 +9627,12 @@
       <c r="K5" s="20" t="n">
         <v>1</v>
       </c>
+      <c r="L5" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="M5" s="20" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" ht="12.75" customHeight="1" s="23">
       <c r="B6" s="20" t="inlineStr">
@@ -9636,6 +9660,12 @@
       <c r="K6" s="20" t="n">
         <v>1</v>
       </c>
+      <c r="L6" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="M6" s="20" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" ht="12.75" customHeight="1" s="23">
       <c r="B7" s="20" t="inlineStr">
@@ -9663,6 +9693,12 @@
       <c r="K7" s="20" t="n">
         <v>1</v>
       </c>
+      <c r="L7" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="M7" s="20" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" ht="12.75" customHeight="1" s="23">
       <c r="F8" s="20" t="inlineStr">
@@ -9685,6 +9721,12 @@
       <c r="K8" s="20" t="n">
         <v>0</v>
       </c>
+      <c r="L8" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="M8" s="20" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" ht="12.75" customHeight="1" s="23">
       <c r="F9" s="20" t="inlineStr">
@@ -9707,6 +9749,12 @@
       <c r="K9" s="20" t="n">
         <v>1</v>
       </c>
+      <c r="L9" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="M9" s="20" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" ht="12.75" customHeight="1" s="23">
       <c r="F10" s="20" t="inlineStr">
@@ -9729,6 +9777,12 @@
       <c r="K10" s="20" t="n">
         <v>0</v>
       </c>
+      <c r="L10" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="M10" s="20" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" ht="12.75" customHeight="1" s="23">
       <c r="F11" s="20" t="inlineStr">
@@ -9751,6 +9805,12 @@
       <c r="K11" s="20" t="n">
         <v>1</v>
       </c>
+      <c r="L11" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="M11" s="20" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" ht="12.75" customHeight="1" s="23">
       <c r="F12" s="20" t="inlineStr">
@@ -9773,6 +9833,12 @@
       <c r="K12" s="20" t="n">
         <v>1</v>
       </c>
+      <c r="L12" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="M12" s="20" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" ht="12.75" customHeight="1" s="23">
       <c r="F13" s="20" t="inlineStr">
@@ -9795,6 +9861,12 @@
       <c r="K13" s="20" t="n">
         <v>1</v>
       </c>
+      <c r="L13" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="M13" s="20" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" ht="12.75" customHeight="1" s="23">
       <c r="F14" s="20" t="inlineStr">
@@ -9815,6 +9887,12 @@
         <v>1</v>
       </c>
       <c r="K14" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="L14" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="M14" s="20" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
factor(xlspython_factorise): factor cutsendmail and multipletabs
</commit_message>
<xml_diff>
--- a/fichiers_xls/test.xlsx
+++ b/fichiers_xls/test.xlsx
@@ -94,7 +94,7 @@
       <sz val="11"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill/>
     </fill>
@@ -161,6 +161,11 @@
         <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0000a933"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -181,7 +186,7 @@
     <xf numFmtId="42" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
@@ -298,6 +303,15 @@
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -475,7 +489,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:t/>
+                  <a:t>None</a:t>
                 </a:r>
               </a:p>
             </txPr>
@@ -638,7 +652,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
           </a:p>
         </txPr>
@@ -690,7 +704,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
           </a:p>
         </txPr>
@@ -819,7 +833,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:t/>
+                  <a:t>None</a:t>
                 </a:r>
               </a:p>
             </txPr>
@@ -982,7 +996,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
           </a:p>
         </txPr>
@@ -1034,7 +1048,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
           </a:p>
         </txPr>
@@ -1164,7 +1178,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:t/>
+                  <a:t>None</a:t>
                 </a:r>
               </a:p>
             </txPr>
@@ -1327,7 +1341,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
           </a:p>
         </txPr>
@@ -1379,7 +1393,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
           </a:p>
         </txPr>
@@ -1509,7 +1523,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:t/>
+                  <a:t>None</a:t>
                 </a:r>
               </a:p>
             </txPr>
@@ -1672,7 +1686,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
           </a:p>
         </txPr>
@@ -1724,7 +1738,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
           </a:p>
         </txPr>
@@ -1854,7 +1868,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:t/>
+                  <a:t>None</a:t>
                 </a:r>
               </a:p>
             </txPr>
@@ -2017,7 +2031,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
           </a:p>
         </txPr>
@@ -2069,7 +2083,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
           </a:p>
         </txPr>
@@ -2199,7 +2213,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:t/>
+                  <a:t>None</a:t>
                 </a:r>
               </a:p>
             </txPr>
@@ -2362,7 +2376,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
           </a:p>
         </txPr>
@@ -2414,7 +2428,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
           </a:p>
         </txPr>
@@ -2544,7 +2558,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:t/>
+                  <a:t>None</a:t>
                 </a:r>
               </a:p>
             </txPr>
@@ -2707,7 +2721,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
           </a:p>
         </txPr>
@@ -2759,7 +2773,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
           </a:p>
         </txPr>
@@ -3191,7 +3205,7 @@
       <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.66796875" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.66796875" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col width="11.09" customWidth="1" style="20" min="1" max="7"/>
     <col width="140.36" customWidth="1" style="20" min="8" max="8"/>
@@ -8264,7 +8278,7 @@
       <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.9140625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.9140625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col width="11.31" customWidth="1" style="20" min="1" max="3"/>
     <col width="21.53" customWidth="1" style="20" min="4" max="4"/>
@@ -8301,7 +8315,7 @@
           <t xml:space="preserve">partie 1 : Vrai; partie 2 : Faux; partie 3 : Vrai </t>
         </is>
       </c>
-      <c r="C2" s="21" t="inlineStr">
+      <c r="C2" s="40" t="inlineStr">
         <is>
           <t>partie 1 : Vrai</t>
         </is>
@@ -8316,7 +8330,7 @@
           <t xml:space="preserve"> partie 3 : Vrai </t>
         </is>
       </c>
-      <c r="F2" s="20" t="inlineStr">
+      <c r="F2" s="41" t="inlineStr">
         <is>
           <t>partie 1 : Vrai</t>
         </is>
@@ -8328,7 +8342,7 @@
       </c>
     </row>
     <row r="3" ht="12.75" customHeight="1" s="23">
-      <c r="A3" s="20" t="inlineStr">
+      <c r="A3" s="41" t="inlineStr">
         <is>
           <t>Abbas</t>
         </is>
@@ -8338,7 +8352,7 @@
           <t xml:space="preserve">partie 1 : Vrai; partie 2 : Vrai; partie 3 : Vrai </t>
         </is>
       </c>
-      <c r="C3" s="21" t="inlineStr">
+      <c r="C3" s="40" t="inlineStr">
         <is>
           <t>partie 1 : Vrai</t>
         </is>
@@ -8353,7 +8367,7 @@
           <t xml:space="preserve"> partie 3 : Vrai </t>
         </is>
       </c>
-      <c r="F3" s="20" t="inlineStr">
+      <c r="F3" s="41" t="inlineStr">
         <is>
           <t>partie 1 : Vrai</t>
         </is>
@@ -8373,7 +8387,7 @@
           <t xml:space="preserve">partie 1 : Vrai; partie 2 : Faux; partie 3 : Vrai </t>
         </is>
       </c>
-      <c r="C4" s="21" t="inlineStr">
+      <c r="C4" s="40" t="inlineStr">
         <is>
           <t>partie 1 : Vrai</t>
         </is>
@@ -8388,7 +8402,7 @@
           <t xml:space="preserve"> partie 3 : Vrai </t>
         </is>
       </c>
-      <c r="F4" s="20" t="inlineStr">
+      <c r="F4" s="41" t="inlineStr">
         <is>
           <t>partie 1 : Vrai</t>
         </is>
@@ -8410,7 +8424,7 @@
           <t xml:space="preserve">partie 1 : Vrai; partie 2 : Faux; partie 3 : Vrai </t>
         </is>
       </c>
-      <c r="C5" s="21" t="inlineStr">
+      <c r="C5" s="40" t="inlineStr">
         <is>
           <t>partie 1 : Vrai</t>
         </is>
@@ -8472,7 +8486,7 @@
       <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.55078125" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.55078125" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col width="11.54" customWidth="1" style="20" min="1" max="1024"/>
   </cols>
@@ -8836,7 +8850,7 @@
       <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.55078125" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.55078125" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col width="11.54" customWidth="1" style="20" min="1" max="1024"/>
   </cols>
@@ -9186,7 +9200,7 @@
       <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.9765625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.9765625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col width="11.53" customWidth="1" style="20" min="16345" max="16384"/>
   </cols>
@@ -9356,7 +9370,7 @@
       <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.9765625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.9765625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col width="11.53" customWidth="1" style="20" min="16361" max="16384"/>
   </cols>
@@ -9540,13 +9554,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:L14"/>
+  <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="12.2109375" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.2109375" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col width="11.08" customWidth="1" style="20" min="6" max="6"/>
     <col width="11.52" customWidth="1" style="20" min="932" max="1009"/>
@@ -9559,12 +9573,12 @@
           <t>Test !!!!</t>
         </is>
       </c>
-      <c r="G1" s="24" t="inlineStr">
+      <c r="H1" s="24" t="inlineStr">
         <is>
           <t>Le cerveau est constitué uniquement de neurones</t>
         </is>
       </c>
-      <c r="L1" s="24" t="inlineStr">
+      <c r="M1" s="24" t="inlineStr">
         <is>
           <t>accuracy_Q27</t>
         </is>
@@ -9574,14 +9588,14 @@
       <c r="F2" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="G2" s="20" t="inlineStr">
+      <c r="G2" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" s="20" t="inlineStr">
         <is>
           <t xml:space="preserve"> partie 12 : Faux</t>
         </is>
       </c>
-      <c r="H2" s="20" t="n">
-        <v>0</v>
-      </c>
       <c r="I2" s="20" t="n">
         <v>0</v>
       </c>
@@ -9589,9 +9603,12 @@
         <v>0</v>
       </c>
       <c r="K2" s="20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L2" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="M2" s="20" t="n">
         <v>1</v>
       </c>
     </row>
@@ -9604,14 +9621,14 @@
       <c r="F3" s="20" t="n">
         <v>1</v>
       </c>
-      <c r="G3" s="20" t="inlineStr">
+      <c r="G3" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="20" t="inlineStr">
         <is>
           <t xml:space="preserve"> partie 12 : Faux</t>
         </is>
       </c>
-      <c r="H3" s="20" t="n">
-        <v>0</v>
-      </c>
       <c r="I3" s="20" t="n">
         <v>0</v>
       </c>
@@ -9619,9 +9636,12 @@
         <v>0</v>
       </c>
       <c r="K3" s="20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L3" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="M3" s="20" t="n">
         <v>1</v>
       </c>
     </row>
@@ -9639,14 +9659,14 @@
       <c r="F4" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="G4" s="20" t="inlineStr">
+      <c r="G4" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" s="20" t="inlineStr">
         <is>
           <t xml:space="preserve"> partie 12 : Faux</t>
         </is>
       </c>
-      <c r="H4" s="20" t="n">
-        <v>0</v>
-      </c>
       <c r="I4" s="20" t="n">
         <v>0</v>
       </c>
@@ -9654,9 +9674,12 @@
         <v>0</v>
       </c>
       <c r="K4" s="20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L4" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="M4" s="20" t="n">
         <v>1</v>
       </c>
     </row>
@@ -9669,14 +9692,14 @@
       <c r="F5" s="20" t="n">
         <v>1</v>
       </c>
-      <c r="G5" s="20" t="inlineStr">
+      <c r="G5" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="20" t="inlineStr">
         <is>
           <t xml:space="preserve"> partie 12 : Faux</t>
         </is>
       </c>
-      <c r="H5" s="20" t="n">
-        <v>0</v>
-      </c>
       <c r="I5" s="20" t="n">
         <v>0</v>
       </c>
@@ -9684,9 +9707,12 @@
         <v>0</v>
       </c>
       <c r="K5" s="20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L5" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="M5" s="20" t="n">
         <v>1</v>
       </c>
     </row>
@@ -9704,14 +9730,14 @@
       <c r="F6" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="G6" s="20" t="inlineStr">
+      <c r="G6" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="20" t="inlineStr">
         <is>
           <t xml:space="preserve"> partie 12 : Faux</t>
         </is>
       </c>
-      <c r="H6" s="20" t="n">
-        <v>0</v>
-      </c>
       <c r="I6" s="20" t="n">
         <v>0</v>
       </c>
@@ -9719,9 +9745,12 @@
         <v>0</v>
       </c>
       <c r="K6" s="20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L6" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="M6" s="20" t="n">
         <v>1</v>
       </c>
     </row>
@@ -9734,14 +9763,14 @@
       <c r="F7" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="G7" s="20" t="inlineStr">
+      <c r="G7" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" s="20" t="inlineStr">
         <is>
           <t xml:space="preserve"> partie 12 : Faux</t>
         </is>
       </c>
-      <c r="H7" s="20" t="n">
-        <v>0</v>
-      </c>
       <c r="I7" s="20" t="n">
         <v>0</v>
       </c>
@@ -9749,9 +9778,12 @@
         <v>0</v>
       </c>
       <c r="K7" s="20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L7" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="M7" s="20" t="n">
         <v>1</v>
       </c>
     </row>
@@ -9759,14 +9791,14 @@
       <c r="F8" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="G8" s="20" t="inlineStr">
+      <c r="G8" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" s="20" t="inlineStr">
         <is>
           <t xml:space="preserve"> partie 12 : Vrai</t>
         </is>
       </c>
-      <c r="H8" s="20" t="n">
-        <v>0</v>
-      </c>
       <c r="I8" s="20" t="n">
         <v>0</v>
       </c>
@@ -9777,6 +9809,9 @@
         <v>0</v>
       </c>
       <c r="L8" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="M8" s="20" t="n">
         <v>0</v>
       </c>
     </row>
@@ -9784,14 +9819,14 @@
       <c r="F9" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="G9" s="20" t="inlineStr">
+      <c r="G9" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="20" t="inlineStr">
         <is>
           <t xml:space="preserve"> partie 12 : Faux</t>
         </is>
       </c>
-      <c r="H9" s="20" t="n">
-        <v>0</v>
-      </c>
       <c r="I9" s="20" t="n">
         <v>0</v>
       </c>
@@ -9799,9 +9834,12 @@
         <v>0</v>
       </c>
       <c r="K9" s="20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L9" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="M9" s="20" t="n">
         <v>1</v>
       </c>
     </row>
@@ -9809,14 +9847,14 @@
       <c r="F10" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="G10" s="20" t="inlineStr">
+      <c r="G10" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" s="20" t="inlineStr">
         <is>
           <t xml:space="preserve"> partie 12 : Vrai</t>
         </is>
       </c>
-      <c r="H10" s="20" t="n">
-        <v>0</v>
-      </c>
       <c r="I10" s="20" t="n">
         <v>0</v>
       </c>
@@ -9827,6 +9865,9 @@
         <v>0</v>
       </c>
       <c r="L10" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="M10" s="20" t="n">
         <v>0</v>
       </c>
     </row>
@@ -9834,14 +9875,14 @@
       <c r="F11" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="G11" s="20" t="inlineStr">
+      <c r="G11" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" s="20" t="inlineStr">
         <is>
           <t xml:space="preserve"> partie 12 : Faux</t>
         </is>
       </c>
-      <c r="H11" s="20" t="n">
-        <v>0</v>
-      </c>
       <c r="I11" s="20" t="n">
         <v>0</v>
       </c>
@@ -9849,9 +9890,12 @@
         <v>0</v>
       </c>
       <c r="K11" s="20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L11" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="M11" s="20" t="n">
         <v>1</v>
       </c>
     </row>
@@ -9859,14 +9903,14 @@
       <c r="F12" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="G12" s="20" t="inlineStr">
+      <c r="G12" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" s="20" t="inlineStr">
         <is>
           <t xml:space="preserve"> partie 12 : Faux</t>
         </is>
       </c>
-      <c r="H12" s="20" t="n">
-        <v>0</v>
-      </c>
       <c r="I12" s="20" t="n">
         <v>0</v>
       </c>
@@ -9874,9 +9918,12 @@
         <v>0</v>
       </c>
       <c r="K12" s="20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L12" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="M12" s="20" t="n">
         <v>1</v>
       </c>
     </row>
@@ -9884,14 +9931,14 @@
       <c r="F13" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="G13" s="20" t="inlineStr">
+      <c r="G13" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" s="20" t="inlineStr">
         <is>
           <t xml:space="preserve"> partie 12 : Faux</t>
         </is>
       </c>
-      <c r="H13" s="20" t="n">
-        <v>0</v>
-      </c>
       <c r="I13" s="20" t="n">
         <v>0</v>
       </c>
@@ -9899,9 +9946,12 @@
         <v>0</v>
       </c>
       <c r="K13" s="20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L13" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="M13" s="20" t="n">
         <v>1</v>
       </c>
     </row>
@@ -9909,14 +9959,14 @@
       <c r="F14" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="G14" s="20" t="inlineStr">
+      <c r="G14" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" s="20" t="inlineStr">
         <is>
           <t xml:space="preserve"> partie 12 : Faux</t>
         </is>
       </c>
-      <c r="H14" s="20" t="n">
-        <v>0</v>
-      </c>
       <c r="I14" s="20" t="n">
         <v>0</v>
       </c>
@@ -9924,9 +9974,12 @@
         <v>0</v>
       </c>
       <c r="K14" s="20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L14" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="M14" s="20" t="n">
         <v>1</v>
       </c>
     </row>
@@ -9957,7 +10010,7 @@
       <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="12.2109375" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.2109375" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col width="11.08" customWidth="1" style="20" min="6" max="6"/>
     <col width="11.52" customWidth="1" style="20" min="932" max="1009"/>
@@ -10368,7 +10421,7 @@
       <selection pane="topLeft" activeCell="I22" activeCellId="0" sqref="I22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.55078125" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.55078125" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col width="11.54" customWidth="1" style="20" min="1" max="1024"/>
   </cols>
@@ -10770,7 +10823,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.55078125" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.55078125" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col width="11.54" customWidth="1" style="20" min="1" max="1024"/>
   </cols>
@@ -11172,7 +11225,7 @@
       <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.9765625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.9765625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col width="11.53" customWidth="1" style="20" min="16341" max="16384"/>
   </cols>
@@ -11588,7 +11641,7 @@
       <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.9765625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.9765625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col width="11.53" customWidth="1" style="20" min="16383" max="16384"/>
   </cols>
@@ -12143,7 +12196,7 @@
       <selection pane="topLeft" activeCell="H12" activeCellId="0" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.9765625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.9765625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col width="11.97" customWidth="1" style="20" min="1" max="16384"/>
   </cols>
@@ -12260,37 +12313,37 @@
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1" s="23">
-      <c r="A4" s="38" t="inlineStr">
+      <c r="A4" s="42" t="inlineStr">
         <is>
           <t>Abbas</t>
         </is>
       </c>
-      <c r="B4" s="38" t="inlineStr">
+      <c r="B4" s="42" t="inlineStr">
         <is>
           <t>Zina</t>
         </is>
       </c>
-      <c r="C4" s="38" t="inlineStr">
+      <c r="C4" s="42" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="D4" s="38" t="inlineStr">
+      <c r="D4" s="42" t="inlineStr">
         <is>
           <t>Terminé</t>
         </is>
       </c>
-      <c r="E4" s="38" t="inlineStr">
+      <c r="E4" s="42" t="inlineStr">
         <is>
           <t>Zina</t>
         </is>
       </c>
-      <c r="F4" s="38" t="inlineStr">
+      <c r="F4" s="42" t="inlineStr">
         <is>
           <t>7,28</t>
         </is>
       </c>
-      <c r="G4" s="38" t="inlineStr">
+      <c r="G4" s="42" t="inlineStr">
         <is>
           <t>5 min 15 s</t>
         </is>
@@ -12371,37 +12424,37 @@
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1" s="23">
-      <c r="A7" s="38" t="inlineStr">
+      <c r="A7" s="42" t="inlineStr">
         <is>
           <t>Abdelgow</t>
         </is>
       </c>
-      <c r="B7" s="38" t="inlineStr">
+      <c r="B7" s="42" t="inlineStr">
         <is>
           <t>Hassan Mahamat</t>
         </is>
       </c>
-      <c r="C7" s="38" t="inlineStr">
+      <c r="C7" s="42" t="inlineStr">
         <is>
           <t>hassan-mahamat.abdelgow@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D7" s="38" t="inlineStr">
+      <c r="D7" s="42" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="E7" s="38" t="inlineStr">
+      <c r="E7" s="42" t="inlineStr">
         <is>
           <t>Hassan Mahamat</t>
         </is>
       </c>
-      <c r="F7" s="38" t="inlineStr">
+      <c r="F7" s="42" t="inlineStr">
         <is>
           <t>7,52</t>
         </is>
       </c>
-      <c r="G7" s="38" t="inlineStr">
+      <c r="G7" s="42" t="inlineStr">
         <is>
           <t>23 min 37 s</t>
         </is>
@@ -12482,37 +12535,37 @@
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1" s="23">
-      <c r="A10" s="38" t="inlineStr">
+      <c r="A10" s="42" t="inlineStr">
         <is>
           <t>Abi Rizk</t>
         </is>
       </c>
-      <c r="B10" s="38" t="inlineStr">
+      <c r="B10" s="42" t="inlineStr">
         <is>
           <t>Rodolphe</t>
         </is>
       </c>
-      <c r="C10" s="38" t="inlineStr">
+      <c r="C10" s="42" t="inlineStr">
         <is>
           <t>rodolphe.abi-rizk@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D10" s="38" t="inlineStr">
+      <c r="D10" s="42" t="inlineStr">
         <is>
           <t>Terminé</t>
         </is>
       </c>
-      <c r="E10" s="38" t="inlineStr">
+      <c r="E10" s="42" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="F10" s="38" t="inlineStr">
+      <c r="F10" s="42" t="inlineStr">
         <is>
           <t>8,88</t>
         </is>
       </c>
-      <c r="G10" s="38" t="inlineStr">
+      <c r="G10" s="42" t="inlineStr">
         <is>
           <t>15 min 32 s</t>
         </is>
@@ -12556,37 +12609,37 @@
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1" s="23">
-      <c r="A12" s="38" t="inlineStr">
+      <c r="A12" s="42" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="B12" s="38" t="inlineStr">
+      <c r="B12" s="42" t="inlineStr">
         <is>
           <t>Iness</t>
         </is>
       </c>
-      <c r="C12" s="38" t="inlineStr">
+      <c r="C12" s="42" t="inlineStr">
         <is>
           <t>iness.abdenbaoui@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D12" s="38" t="inlineStr">
+      <c r="D12" s="42" t="inlineStr">
         <is>
           <t>Terminé</t>
         </is>
       </c>
-      <c r="E12" s="38" t="inlineStr">
+      <c r="E12" s="42" t="inlineStr">
         <is>
           <t>Iness</t>
         </is>
       </c>
-      <c r="F12" s="38" t="inlineStr">
+      <c r="F12" s="42" t="inlineStr">
         <is>
           <t>6,51</t>
         </is>
       </c>
-      <c r="G12" s="38" t="inlineStr">
+      <c r="G12" s="42" t="inlineStr">
         <is>
           <t>10 min 33 s</t>
         </is>
@@ -12630,37 +12683,37 @@
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1" s="23">
-      <c r="A14" s="38" t="inlineStr">
+      <c r="A14" s="42" t="inlineStr">
         <is>
           <t>Abi Rizk</t>
         </is>
       </c>
-      <c r="B14" s="38" t="inlineStr">
+      <c r="B14" s="42" t="inlineStr">
         <is>
           <t>Christian</t>
         </is>
       </c>
-      <c r="C14" s="38" t="inlineStr">
+      <c r="C14" s="42" t="inlineStr">
         <is>
           <t>christian.abi-rizk@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="D14" s="38" t="inlineStr">
+      <c r="D14" s="42" t="inlineStr">
         <is>
           <t>Terminé</t>
         </is>
       </c>
-      <c r="E14" s="38" t="inlineStr">
+      <c r="E14" s="42" t="inlineStr">
         <is>
           <t>Christian</t>
         </is>
       </c>
-      <c r="F14" s="38" t="inlineStr">
+      <c r="F14" s="42" t="inlineStr">
         <is>
           <t>+</t>
         </is>
       </c>
-      <c r="G14" s="38" t="inlineStr">
+      <c r="G14" s="42" t="inlineStr">
         <is>
           <t>21 min 49 s</t>
         </is>
@@ -12688,13 +12741,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.9140625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.9140625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col width="11.31" customWidth="1" style="20" min="1" max="2"/>
     <col width="11.52" customWidth="1" style="20" min="948" max="974"/>
@@ -12712,7 +12765,7 @@
           <t>Réponse 2</t>
         </is>
       </c>
-      <c r="C1" s="24" t="inlineStr">
+      <c r="F1" s="24" t="inlineStr">
         <is>
           <t>Les chromosomes du père déterminent si le bébé est un garçon ou une fille</t>
         </is>
@@ -12734,6 +12787,21 @@
           <t>partie 1 : Vrai</t>
         </is>
       </c>
+      <c r="D2" s="20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> partie 2 : Faux</t>
+        </is>
+      </c>
+      <c r="E2" s="20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> partie 3 : Vrai </t>
+        </is>
+      </c>
+      <c r="F2" s="20" t="inlineStr">
+        <is>
+          <t>partie 1 : Vrai</t>
+        </is>
+      </c>
     </row>
     <row r="3" ht="12.75" customHeight="1" s="23">
       <c r="A3" s="20" t="inlineStr">
@@ -12751,6 +12819,21 @@
           <t>partie 1 : Vrai</t>
         </is>
       </c>
+      <c r="D3" s="20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> partie 2 : Vrai</t>
+        </is>
+      </c>
+      <c r="E3" s="20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> partie 3 : Vrai </t>
+        </is>
+      </c>
+      <c r="F3" s="20" t="inlineStr">
+        <is>
+          <t>partie 1 : Vrai</t>
+        </is>
+      </c>
     </row>
     <row r="4" ht="12.75" customHeight="1" s="23">
       <c r="A4" s="20" t="inlineStr">
@@ -12768,6 +12851,21 @@
           <t>partie 1 : Vrai</t>
         </is>
       </c>
+      <c r="D4" s="20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> partie 2 : Faux</t>
+        </is>
+      </c>
+      <c r="E4" s="20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> partie 3 : Vrai </t>
+        </is>
+      </c>
+      <c r="F4" s="20" t="inlineStr">
+        <is>
+          <t>partie 1 : Vrai</t>
+        </is>
+      </c>
     </row>
     <row r="5" ht="12.75" customHeight="1" s="23">
       <c r="A5" s="20" t="inlineStr">
@@ -12781,6 +12879,21 @@
         </is>
       </c>
       <c r="C5" s="20" t="inlineStr">
+        <is>
+          <t>partie 1 : Vrai</t>
+        </is>
+      </c>
+      <c r="D5" s="20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> partie 2 : Faux</t>
+        </is>
+      </c>
+      <c r="E5" s="20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> partie 3 : Vrai </t>
+        </is>
+      </c>
+      <c r="F5" s="20" t="inlineStr">
         <is>
           <t>partie 1 : Faux</t>
         </is>

</xml_diff>

<commit_message>
feat(utils): add class StringExtractor() and associated test
</commit_message>
<xml_diff>
--- a/fichiers_xls/test.xlsx
+++ b/fichiers_xls/test.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="12" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -412,8 +412,8 @@
           <yMode val="edge"/>
           <wMode val="factor"/>
           <hMode val="factor"/>
-          <x val="0.306378986866792"/>
-          <y val="0.036522633744856"/>
+          <x val="0.30639814872725"/>
+          <y val="0.0366559485530547"/>
         </manualLayout>
       </layout>
       <overlay val="0"/>
@@ -432,10 +432,10 @@
           <yMode val="edge"/>
           <wMode val="factor"/>
           <hMode val="factor"/>
-          <x val="0.0127579737335835"/>
-          <y val="0.126414609053498"/>
-          <w val="0.960225140712946"/>
-          <h val="0.84863683127572"/>
+          <x val="0.0127587716555132"/>
+          <y val="0.126430868167203"/>
+          <w val="0.960160110075677"/>
+          <h val="0.848488745980707"/>
         </manualLayout>
       </layout>
       <barChart>
@@ -608,11 +608,11 @@
         </ser>
         <gapWidth val="219"/>
         <overlap val="-27"/>
-        <axId val="27030680"/>
-        <axId val="52412455"/>
+        <axId val="93924197"/>
+        <axId val="19988085"/>
       </barChart>
       <catAx>
-        <axId val="27030680"/>
+        <axId val="93924197"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
@@ -647,7 +647,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="52412455"/>
+        <crossAx val="19988085"/>
         <crossesAt val="0"/>
         <auto val="1"/>
         <lblAlgn val="ctr"/>
@@ -655,7 +655,7 @@
         <noMultiLvlLbl val="0"/>
       </catAx>
       <valAx>
-        <axId val="52412455"/>
+        <axId val="19988085"/>
         <scaling>
           <orientation val="minMax"/>
           <max val="100"/>
@@ -699,7 +699,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="27030680"/>
+        <crossAx val="93924197"/>
         <crossesAt val="1"/>
         <crossBetween val="midCat"/>
       </valAx>
@@ -756,8 +756,8 @@
           <yMode val="edge"/>
           <wMode val="factor"/>
           <hMode val="factor"/>
-          <x val="0.306243306243306"/>
-          <y val="0.036522633744856"/>
+          <x val="0.306262600806452"/>
+          <y val="0.0366559485530547"/>
         </manualLayout>
       </layout>
       <overlay val="0"/>
@@ -776,10 +776,10 @@
           <yMode val="edge"/>
           <wMode val="factor"/>
           <hMode val="factor"/>
-          <x val="0.0127890127890128"/>
-          <y val="0.126414609053498"/>
-          <w val="0.95980595980596"/>
-          <h val="0.84863683127572"/>
+          <x val="0.0127898185483871"/>
+          <y val="0.126430868167203"/>
+          <w val="0.959740423387097"/>
+          <h val="0.848488745980707"/>
         </manualLayout>
       </layout>
       <barChart>
@@ -952,11 +952,11 @@
         </ser>
         <gapWidth val="219"/>
         <overlap val="-27"/>
-        <axId val="21155409"/>
-        <axId val="40050850"/>
+        <axId val="79837500"/>
+        <axId val="28518525"/>
       </barChart>
       <catAx>
-        <axId val="21155409"/>
+        <axId val="79837500"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
@@ -991,7 +991,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="40050850"/>
+        <crossAx val="28518525"/>
         <crossesAt val="0"/>
         <auto val="1"/>
         <lblAlgn val="ctr"/>
@@ -999,7 +999,7 @@
         <noMultiLvlLbl val="0"/>
       </catAx>
       <valAx>
-        <axId val="40050850"/>
+        <axId val="28518525"/>
         <scaling>
           <orientation val="minMax"/>
           <max val="100"/>
@@ -1043,7 +1043,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="21155409"/>
+        <crossAx val="79837500"/>
         <crossesAt val="1"/>
         <crossBetween val="midCat"/>
       </valAx>
@@ -1100,8 +1100,8 @@
           <yMode val="edge"/>
           <wMode val="factor"/>
           <hMode val="factor"/>
-          <x val="0.306413002393852"/>
-          <y val="0.0367798353909465"/>
+          <x val="0.306432306432306"/>
+          <y val="0.0369131832797428"/>
         </manualLayout>
       </layout>
       <overlay val="0"/>
@@ -1121,10 +1121,10 @@
           <yMode val="edge"/>
           <wMode val="factor"/>
           <hMode val="factor"/>
-          <x val="0.0525387425979589"/>
-          <y val="0.146862139917695"/>
-          <w val="0.921191886103062"/>
-          <h val="0.807741769547325"/>
+          <x val="0.0525420525420525"/>
+          <y val="0.146881028938907"/>
+          <w val="0.9211239211239211"/>
+          <h val="0.8075884244372989"/>
         </manualLayout>
       </layout>
       <barChart>
@@ -1297,11 +1297,11 @@
         </ser>
         <gapWidth val="219"/>
         <overlap val="-27"/>
-        <axId val="22178728"/>
-        <axId val="46711584"/>
+        <axId val="79897923"/>
+        <axId val="58552170"/>
       </barChart>
       <catAx>
-        <axId val="22178728"/>
+        <axId val="79897923"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
@@ -1336,7 +1336,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="46711584"/>
+        <crossAx val="58552170"/>
         <crosses val="autoZero"/>
         <auto val="1"/>
         <lblAlgn val="ctr"/>
@@ -1344,7 +1344,7 @@
         <noMultiLvlLbl val="0"/>
       </catAx>
       <valAx>
-        <axId val="46711584"/>
+        <axId val="58552170"/>
         <scaling>
           <orientation val="minMax"/>
           <max val="100"/>
@@ -1388,7 +1388,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="22178728"/>
+        <crossAx val="79897923"/>
         <crossesAt val="1"/>
         <crossBetween val="midCat"/>
       </valAx>
@@ -1445,8 +1445,8 @@
           <yMode val="edge"/>
           <wMode val="factor"/>
           <hMode val="factor"/>
-          <x val="0.306475998488094"/>
-          <y val="0.0367798353909465"/>
+          <x val="0.306495306495307"/>
+          <y val="0.0369131832797428"/>
         </manualLayout>
       </layout>
       <overlay val="0"/>
@@ -1466,10 +1466,10 @@
           <yMode val="edge"/>
           <wMode val="factor"/>
           <hMode val="factor"/>
-          <x val="0.0525387425979589"/>
-          <y val="0.146862139917695"/>
-          <w val="0.921191886103062"/>
-          <h val="0.807741769547325"/>
+          <x val="0.0525420525420525"/>
+          <y val="0.146881028938907"/>
+          <w val="0.9211239211239211"/>
+          <h val="0.8075884244372989"/>
         </manualLayout>
       </layout>
       <barChart>
@@ -1642,11 +1642,11 @@
         </ser>
         <gapWidth val="219"/>
         <overlap val="-27"/>
-        <axId val="39042115"/>
-        <axId val="99836153"/>
+        <axId val="20140759"/>
+        <axId val="81865055"/>
       </barChart>
       <catAx>
-        <axId val="39042115"/>
+        <axId val="20140759"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
@@ -1681,7 +1681,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="99836153"/>
+        <crossAx val="81865055"/>
         <crosses val="autoZero"/>
         <auto val="1"/>
         <lblAlgn val="ctr"/>
@@ -1689,7 +1689,7 @@
         <noMultiLvlLbl val="0"/>
       </catAx>
       <valAx>
-        <axId val="99836153"/>
+        <axId val="81865055"/>
         <scaling>
           <orientation val="minMax"/>
           <max val="100"/>
@@ -1733,7 +1733,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="39042115"/>
+        <crossAx val="20140759"/>
         <crossesAt val="1"/>
         <crossBetween val="midCat"/>
       </valAx>
@@ -1790,8 +1790,8 @@
           <yMode val="edge"/>
           <wMode val="factor"/>
           <hMode val="factor"/>
-          <x val="0.306369306369306"/>
-          <y val="0.0367798353909465"/>
+          <x val="0.306388608870968"/>
+          <y val="0.0369131832797428"/>
         </manualLayout>
       </layout>
       <overlay val="0"/>
@@ -1811,10 +1811,10 @@
           <yMode val="edge"/>
           <wMode val="factor"/>
           <hMode val="factor"/>
-          <x val="0.0485100485100485"/>
-          <y val="0.146862139917695"/>
-          <w val="0.924084924084924"/>
-          <h val="0.80761316872428"/>
+          <x val="0.0485131048387097"/>
+          <y val="0.146881028938907"/>
+          <w val="0.924017137096774"/>
+          <h val="0.807459807073955"/>
         </manualLayout>
       </layout>
       <barChart>
@@ -1826,7 +1826,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>time_min!$AG$13:$AG$13</f>
+              <f>time_min!$AF$13:$AF$13</f>
               <strCache>
                 <ptCount val="1"/>
                 <pt idx="0">
@@ -1873,7 +1873,7 @@
           </dLbls>
           <cat>
             <strRef>
-              <f>time_min!$AH$12:$BM$12</f>
+              <f>time_min!$AG$12:$BL$12</f>
               <strCache>
                 <ptCount val="32"/>
                 <pt idx="0">
@@ -1977,7 +1977,7 @@
           </cat>
           <val>
             <numRef>
-              <f>time_min!$AH$13:$BM$13</f>
+              <f>time_min!$AG$13:$BL$13</f>
               <numCache>
                 <formatCode>General</formatCode>
                 <ptCount val="32"/>
@@ -1987,11 +1987,11 @@
         </ser>
         <gapWidth val="219"/>
         <overlap val="-27"/>
-        <axId val="68121222"/>
-        <axId val="86841765"/>
+        <axId val="92727579"/>
+        <axId val="88261216"/>
       </barChart>
       <catAx>
-        <axId val="68121222"/>
+        <axId val="92727579"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
@@ -2026,7 +2026,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="86841765"/>
+        <crossAx val="88261216"/>
         <crosses val="autoZero"/>
         <auto val="1"/>
         <lblAlgn val="ctr"/>
@@ -2034,7 +2034,7 @@
         <noMultiLvlLbl val="0"/>
       </catAx>
       <valAx>
-        <axId val="86841765"/>
+        <axId val="88261216"/>
         <scaling>
           <orientation val="minMax"/>
           <max val="100"/>
@@ -2078,7 +2078,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="68121222"/>
+        <crossAx val="92727579"/>
         <crossesAt val="1"/>
         <crossBetween val="midCat"/>
       </valAx>
@@ -2135,8 +2135,8 @@
           <yMode val="edge"/>
           <wMode val="factor"/>
           <hMode val="factor"/>
-          <x val="0.306369306369306"/>
-          <y val="0.0364011875564735"/>
+          <x val="0.306388608870968"/>
+          <y val="0.0365349857991221"/>
         </manualLayout>
       </layout>
       <overlay val="0"/>
@@ -2156,10 +2156,10 @@
           <yMode val="edge"/>
           <wMode val="factor"/>
           <hMode val="factor"/>
-          <x val="0.0485100485100485"/>
-          <y val="0.146766490254292"/>
-          <w val="0.924084924084924"/>
-          <h val="0.807667484187427"/>
+          <x val="0.0485131048387097"/>
+          <y val="0.146785437645236"/>
+          <w val="0.924017137096774"/>
+          <h val="0.807513555383424"/>
         </manualLayout>
       </layout>
       <barChart>
@@ -2332,11 +2332,11 @@
         </ser>
         <gapWidth val="219"/>
         <overlap val="-27"/>
-        <axId val="47435458"/>
-        <axId val="89917584"/>
+        <axId val="67782603"/>
+        <axId val="47198003"/>
       </barChart>
       <catAx>
-        <axId val="47435458"/>
+        <axId val="67782603"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
@@ -2371,7 +2371,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="89917584"/>
+        <crossAx val="47198003"/>
         <crosses val="autoZero"/>
         <auto val="1"/>
         <lblAlgn val="ctr"/>
@@ -2379,7 +2379,7 @@
         <noMultiLvlLbl val="0"/>
       </catAx>
       <valAx>
-        <axId val="89917584"/>
+        <axId val="47198003"/>
         <scaling>
           <orientation val="minMax"/>
           <max val="100"/>
@@ -2423,7 +2423,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="47435458"/>
+        <crossAx val="67782603"/>
         <crossesAt val="1"/>
         <crossBetween val="midCat"/>
       </valAx>
@@ -2480,8 +2480,8 @@
           <yMode val="edge"/>
           <wMode val="factor"/>
           <hMode val="factor"/>
-          <x val="0.306495306495307"/>
-          <y val="0.0371756809087389"/>
+          <x val="0.306514616935484"/>
+          <y val="0.0373095791376194"/>
         </manualLayout>
       </layout>
       <overlay val="0"/>
@@ -2501,10 +2501,10 @@
           <yMode val="edge"/>
           <wMode val="factor"/>
           <hMode val="factor"/>
-          <x val="0.0485100485100485"/>
-          <y val="0.146766490254292"/>
-          <w val="0.924084924084924"/>
-          <h val="0.807667484187427"/>
+          <x val="0.0485131048387097"/>
+          <y val="0.146785437645236"/>
+          <w val="0.924017137096774"/>
+          <h val="0.807513555383424"/>
         </manualLayout>
       </layout>
       <barChart>
@@ -2677,11 +2677,11 @@
         </ser>
         <gapWidth val="219"/>
         <overlap val="-27"/>
-        <axId val="79012813"/>
-        <axId val="96399382"/>
+        <axId val="65227680"/>
+        <axId val="97130071"/>
       </barChart>
       <catAx>
-        <axId val="79012813"/>
+        <axId val="65227680"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
@@ -2716,7 +2716,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="96399382"/>
+        <crossAx val="97130071"/>
         <crosses val="autoZero"/>
         <auto val="1"/>
         <lblAlgn val="ctr"/>
@@ -2724,7 +2724,7 @@
         <noMultiLvlLbl val="0"/>
       </catAx>
       <valAx>
-        <axId val="96399382"/>
+        <axId val="97130071"/>
         <scaling>
           <orientation val="minMax"/>
           <max val="100"/>
@@ -2768,7 +2768,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="79012813"/>
+        <crossAx val="65227680"/>
         <crossesAt val="1"/>
         <crossBetween val="midCat"/>
       </valAx>
@@ -2801,9 +2801,9 @@
     </from>
     <to>
       <col>99</col>
-      <colOff>188640</colOff>
+      <colOff>188280</colOff>
       <row>30</row>
-      <rowOff>102240</rowOff>
+      <rowOff>101880</rowOff>
     </to>
     <graphicFrame>
       <nvGraphicFramePr>
@@ -2833,9 +2833,9 @@
     </from>
     <to>
       <col>56</col>
-      <colOff>659880</colOff>
+      <colOff>659520</colOff>
       <row>30</row>
-      <rowOff>101880</rowOff>
+      <rowOff>101520</rowOff>
     </to>
     <graphicFrame>
       <nvGraphicFramePr>
@@ -2865,9 +2865,9 @@
     </from>
     <to>
       <col>107</col>
-      <colOff>660240</colOff>
+      <colOff>659880</colOff>
       <row>30</row>
-      <rowOff>101160</rowOff>
+      <rowOff>100800</rowOff>
     </to>
     <graphicFrame>
       <nvGraphicFramePr>
@@ -2897,9 +2897,9 @@
     </from>
     <to>
       <col>107</col>
-      <colOff>660240</colOff>
+      <colOff>659880</colOff>
       <row>30</row>
-      <rowOff>101160</rowOff>
+      <rowOff>100800</rowOff>
     </to>
     <graphicFrame>
       <nvGraphicFramePr>
@@ -2922,16 +2922,16 @@
 <wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <twoCellAnchor editAs="oneCell">
     <from>
-      <col>54</col>
+      <col>53</col>
       <colOff>9720</colOff>
       <row>13</row>
       <rowOff>93600</rowOff>
     </from>
     <to>
-      <col>60</col>
+      <col>59</col>
       <colOff>659880</colOff>
       <row>30</row>
-      <rowOff>139680</rowOff>
+      <rowOff>139320</rowOff>
     </to>
     <graphicFrame>
       <nvGraphicFramePr>
@@ -2961,9 +2961,9 @@
     </from>
     <to>
       <col>76</col>
-      <colOff>660240</colOff>
+      <colOff>659880</colOff>
       <row>30</row>
-      <rowOff>129240</rowOff>
+      <rowOff>128880</rowOff>
     </to>
     <graphicFrame>
       <nvGraphicFramePr>
@@ -2988,9 +2988,9 @@
     </from>
     <to>
       <col>76</col>
-      <colOff>660240</colOff>
+      <colOff>659880</colOff>
       <row>30</row>
-      <rowOff>129240</rowOff>
+      <rowOff>128880</rowOff>
     </to>
     <graphicFrame>
       <nvGraphicFramePr>
@@ -9179,13 +9179,13 @@
   </sheetPr>
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="11.9765625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col width="11.53" customWidth="1" style="19" min="16345" max="16384"/>
+    <col width="11.53" customWidth="1" style="19" min="16344" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1" s="22">
@@ -12726,7 +12726,7 @@
   </sheetPr>
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>

</xml_diff>